<commit_message>
Updated to reflect latest mindmap and small bug fix
</commit_message>
<xml_diff>
--- a/mind_maps/malware_capabilities_descriptions.xlsx
+++ b/mind_maps/malware_capabilities_descriptions.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="84" windowWidth="11460" windowHeight="4452"/>
+    <workbookView xWindow="0" yWindow="192" windowWidth="20100" windowHeight="8412"/>
   </bookViews>
   <sheets>
-    <sheet name="malware_capabilities_01092014" sheetId="1" r:id="rId1"/>
+    <sheet name="malware_capabilities" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="206">
   <si>
     <t>Capability</t>
   </si>
@@ -34,19 +34,16 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve"> Gain Access</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Exploit Application Vulnerability</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Exploit Configuration Vulnerabiity</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Infect Machine</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Exploit Application/OS to Bypass Security Features</t>
+    <t xml:space="preserve"> Infect Remote Machine</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Identify Target Machine(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Perform User-Involved Remote Infection</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Perform Autonomous Remote Infection</t>
   </si>
   <si>
     <t xml:space="preserve"> Infect File</t>
@@ -55,16 +52,7 @@
     <t xml:space="preserve"> Identify File</t>
   </si>
   <si>
-    <t xml:space="preserve"> Inject Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bypass Security Filter</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Use Alternate Encoding</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Use Bridge Building</t>
+    <t xml:space="preserve"> Write Code Into File</t>
   </si>
   <si>
     <t>Anti-Behavioral Analysis</t>
@@ -172,7 +160,7 @@
     <t xml:space="preserve"> Hide Open Network Ports</t>
   </si>
   <si>
-    <t xml:space="preserve"> Hide Network Traffic (from host-based firewalls/sniffers)</t>
+    <t xml:space="preserve"> Hide Network Traffic</t>
   </si>
   <si>
     <t xml:space="preserve"> Obfuscate Artifact Properties</t>
@@ -217,12 +205,6 @@
     <t xml:space="preserve"> Hide Arbitrary Virtual Memory</t>
   </si>
   <si>
-    <t xml:space="preserve"> Exploit Tool Weaknesses</t>
-  </si>
-  <si>
-    <t>to Hide Information</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Security Software Evasion</t>
   </si>
   <si>
@@ -352,6 +334,102 @@
     <t xml:space="preserve"> Communicate with C2 Servers</t>
   </si>
   <si>
+    <t xml:space="preserve"> Determine C2 Server</t>
+  </si>
+  <si>
+    <t>Remote Machine Manipulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Search For Remote Machines</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Access Remote Machine</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Compromise Remote Machine</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Control Remote Machine</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Execute Remote Command</t>
+  </si>
+  <si>
+    <t>Privilege Escalation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Escalate User Privilege</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Elevate CPU Mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Impersonate User</t>
+  </si>
+  <si>
+    <t>Data Exfiltration</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Stage Data for Exfiltration</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Move Data to Staging Server</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Package Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Obfuscate Data for Exfiltration</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Encrypt Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hide Data in Other Formats (steganography)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Exfiltrate Stolen Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Exfiltrate via Network</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Exfiltrate via Physical Media</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Exfiltrate via Covert Channel</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Exfiltrate via Dumpster Dive</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Exfiltrate via VoIP/Phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Exfiltrate via Fax</t>
+  </si>
+  <si>
+    <t>Post-Operation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Install Other Components</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Install Secondary Module</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Install Secondary Malware</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Remove Traces of Infection</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Remove Self</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Remove System Artifacts</t>
+  </si>
+  <si>
     <t>Data Theft</t>
   </si>
   <si>
@@ -421,24 +499,6 @@
     <t xml:space="preserve"> Steal Make/Model</t>
   </si>
   <si>
-    <t>Remote Machine Manipulation</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Search For Remote Machines</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Access Remote Machine</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Compromise Remote Machine</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Control Remote Machine</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Execute Remote Command</t>
-  </si>
-  <si>
     <t>Spying</t>
   </si>
   <si>
@@ -481,15 +541,6 @@
     <t xml:space="preserve"> Capture File System Dump</t>
   </si>
   <si>
-    <t>Privilege Escalation</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Escalate User Privilege</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Elevate CPU Mode</t>
-  </si>
-  <si>
     <t>Destruction</t>
   </si>
   <si>
@@ -508,39 +559,6 @@
     <t xml:space="preserve"> Erase Data</t>
   </si>
   <si>
-    <t>Data Exfiltration</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Exfiltrate Stolen Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Exfiltrate via Network</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Exfiltrate via Physical Media</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Exfiltrate via Covert Channel</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Exfiltrate via Dumpster Dive</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Exfiltrate via VoIP/Phone</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Exfiltrate via Fax</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Prepare Data for Exfiltration</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Encrypt Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hide Data in Other Formats (steganography)</t>
-  </si>
-  <si>
     <t>Integrity Violation</t>
   </si>
   <si>
@@ -577,7 +595,7 @@
     <t xml:space="preserve"> Consume System Resources</t>
   </si>
   <si>
-    <t xml:space="preserve"> Mine for Bitcoins</t>
+    <t xml:space="preserve"> Mine for CryptoCurrency</t>
   </si>
   <si>
     <t xml:space="preserve"> Crack Passwords</t>
@@ -611,6 +629,9 @@
   </si>
   <si>
     <t>Reference(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Exploit Tool Weaknesses to Hide Information</t>
   </si>
 </sst>
 </file>
@@ -1448,19 +1469,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E194"/>
+  <dimension ref="A1:E201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" customWidth="1"/>
-    <col min="3" max="3" width="50.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" customWidth="1"/>
-    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="1" max="1" width="26.77734375" customWidth="1"/>
+    <col min="2" max="2" width="38.77734375" customWidth="1"/>
+    <col min="3" max="3" width="52.6640625" customWidth="1"/>
+    <col min="4" max="4" width="35.88671875" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -1477,7 +1498,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1520,6 +1541,9 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1528,9 +1552,6 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1539,6 +1560,9 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1555,12 +1579,6 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1596,6 +1614,9 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1604,6 +1625,9 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1620,12 +1644,6 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1661,6 +1679,9 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1669,6 +1690,9 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1699,6 +1723,9 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1718,9 +1745,6 @@
         <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1759,9 +1783,6 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1770,9 +1791,6 @@
         <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1781,9 +1799,6 @@
         <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1800,6 +1815,12 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1808,6 +1829,9 @@
         <v>5</v>
       </c>
       <c r="B36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1843,12 +1867,6 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>5</v>
-      </c>
-      <c r="B40" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1884,6 +1902,12 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1892,6 +1916,9 @@
         <v>5</v>
       </c>
       <c r="B45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1911,9 +1938,6 @@
         <v>5</v>
       </c>
       <c r="B47" t="s">
-        <v>5</v>
-      </c>
-      <c r="C47" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1955,6 +1979,9 @@
         <v>5</v>
       </c>
       <c r="B51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2007,9 +2034,6 @@
         <v>5</v>
       </c>
       <c r="B56" t="s">
-        <v>5</v>
-      </c>
-      <c r="C56" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2051,7 +2075,10 @@
         <v>5</v>
       </c>
       <c r="B60" t="s">
-        <v>63</v>
+        <v>5</v>
+      </c>
+      <c r="C60" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
@@ -2059,10 +2086,7 @@
         <v>5</v>
       </c>
       <c r="B61" t="s">
-        <v>5</v>
-      </c>
-      <c r="C61" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
@@ -2073,7 +2097,7 @@
         <v>5</v>
       </c>
       <c r="C62" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
@@ -2081,10 +2105,7 @@
         <v>5</v>
       </c>
       <c r="B63" t="s">
-        <v>5</v>
-      </c>
-      <c r="C63" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
@@ -2095,12 +2116,18 @@
         <v>5</v>
       </c>
       <c r="C64" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>68</v>
+        <v>5</v>
+      </c>
+      <c r="B65" t="s">
+        <v>5</v>
+      </c>
+      <c r="C65" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
@@ -2108,7 +2135,10 @@
         <v>5</v>
       </c>
       <c r="B66" t="s">
-        <v>69</v>
+        <v>5</v>
+      </c>
+      <c r="C66" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
@@ -2116,10 +2146,7 @@
         <v>5</v>
       </c>
       <c r="B67" t="s">
-        <v>5</v>
-      </c>
-      <c r="C67" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
@@ -2127,18 +2154,15 @@
         <v>5</v>
       </c>
       <c r="B68" t="s">
-        <v>71</v>
+        <v>5</v>
+      </c>
+      <c r="C68" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>5</v>
-      </c>
-      <c r="B69" t="s">
-        <v>5</v>
-      </c>
-      <c r="C69" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
@@ -2146,10 +2170,7 @@
         <v>5</v>
       </c>
       <c r="B70" t="s">
-        <v>5</v>
-      </c>
-      <c r="C70" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
@@ -2160,7 +2181,7 @@
         <v>5</v>
       </c>
       <c r="C71" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
@@ -2168,7 +2189,10 @@
         <v>5</v>
       </c>
       <c r="B72" t="s">
-        <v>75</v>
+        <v>5</v>
+      </c>
+      <c r="C72" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
@@ -2179,12 +2203,15 @@
         <v>5</v>
       </c>
       <c r="C73" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>77</v>
+        <v>5</v>
+      </c>
+      <c r="B74" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
@@ -2192,7 +2219,10 @@
         <v>5</v>
       </c>
       <c r="B75" t="s">
-        <v>78</v>
+        <v>5</v>
+      </c>
+      <c r="C75" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
@@ -2200,10 +2230,7 @@
         <v>5</v>
       </c>
       <c r="B76" t="s">
-        <v>5</v>
-      </c>
-      <c r="C76" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
@@ -2214,18 +2241,12 @@
         <v>5</v>
       </c>
       <c r="C77" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>5</v>
-      </c>
-      <c r="B78" t="s">
-        <v>5</v>
-      </c>
-      <c r="C78" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
@@ -2233,7 +2254,7 @@
         <v>5</v>
       </c>
       <c r="B79" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
@@ -2244,7 +2265,7 @@
         <v>5</v>
       </c>
       <c r="C80" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
@@ -2252,7 +2273,7 @@
         <v>5</v>
       </c>
       <c r="B81" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
@@ -2263,12 +2284,18 @@
         <v>5</v>
       </c>
       <c r="C82" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>86</v>
+        <v>5</v>
+      </c>
+      <c r="B83" t="s">
+        <v>5</v>
+      </c>
+      <c r="C83" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
@@ -2276,7 +2303,10 @@
         <v>5</v>
       </c>
       <c r="B84" t="s">
-        <v>87</v>
+        <v>5</v>
+      </c>
+      <c r="C84" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
@@ -2287,7 +2317,7 @@
         <v>5</v>
       </c>
       <c r="C85" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
@@ -2295,7 +2325,7 @@
         <v>5</v>
       </c>
       <c r="B86" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
@@ -2306,7 +2336,7 @@
         <v>5</v>
       </c>
       <c r="C87" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
@@ -2317,7 +2347,7 @@
         <v>5</v>
       </c>
       <c r="C88" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
@@ -2328,7 +2358,7 @@
         <v>5</v>
       </c>
       <c r="C89" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
@@ -2336,10 +2366,7 @@
         <v>5</v>
       </c>
       <c r="B90" t="s">
-        <v>5</v>
-      </c>
-      <c r="C90" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
@@ -2347,7 +2374,10 @@
         <v>5</v>
       </c>
       <c r="B91" t="s">
-        <v>94</v>
+        <v>5</v>
+      </c>
+      <c r="C91" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
@@ -2358,7 +2388,7 @@
         <v>5</v>
       </c>
       <c r="C92" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
@@ -2366,10 +2396,7 @@
         <v>5</v>
       </c>
       <c r="B93" t="s">
-        <v>5</v>
-      </c>
-      <c r="C93" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
@@ -2380,7 +2407,7 @@
         <v>5</v>
       </c>
       <c r="C94" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
@@ -2388,7 +2415,10 @@
         <v>5</v>
       </c>
       <c r="B95" t="s">
-        <v>98</v>
+        <v>5</v>
+      </c>
+      <c r="C95" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
@@ -2399,7 +2429,7 @@
         <v>5</v>
       </c>
       <c r="C96" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
@@ -2410,7 +2440,7 @@
         <v>5</v>
       </c>
       <c r="C97" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
@@ -2418,18 +2448,15 @@
         <v>5</v>
       </c>
       <c r="B98" t="s">
-        <v>101</v>
+        <v>5</v>
+      </c>
+      <c r="C98" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>5</v>
-      </c>
-      <c r="B99" t="s">
-        <v>5</v>
-      </c>
-      <c r="C99" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
@@ -2437,10 +2464,7 @@
         <v>5</v>
       </c>
       <c r="B100" t="s">
-        <v>5</v>
-      </c>
-      <c r="C100" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
@@ -2451,7 +2475,7 @@
         <v>5</v>
       </c>
       <c r="C101" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
@@ -2462,7 +2486,7 @@
         <v>5</v>
       </c>
       <c r="C102" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
@@ -2470,23 +2494,23 @@
         <v>5</v>
       </c>
       <c r="B103" t="s">
-        <v>5</v>
-      </c>
-      <c r="C103" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>107</v>
+        <v>5</v>
+      </c>
+      <c r="B104" t="s">
+        <v>5</v>
+      </c>
+      <c r="C104" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>5</v>
-      </c>
-      <c r="B105" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
@@ -2494,10 +2518,7 @@
         <v>5</v>
       </c>
       <c r="B106" t="s">
-        <v>5</v>
-      </c>
-      <c r="C106" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
@@ -2505,10 +2526,7 @@
         <v>5</v>
       </c>
       <c r="B107" t="s">
-        <v>5</v>
-      </c>
-      <c r="C107" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
@@ -2516,12 +2534,18 @@
         <v>5</v>
       </c>
       <c r="B108" t="s">
-        <v>111</v>
+        <v>5</v>
+      </c>
+      <c r="C108" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>112</v>
+        <v>5</v>
+      </c>
+      <c r="B109" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
@@ -2529,18 +2553,15 @@
         <v>5</v>
       </c>
       <c r="B110" t="s">
-        <v>113</v>
+        <v>5</v>
+      </c>
+      <c r="C110" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>5</v>
-      </c>
-      <c r="B111" t="s">
-        <v>5</v>
-      </c>
-      <c r="C111" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
@@ -2548,10 +2569,7 @@
         <v>5</v>
       </c>
       <c r="B112" t="s">
-        <v>5</v>
-      </c>
-      <c r="C112" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
@@ -2562,7 +2580,7 @@
         <v>5</v>
       </c>
       <c r="C113" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
@@ -2570,18 +2588,12 @@
         <v>5</v>
       </c>
       <c r="B114" t="s">
-        <v>5</v>
-      </c>
-      <c r="C114" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>5</v>
-      </c>
-      <c r="B115" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
@@ -2589,10 +2601,7 @@
         <v>5</v>
       </c>
       <c r="B116" t="s">
-        <v>5</v>
-      </c>
-      <c r="C116" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
@@ -2603,7 +2612,7 @@
         <v>5</v>
       </c>
       <c r="C117" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
@@ -2614,7 +2623,7 @@
         <v>5</v>
       </c>
       <c r="C118" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
@@ -2622,10 +2631,7 @@
         <v>5</v>
       </c>
       <c r="B119" t="s">
-        <v>5</v>
-      </c>
-      <c r="C119" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
@@ -2636,7 +2642,7 @@
         <v>5</v>
       </c>
       <c r="C120" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
@@ -2644,7 +2650,10 @@
         <v>5</v>
       </c>
       <c r="B121" t="s">
-        <v>124</v>
+        <v>5</v>
+      </c>
+      <c r="C121" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
@@ -2652,10 +2661,7 @@
         <v>5</v>
       </c>
       <c r="B122" t="s">
-        <v>5</v>
-      </c>
-      <c r="C122" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
@@ -2666,7 +2672,7 @@
         <v>5</v>
       </c>
       <c r="C123" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
@@ -2677,7 +2683,7 @@
         <v>5</v>
       </c>
       <c r="C124" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
@@ -2688,7 +2694,7 @@
         <v>5</v>
       </c>
       <c r="C125" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
@@ -2699,7 +2705,7 @@
         <v>5</v>
       </c>
       <c r="C126" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
@@ -2710,7 +2716,7 @@
         <v>5</v>
       </c>
       <c r="C127" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
@@ -2718,18 +2724,15 @@
         <v>5</v>
       </c>
       <c r="B128" t="s">
-        <v>131</v>
+        <v>5</v>
+      </c>
+      <c r="C128" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>5</v>
-      </c>
-      <c r="B129" t="s">
-        <v>5</v>
-      </c>
-      <c r="C129" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
@@ -2737,10 +2740,7 @@
         <v>5</v>
       </c>
       <c r="B130" t="s">
-        <v>5</v>
-      </c>
-      <c r="C130" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
@@ -2751,12 +2751,18 @@
         <v>5</v>
       </c>
       <c r="C131" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>135</v>
+        <v>5</v>
+      </c>
+      <c r="B132" t="s">
+        <v>5</v>
+      </c>
+      <c r="C132" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
@@ -2764,7 +2770,7 @@
         <v>5</v>
       </c>
       <c r="B133" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
@@ -2772,7 +2778,10 @@
         <v>5</v>
       </c>
       <c r="B134" t="s">
-        <v>137</v>
+        <v>5</v>
+      </c>
+      <c r="C134" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
@@ -2783,15 +2792,12 @@
         <v>5</v>
       </c>
       <c r="C135" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>5</v>
-      </c>
-      <c r="B136" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
@@ -2799,15 +2805,18 @@
         <v>5</v>
       </c>
       <c r="B137" t="s">
-        <v>5</v>
-      </c>
-      <c r="C137" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>141</v>
+        <v>5</v>
+      </c>
+      <c r="B138" t="s">
+        <v>5</v>
+      </c>
+      <c r="C138" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
@@ -2815,7 +2824,10 @@
         <v>5</v>
       </c>
       <c r="B139" t="s">
-        <v>142</v>
+        <v>5</v>
+      </c>
+      <c r="C139" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
@@ -2826,7 +2838,7 @@
         <v>5</v>
       </c>
       <c r="C140" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
@@ -2837,7 +2849,7 @@
         <v>5</v>
       </c>
       <c r="C141" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
@@ -2845,10 +2857,7 @@
         <v>5</v>
       </c>
       <c r="B142" t="s">
-        <v>5</v>
-      </c>
-      <c r="C142" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
@@ -2859,7 +2868,7 @@
         <v>5</v>
       </c>
       <c r="C143" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
@@ -2870,7 +2879,7 @@
         <v>5</v>
       </c>
       <c r="C144" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
@@ -2878,7 +2887,10 @@
         <v>5</v>
       </c>
       <c r="B145" t="s">
-        <v>148</v>
+        <v>5</v>
+      </c>
+      <c r="C145" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
@@ -2889,7 +2901,7 @@
         <v>5</v>
       </c>
       <c r="C146" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
@@ -2900,7 +2912,7 @@
         <v>5</v>
       </c>
       <c r="C147" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
@@ -2908,7 +2920,7 @@
         <v>5</v>
       </c>
       <c r="B148" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
@@ -2919,7 +2931,7 @@
         <v>5</v>
       </c>
       <c r="C149" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
@@ -2930,7 +2942,7 @@
         <v>5</v>
       </c>
       <c r="C150" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
@@ -2941,12 +2953,18 @@
         <v>5</v>
       </c>
       <c r="C151" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>155</v>
+        <v>5</v>
+      </c>
+      <c r="B152" t="s">
+        <v>5</v>
+      </c>
+      <c r="C152" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
@@ -2954,7 +2972,10 @@
         <v>5</v>
       </c>
       <c r="B153" t="s">
-        <v>156</v>
+        <v>5</v>
+      </c>
+      <c r="C153" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
@@ -2962,12 +2983,18 @@
         <v>5</v>
       </c>
       <c r="B154" t="s">
-        <v>157</v>
+        <v>5</v>
+      </c>
+      <c r="C154" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>158</v>
+        <v>5</v>
+      </c>
+      <c r="B155" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
@@ -2975,7 +3002,10 @@
         <v>5</v>
       </c>
       <c r="B156" t="s">
-        <v>159</v>
+        <v>5</v>
+      </c>
+      <c r="C156" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
@@ -2986,7 +3016,7 @@
         <v>5</v>
       </c>
       <c r="C157" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
@@ -2997,15 +3027,12 @@
         <v>5</v>
       </c>
       <c r="C158" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>5</v>
-      </c>
-      <c r="B159" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
@@ -3013,15 +3040,18 @@
         <v>5</v>
       </c>
       <c r="B160" t="s">
-        <v>5</v>
-      </c>
-      <c r="C160" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>164</v>
+        <v>5</v>
+      </c>
+      <c r="B161" t="s">
+        <v>5</v>
+      </c>
+      <c r="C161" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
@@ -3029,7 +3059,10 @@
         <v>5</v>
       </c>
       <c r="B162" t="s">
-        <v>165</v>
+        <v>5</v>
+      </c>
+      <c r="C162" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
@@ -3040,7 +3073,7 @@
         <v>5</v>
       </c>
       <c r="C163" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
@@ -3051,7 +3084,7 @@
         <v>5</v>
       </c>
       <c r="C164" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
@@ -3062,7 +3095,7 @@
         <v>5</v>
       </c>
       <c r="C165" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
@@ -3070,10 +3103,7 @@
         <v>5</v>
       </c>
       <c r="B166" t="s">
-        <v>5</v>
-      </c>
-      <c r="C166" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
@@ -3084,7 +3114,7 @@
         <v>5</v>
       </c>
       <c r="C167" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
@@ -3095,7 +3125,7 @@
         <v>5</v>
       </c>
       <c r="C168" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
@@ -3103,7 +3133,7 @@
         <v>5</v>
       </c>
       <c r="B169" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
@@ -3114,7 +3144,7 @@
         <v>5</v>
       </c>
       <c r="C170" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
@@ -3125,20 +3155,23 @@
         <v>5</v>
       </c>
       <c r="C171" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>175</v>
+        <v>5</v>
+      </c>
+      <c r="B172" t="s">
+        <v>5</v>
+      </c>
+      <c r="C172" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>5</v>
-      </c>
-      <c r="B173" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
@@ -3146,10 +3179,7 @@
         <v>5</v>
       </c>
       <c r="B174" t="s">
-        <v>5</v>
-      </c>
-      <c r="C174" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
@@ -3157,7 +3187,10 @@
         <v>5</v>
       </c>
       <c r="B175" t="s">
-        <v>178</v>
+        <v>5</v>
+      </c>
+      <c r="C175" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
@@ -3168,7 +3201,7 @@
         <v>5</v>
       </c>
       <c r="C176" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
@@ -3176,7 +3209,7 @@
         <v>5</v>
       </c>
       <c r="B177" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
@@ -3187,15 +3220,12 @@
         <v>5</v>
       </c>
       <c r="C178" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>5</v>
-      </c>
-      <c r="B179" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
@@ -3203,10 +3233,7 @@
         <v>5</v>
       </c>
       <c r="B180" t="s">
-        <v>5</v>
-      </c>
-      <c r="C180" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
@@ -3217,12 +3244,15 @@
         <v>5</v>
       </c>
       <c r="C181" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>185</v>
+        <v>5</v>
+      </c>
+      <c r="B182" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.3">
@@ -3230,7 +3260,10 @@
         <v>5</v>
       </c>
       <c r="B183" t="s">
-        <v>186</v>
+        <v>5</v>
+      </c>
+      <c r="C183" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.3">
@@ -3238,10 +3271,7 @@
         <v>5</v>
       </c>
       <c r="B184" t="s">
-        <v>5</v>
-      </c>
-      <c r="C184" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.3">
@@ -3252,7 +3282,7 @@
         <v>5</v>
       </c>
       <c r="C185" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
@@ -3260,7 +3290,7 @@
         <v>5</v>
       </c>
       <c r="B186" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.3">
@@ -3271,7 +3301,7 @@
         <v>5</v>
       </c>
       <c r="C187" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.3">
@@ -3282,15 +3312,12 @@
         <v>5</v>
       </c>
       <c r="C188" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>5</v>
-      </c>
-      <c r="B189" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.3">
@@ -3298,15 +3325,18 @@
         <v>5</v>
       </c>
       <c r="B190" t="s">
-        <v>5</v>
-      </c>
-      <c r="C190" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>194</v>
+        <v>5</v>
+      </c>
+      <c r="B191" t="s">
+        <v>5</v>
+      </c>
+      <c r="C191" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.3">
@@ -3314,7 +3344,10 @@
         <v>5</v>
       </c>
       <c r="B192" t="s">
-        <v>195</v>
+        <v>5</v>
+      </c>
+      <c r="C192" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
@@ -3322,10 +3355,7 @@
         <v>5</v>
       </c>
       <c r="B193" t="s">
-        <v>5</v>
-      </c>
-      <c r="C193" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.3">
@@ -3333,7 +3363,72 @@
         <v>5</v>
       </c>
       <c r="B194" t="s">
+        <v>5</v>
+      </c>
+      <c r="C194" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A195" t="s">
+        <v>5</v>
+      </c>
+      <c r="B195" t="s">
+        <v>5</v>
+      </c>
+      <c r="C195" t="s">
         <v>197</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>5</v>
+      </c>
+      <c r="B196" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
+        <v>5</v>
+      </c>
+      <c r="B197" t="s">
+        <v>5</v>
+      </c>
+      <c r="C197" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A199" t="s">
+        <v>5</v>
+      </c>
+      <c r="B199" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
+        <v>5</v>
+      </c>
+      <c r="B200" t="s">
+        <v>5</v>
+      </c>
+      <c r="C200" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A201" t="s">
+        <v>5</v>
+      </c>
+      <c r="B201" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated descriptions based on latest mind map changes
</commit_message>
<xml_diff>
--- a/mind_maps/malware_capabilities_descriptions.xlsx
+++ b/mind_maps/malware_capabilities_descriptions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="403">
   <si>
     <t>Capability</t>
   </si>
@@ -1217,6 +1217,12 @@
   </si>
   <si>
     <t>The 'compromise data availabilty' value indicates that the malware instance compromises the availability of data on the system.</t>
+  </si>
+  <si>
+    <t>Control Self</t>
+  </si>
+  <si>
+    <t>The 'control self' value indicates that the malware instance can be controlled remotely, through commands or some other interface.</t>
   </si>
 </sst>
 </file>
@@ -2102,10 +2108,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F201"/>
+  <dimension ref="A1:F203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0">
-      <selection activeCell="B187" sqref="B187"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3421,24 +3427,15 @@
         <v>371</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>3</v>
-      </c>
+    <row r="105" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B105" s="6" t="s">
-        <v>377</v>
-      </c>
-      <c r="D105" s="4" t="s">
-        <v>378</v>
+        <v>401</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
-        <v>3</v>
-      </c>
-      <c r="B106" s="6" t="s">
-        <v>3</v>
-      </c>
       <c r="C106" t="s">
         <v>98</v>
       </c>
@@ -3490,40 +3487,37 @@
         <v>244</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>99</v>
-      </c>
-      <c r="D111" s="3" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="B111" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="D111" s="4" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>3</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>100</v>
+        <v>3</v>
+      </c>
+      <c r="C112" t="s">
+        <v>98</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="F112" s="10" t="s">
-        <v>245</v>
+        <v>379</v>
       </c>
     </row>
     <row r="113" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>3</v>
-      </c>
-      <c r="B113" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C113" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>247</v>
+        <v>381</v>
       </c>
     </row>
     <row r="114" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3531,43 +3525,46 @@
         <v>3</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>325</v>
+        <v>246</v>
+      </c>
+      <c r="F114" s="10" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="115" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
+        <v>3</v>
+      </c>
+      <c r="B115" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C115" t="s">
+        <v>101</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>3</v>
+      </c>
+      <c r="B116" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
         <v>103</v>
       </c>
-      <c r="D115" s="3" t="s">
+      <c r="D117" s="3" t="s">
         <v>248</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
-        <v>3</v>
-      </c>
-      <c r="B116" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="D116" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A117" t="s">
-        <v>3</v>
-      </c>
-      <c r="B117" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C117" t="s">
-        <v>105</v>
-      </c>
-      <c r="D117" s="3" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="118" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3575,24 +3572,24 @@
         <v>3</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C118" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>3</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>107</v>
+        <v>3</v>
+      </c>
+      <c r="C119" t="s">
+        <v>105</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>251</v>
+        <v>382</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3603,10 +3600,10 @@
         <v>3</v>
       </c>
       <c r="C120" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3614,16 +3611,10 @@
         <v>3</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C121" t="s">
-        <v>383</v>
+        <v>107</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="F121" s="10" t="s">
-        <v>275</v>
+        <v>251</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3631,10 +3622,13 @@
         <v>3</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>109</v>
+        <v>3</v>
+      </c>
+      <c r="C122" t="s">
+        <v>108</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3645,10 +3639,13 @@
         <v>3</v>
       </c>
       <c r="C123" t="s">
-        <v>110</v>
+        <v>383</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>260</v>
+        <v>253</v>
+      </c>
+      <c r="F123" s="10" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="124" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3656,13 +3653,10 @@
         <v>3</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C124" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="125" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3673,13 +3667,13 @@
         <v>3</v>
       </c>
       <c r="C125" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>3</v>
       </c>
@@ -3687,10 +3681,10 @@
         <v>3</v>
       </c>
       <c r="C126" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="127" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3701,82 +3695,85 @@
         <v>3</v>
       </c>
       <c r="C127" t="s">
+        <v>112</v>
+      </c>
+      <c r="D127" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>3</v>
+      </c>
+      <c r="B128" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C128" t="s">
+        <v>113</v>
+      </c>
+      <c r="D128" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>3</v>
+      </c>
+      <c r="B129" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C129" t="s">
         <v>114</v>
       </c>
-      <c r="D127" s="3" t="s">
+      <c r="D129" s="3" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A128" t="s">
-        <v>3</v>
-      </c>
-      <c r="B128" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C128" t="s">
+    <row r="130" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>3</v>
+      </c>
+      <c r="B130" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C130" t="s">
         <v>115</v>
       </c>
-      <c r="D128" s="3" t="s">
+      <c r="D130" s="3" t="s">
         <v>255</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A129" t="s">
-        <v>116</v>
-      </c>
-      <c r="D129" s="3" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A130" t="s">
-        <v>3</v>
-      </c>
-      <c r="B130" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="D130" s="3" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>3</v>
-      </c>
-      <c r="B131" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C131" t="s">
+        <v>116</v>
+      </c>
+      <c r="D131" s="3" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>3</v>
+      </c>
+      <c r="B132" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>3</v>
+      </c>
+      <c r="B133" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C133" t="s">
         <v>118</v>
       </c>
-      <c r="D131" s="3" t="s">
+      <c r="D133" s="3" t="s">
         <v>297</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A132" t="s">
-        <v>3</v>
-      </c>
-      <c r="B132" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C132" t="s">
-        <v>119</v>
-      </c>
-      <c r="D132" s="3" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A133" t="s">
-        <v>3</v>
-      </c>
-      <c r="B133" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D133" s="3" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -3787,10 +3784,10 @@
         <v>3</v>
       </c>
       <c r="C134" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>299</v>
+        <v>385</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -3798,21 +3795,24 @@
         <v>3</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C135" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>123</v>
+        <v>3</v>
+      </c>
+      <c r="B136" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C136" t="s">
+        <v>121</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>386</v>
+        <v>299</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -3820,38 +3820,32 @@
         <v>3</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>124</v>
+        <v>3</v>
+      </c>
+      <c r="C137" t="s">
+        <v>122</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>3</v>
-      </c>
-      <c r="B138" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C138" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>3</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C139" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>387</v>
+        <v>301</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -3862,10 +3856,10 @@
         <v>3</v>
       </c>
       <c r="C140" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>388</v>
+        <v>302</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -3876,10 +3870,10 @@
         <v>3</v>
       </c>
       <c r="C141" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -3887,13 +3881,16 @@
         <v>3</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>129</v>
+        <v>3</v>
+      </c>
+      <c r="C142" t="s">
+        <v>127</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>3</v>
       </c>
@@ -3901,10 +3898,10 @@
         <v>3</v>
       </c>
       <c r="C143" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>328</v>
+        <v>389</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -3912,13 +3909,10 @@
         <v>3</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C144" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>327</v>
+        <v>303</v>
       </c>
     </row>
     <row r="145" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3929,10 +3923,10 @@
         <v>3</v>
       </c>
       <c r="C145" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>304</v>
+        <v>328</v>
       </c>
     </row>
     <row r="146" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3943,10 +3937,10 @@
         <v>3</v>
       </c>
       <c r="C146" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>305</v>
+        <v>327</v>
       </c>
     </row>
     <row r="147" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3957,10 +3951,10 @@
         <v>3</v>
       </c>
       <c r="C147" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="148" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3968,10 +3962,13 @@
         <v>3</v>
       </c>
       <c r="B148" s="6" t="s">
-        <v>135</v>
+        <v>3</v>
+      </c>
+      <c r="C148" t="s">
+        <v>133</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="149" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3982,10 +3979,10 @@
         <v>3</v>
       </c>
       <c r="C149" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="150" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3993,13 +3990,10 @@
         <v>3</v>
       </c>
       <c r="B150" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C150" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="151" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4010,16 +4004,13 @@
         <v>3</v>
       </c>
       <c r="C151" t="s">
-        <v>390</v>
+        <v>136</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="F151" s="10" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>3</v>
       </c>
@@ -4027,13 +4018,10 @@
         <v>3</v>
       </c>
       <c r="C152" t="s">
-        <v>391</v>
+        <v>137</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="F152" s="10" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="153" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4044,13 +4032,16 @@
         <v>3</v>
       </c>
       <c r="C153" t="s">
-        <v>138</v>
+        <v>390</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>310</v>
+      </c>
+      <c r="F153" s="10" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>3</v>
       </c>
@@ -4058,10 +4049,13 @@
         <v>3</v>
       </c>
       <c r="C154" t="s">
-        <v>139</v>
+        <v>391</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>314</v>
+        <v>311</v>
+      </c>
+      <c r="F154" s="10" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="155" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4069,10 +4063,13 @@
         <v>3</v>
       </c>
       <c r="B155" s="6" t="s">
-        <v>140</v>
+        <v>3</v>
+      </c>
+      <c r="C155" t="s">
+        <v>138</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="156" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4083,10 +4080,10 @@
         <v>3</v>
       </c>
       <c r="C156" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="157" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4094,13 +4091,10 @@
         <v>3</v>
       </c>
       <c r="B157" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C157" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="158" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4111,18 +4105,24 @@
         <v>3</v>
       </c>
       <c r="C158" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="159" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>144</v>
+        <v>3</v>
+      </c>
+      <c r="B159" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C159" t="s">
+        <v>142</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>261</v>
+        <v>317</v>
       </c>
     </row>
     <row r="160" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4130,24 +4130,21 @@
         <v>3</v>
       </c>
       <c r="B160" s="6" t="s">
-        <v>145</v>
+        <v>3</v>
+      </c>
+      <c r="C160" t="s">
+        <v>143</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>263</v>
+        <v>318</v>
       </c>
     </row>
     <row r="161" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>3</v>
-      </c>
-      <c r="B161" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C161" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="162" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4155,13 +4152,10 @@
         <v>3</v>
       </c>
       <c r="B162" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C162" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="163" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4172,10 +4166,10 @@
         <v>3</v>
       </c>
       <c r="C163" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="164" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4186,10 +4180,10 @@
         <v>3</v>
       </c>
       <c r="C164" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="165" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4200,10 +4194,10 @@
         <v>3</v>
       </c>
       <c r="C165" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="166" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4211,10 +4205,13 @@
         <v>3</v>
       </c>
       <c r="B166" s="6" t="s">
-        <v>151</v>
+        <v>3</v>
+      </c>
+      <c r="C166" t="s">
+        <v>149</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>392</v>
+        <v>266</v>
       </c>
     </row>
     <row r="167" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4225,10 +4222,10 @@
         <v>3</v>
       </c>
       <c r="C167" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>393</v>
+        <v>267</v>
       </c>
     </row>
     <row r="168" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4236,24 +4233,24 @@
         <v>3</v>
       </c>
       <c r="B168" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C168" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>3</v>
       </c>
       <c r="B169" s="6" t="s">
-        <v>154</v>
+        <v>3</v>
+      </c>
+      <c r="C169" t="s">
+        <v>152</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="170" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4264,27 +4261,21 @@
         <v>3</v>
       </c>
       <c r="C170" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="F170" s="10" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>3</v>
       </c>
       <c r="B171" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C171" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>270</v>
+        <v>395</v>
       </c>
     </row>
     <row r="172" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4295,18 +4286,27 @@
         <v>3</v>
       </c>
       <c r="C172" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
+      </c>
+      <c r="F172" s="10" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="173" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>158</v>
+        <v>3</v>
+      </c>
+      <c r="B173" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C173" t="s">
+        <v>156</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
     </row>
     <row r="174" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4314,24 +4314,21 @@
         <v>3</v>
       </c>
       <c r="B174" s="6" t="s">
-        <v>159</v>
+        <v>3</v>
+      </c>
+      <c r="C174" t="s">
+        <v>157</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
     </row>
     <row r="175" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>3</v>
-      </c>
-      <c r="B175" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C175" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="176" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4339,13 +4336,10 @@
         <v>3</v>
       </c>
       <c r="B176" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C176" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="177" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4353,10 +4347,13 @@
         <v>3</v>
       </c>
       <c r="B177" s="6" t="s">
-        <v>162</v>
+        <v>3</v>
+      </c>
+      <c r="C177" t="s">
+        <v>160</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="178" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4367,71 +4364,71 @@
         <v>3</v>
       </c>
       <c r="C178" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="179" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
+        <v>3</v>
+      </c>
+      <c r="B179" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D179" s="3" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>3</v>
+      </c>
+      <c r="B180" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C180" t="s">
+        <v>163</v>
+      </c>
+      <c r="D180" s="3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
         <v>164</v>
       </c>
-      <c r="D179" s="3" t="s">
+      <c r="D181" s="3" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="180" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A180" t="s">
-        <v>3</v>
-      </c>
-      <c r="B180" s="6" t="s">
+    <row r="182" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
+        <v>3</v>
+      </c>
+      <c r="B182" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="D180" s="3" t="s">
+      <c r="D182" s="3" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="181" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A181" t="s">
-        <v>3</v>
-      </c>
-      <c r="B181" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C181" t="s">
+    <row r="183" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>3</v>
+      </c>
+      <c r="B183" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C183" t="s">
         <v>396</v>
       </c>
-      <c r="D181" s="3" t="s">
+      <c r="D183" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="F181" s="10" t="s">
+      <c r="F183" s="10" t="s">
         <v>330</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A182" t="s">
-        <v>3</v>
-      </c>
-      <c r="B182" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="D182" s="3" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A183" t="s">
-        <v>3</v>
-      </c>
-      <c r="B183" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C183" t="s">
-        <v>167</v>
-      </c>
-      <c r="D183" s="3" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="184" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4439,10 +4436,10 @@
         <v>3</v>
       </c>
       <c r="B184" s="6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="185" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4453,10 +4450,10 @@
         <v>3</v>
       </c>
       <c r="C185" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="186" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4464,10 +4461,10 @@
         <v>3</v>
       </c>
       <c r="B186" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="187" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4478,10 +4475,10 @@
         <v>3</v>
       </c>
       <c r="C187" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="188" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4489,21 +4486,24 @@
         <v>3</v>
       </c>
       <c r="B188" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C188" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="189" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>173</v>
+        <v>3</v>
+      </c>
+      <c r="B189" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C189" t="s">
+        <v>171</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>238</v>
+        <v>295</v>
       </c>
     </row>
     <row r="190" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4511,24 +4511,21 @@
         <v>3</v>
       </c>
       <c r="B190" s="6" t="s">
-        <v>174</v>
+        <v>3</v>
+      </c>
+      <c r="C190" t="s">
+        <v>172</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="191" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>3</v>
-      </c>
-      <c r="B191" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C191" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D191" s="3" t="s">
-        <v>398</v>
+        <v>238</v>
       </c>
     </row>
     <row r="192" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4536,13 +4533,10 @@
         <v>3</v>
       </c>
       <c r="B192" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C192" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="193" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -4550,13 +4544,16 @@
         <v>3</v>
       </c>
       <c r="B193" s="6" t="s">
-        <v>177</v>
+        <v>3</v>
+      </c>
+      <c r="C193" t="s">
+        <v>175</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>3</v>
       </c>
@@ -4564,10 +4561,10 @@
         <v>3</v>
       </c>
       <c r="C194" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>241</v>
+        <v>399</v>
       </c>
     </row>
     <row r="195" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -4575,81 +4572,106 @@
         <v>3</v>
       </c>
       <c r="B195" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C195" t="s">
+        <v>177</v>
+      </c>
+      <c r="D195" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>3</v>
+      </c>
+      <c r="B196" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C196" t="s">
+        <v>178</v>
+      </c>
+      <c r="D196" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
+        <v>3</v>
+      </c>
+      <c r="B197" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C197" t="s">
         <v>179</v>
       </c>
-      <c r="D195" s="3" t="s">
+      <c r="D197" s="3" t="s">
         <v>240</v>
-      </c>
-    </row>
-    <row r="196" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A196" t="s">
-        <v>3</v>
-      </c>
-      <c r="B196" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="D196" s="3" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="197" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A197" t="s">
-        <v>3</v>
-      </c>
-      <c r="B197" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C197" t="s">
-        <v>181</v>
-      </c>
-      <c r="D197" s="3" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="198" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>182</v>
+        <v>3</v>
+      </c>
+      <c r="B198" s="6" t="s">
+        <v>180</v>
       </c>
       <c r="D198" s="3" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="199" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>3</v>
       </c>
       <c r="B199" s="6" t="s">
-        <v>183</v>
+        <v>3</v>
+      </c>
+      <c r="C199" t="s">
+        <v>181</v>
       </c>
       <c r="D199" s="3" t="s">
-        <v>235</v>
+        <v>331</v>
       </c>
     </row>
     <row r="200" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>3</v>
-      </c>
-      <c r="B200" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C200" t="s">
+        <v>182</v>
+      </c>
+      <c r="D200" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A201" t="s">
+        <v>3</v>
+      </c>
+      <c r="B201" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="D201" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>3</v>
+      </c>
+      <c r="B202" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C202" t="s">
         <v>184</v>
       </c>
-      <c r="D200" s="3" t="s">
+      <c r="D202" s="3" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="201" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A201" t="s">
-        <v>3</v>
-      </c>
-      <c r="B201" s="6" t="s">
+    <row r="203" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
+        <v>3</v>
+      </c>
+      <c r="B203" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="D201" s="3" t="s">
+      <c r="D203" s="3" t="s">
         <v>236</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Small tweaks and updates to Spying objectives
</commit_message>
<xml_diff>
--- a/mind_maps/malware_capabilities_descriptions.xlsx
+++ b/mind_maps/malware_capabilities_descriptions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="15960" windowHeight="12810"/>
+    <workbookView xWindow="0" yWindow="36" windowWidth="15960" windowHeight="12816"/>
   </bookViews>
   <sheets>
     <sheet name="malware_capabilities" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="420">
   <si>
     <t>Capability</t>
   </si>
@@ -301,9 +301,6 @@
     <t xml:space="preserve"> Disable OS Security Alerts</t>
   </si>
   <si>
-    <t xml:space="preserve"> Disable User Account Control (UAC)</t>
-  </si>
-  <si>
     <t>The ‘disable access controls’ value indicates that the malware instance is able to bypass access control mechanisms designed to prevent unauthorized or unprivileged use or execution of applications or files.</t>
   </si>
   <si>
@@ -529,9 +526,6 @@
     <t>Spying</t>
   </si>
   <si>
-    <t xml:space="preserve"> Capture System Peripheral Data</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Capture Keyboard Input</t>
   </si>
   <si>
@@ -541,12 +535,6 @@
     <t xml:space="preserve"> Capture Touchscreen Input</t>
   </si>
   <si>
-    <t xml:space="preserve"> Capture Microphone</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Capture Camera</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Capture System Interface Data</t>
   </si>
   <si>
@@ -631,9 +619,6 @@
     <t>The 'compromise system availability' value indicates that the malware instance compromises the availability of the system.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Compromise Network Server Availability (DOS)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Compromise Local System Availability</t>
   </si>
   <si>
@@ -664,9 +649,6 @@
     <t>The ‘remove sms warning messages’ value indicates that the malware instance is able to capture the message body of incoming SMS messages and abort the broadcasting of a message that meets a certain criteria.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Disable Host-based/OS Access Controls</t>
-  </si>
-  <si>
     <t>The 'infection/propagation' Capability indicates that the malware instance is able to propagate through the infection of a machine or is able to infect a file after executing on a system.  The malware instance may infect actively (e.g., gain access to a machine directly) or passively (e.g., send malicious email).  This Capability does not encompass any aspects of the initial infection that is done independently of the malware instance itself.</t>
   </si>
   <si>
@@ -1006,9 +988,6 @@
     <t>The 'steal dialed phone numbers' value indicates that the malware instance is able to steal the list of phone numbers that a user has dialed.</t>
   </si>
   <si>
-    <t>The 'capture system peripheral data' value indicates that the malware instance is able to capture data from a system's peripheral devices.</t>
-  </si>
-  <si>
     <t>The 'capture keyboard input' value indicates that the malware instance is able to capture data from a system's keyboard.</t>
   </si>
   <si>
@@ -1036,9 +1015,6 @@
     <t>The 'capture system screenshot' value indicates that the malware instance is able to capture images of what is currently being displayed on a system's screen.</t>
   </si>
   <si>
-    <t>The 'steal network address' value indicates that the malware instance is able to steal information about the network addresses used by the system on which it is running.</t>
-  </si>
-  <si>
     <t>The 'capture system memory dump' value indicates that the malware instance is able to capture data from a system's RAM.</t>
   </si>
   <si>
@@ -1153,9 +1129,6 @@
     <t>The 'steal user data' value indicates that the malware instance is able to steal user data (e.g., email).</t>
   </si>
   <si>
-    <t>The 'steal system information' value indicates that the malware instance is able to steal information about the system on which it is running (e.g., network address data).</t>
-  </si>
-  <si>
     <t>The 'capture system state data' value indicates that the malware instance is able to capture information about a system's state (e.g., from its RAM).</t>
   </si>
   <si>
@@ -1198,9 +1171,6 @@
     <t>is it necessarily the system on which the malware instance is running?</t>
   </si>
   <si>
-    <t>The 'spying' Capability indicates that the malware instance is able to capture information from the system related to user or system activity (e.g., from a system's peripheral devices).</t>
-  </si>
-  <si>
     <t>The 'steal pki software certificate' value indicates that the malware instance is able to steal one or more public key infrastructure (PKI) software certficates.</t>
   </si>
   <si>
@@ -1225,15 +1195,6 @@
     <t>The 'annoy remote user' value indicates that the malware instance is able to annoy a remote user.</t>
   </si>
   <si>
-    <t>The 'steal open port' value indicates that the malware instance is able to steal information about the open ports on the system on which it is running.</t>
-  </si>
-  <si>
-    <t>The 'steal make/model' value indicates that the malware instance is able to steal the information on the make and/or model of the system on which it is running.</t>
-  </si>
-  <si>
-    <t>The 'compromise network server availability (DOS)' value indicates that the malware instance is able to cause a server to be unavailable (otherwise known as a denial of service (DOS)).</t>
-  </si>
-  <si>
     <t>The 'overload sandbox' value indicates that the malware instance is able to overload a sandbox (e.g., by generating a flood of meaningless behavioral data).</t>
   </si>
   <si>
@@ -1262,6 +1223,57 @@
   </si>
   <si>
     <t>is it necessarily the system on which the malware instance is running?  Maybe should be, "…steal information about a system" (with "a" system, not "the" system - could be another system on the same network as the compromised machine).</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Disable User Account Control</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Disable [Host-based or OS] Access Controls</t>
+  </si>
+  <si>
+    <t>The 'steal system information' value indicates that the malware instance is able to steal information about a system (e.g., network address data).</t>
+  </si>
+  <si>
+    <t>The 'steal network address' value indicates that the malware instance is able to steal information about the network addresses used by a system.</t>
+  </si>
+  <si>
+    <t>The 'steal open port' value indicates that the malware instance is able to steal information about the open ports on a system.</t>
+  </si>
+  <si>
+    <t>The 'steal make/model' value indicates that the malware instance is able to steal the information on the make and/or model of a system.</t>
+  </si>
+  <si>
+    <t>The 'spying' Capability indicates that the malware instance is able to capture information from a system related to user or system activity (e.g., from a system's peripheral devices).</t>
+  </si>
+  <si>
+    <t>Denial of Service</t>
+  </si>
+  <si>
+    <t>The 'denial of service' value indicates that the malware instance is able to cause a server to be unavailable, otherwise known as a denial of service (DOS).</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Capture Microphone Input</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Capture Camera Input</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Capture System Input Peripheral Data</t>
+  </si>
+  <si>
+    <t>The 'capture system input peripheral data' value indicates that the malware instance is able to capture data from a system's input peripheral devices.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Capture System Output Peripheral Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Capture Printer Output</t>
+  </si>
+  <si>
+    <t>The 'capture printer output' value indicates that the malware instance is able to capture data sent to a system's printer.</t>
+  </si>
+  <si>
+    <t>The 'capture system output peripheral data' value indicates that the malware instance is able to capture data sent to a system's output peripheral devices.</t>
   </si>
 </sst>
 </file>
@@ -1851,24 +1863,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV202"/>
+  <dimension ref="A1:IV204"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F159" sqref="F159"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B160" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D170" sqref="D170"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.61328125" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" style="26" customWidth="1"/>
     <col min="2" max="2" width="29" style="26" customWidth="1"/>
-    <col min="3" max="3" width="33.59765625" style="26" customWidth="1"/>
-    <col min="4" max="4" width="46.09765625" style="21" customWidth="1"/>
-    <col min="5" max="5" width="9.19921875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="37.3984375" style="1" customWidth="1"/>
-    <col min="7" max="256" width="6.59765625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33.61328125" style="26" customWidth="1"/>
+    <col min="4" max="4" width="46.07421875" style="21" customWidth="1"/>
+    <col min="5" max="5" width="9.23046875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="37.3828125" style="1" customWidth="1"/>
+    <col min="7" max="256" width="6.61328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1888,19 +1900,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
       <c r="D2" s="22" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -1909,12 +1921,12 @@
       </c>
       <c r="C3" s="25"/>
       <c r="D3" s="18" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
@@ -1925,12 +1937,12 @@
         <v>9</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
@@ -1941,12 +1953,12 @@
         <v>10</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
@@ -1957,12 +1969,12 @@
         <v>11</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
@@ -1971,12 +1983,12 @@
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="18" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
@@ -1987,12 +1999,12 @@
         <v>13</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="11"/>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
@@ -2003,24 +2015,24 @@
         <v>14</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="25"/>
       <c r="C10" s="25"/>
       <c r="D10" s="18" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="11"/>
     </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>7</v>
       </c>
@@ -2029,12 +2041,12 @@
       </c>
       <c r="C11" s="25"/>
       <c r="D11" s="18" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="11"/>
     </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>7</v>
       </c>
@@ -2045,12 +2057,12 @@
         <v>17</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>7</v>
       </c>
@@ -2061,12 +2073,12 @@
         <v>18</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="11"/>
     </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>7</v>
       </c>
@@ -2075,12 +2087,12 @@
       </c>
       <c r="C14" s="25"/>
       <c r="D14" s="18" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="11"/>
     </row>
-    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>7</v>
       </c>
@@ -2091,24 +2103,24 @@
         <v>20</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="11"/>
     </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="25"/>
       <c r="B16" s="25"/>
       <c r="C16" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="11"/>
     </row>
-    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>7</v>
       </c>
@@ -2119,24 +2131,24 @@
         <v>22</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>406</v>
+        <v>393</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="11"/>
     </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25"/>
       <c r="D18" s="18" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="11"/>
     </row>
-    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>7</v>
       </c>
@@ -2145,12 +2157,12 @@
       </c>
       <c r="C19" s="25"/>
       <c r="D19" s="18" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="11"/>
     </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>7</v>
       </c>
@@ -2161,12 +2173,12 @@
         <v>25</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="11"/>
     </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>7</v>
       </c>
@@ -2177,12 +2189,12 @@
         <v>26</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="13"/>
     </row>
-    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>7</v>
       </c>
@@ -2191,12 +2203,12 @@
       </c>
       <c r="C22" s="25"/>
       <c r="D22" s="18" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="13"/>
     </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>7</v>
       </c>
@@ -2207,12 +2219,12 @@
         <v>28</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="9"/>
     </row>
-    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>7</v>
       </c>
@@ -2223,14 +2235,14 @@
         <v>29</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="E24" s="10"/>
       <c r="F24" s="12" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>7</v>
       </c>
@@ -2241,12 +2253,12 @@
         <v>30</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>7</v>
       </c>
@@ -2257,12 +2269,12 @@
         <v>31</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E26" s="8"/>
       <c r="F26" s="13"/>
     </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>7</v>
       </c>
@@ -2273,12 +2285,12 @@
         <v>32</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="E27" s="8"/>
       <c r="F27" s="11"/>
     </row>
-    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>7</v>
       </c>
@@ -2287,12 +2299,12 @@
       </c>
       <c r="C28" s="25"/>
       <c r="D28" s="18" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="E28" s="8"/>
       <c r="F28" s="11"/>
     </row>
-    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>7</v>
       </c>
@@ -2303,12 +2315,12 @@
         <v>34</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="E29" s="8"/>
       <c r="F29" s="11"/>
     </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>7</v>
       </c>
@@ -2324,7 +2336,7 @@
       <c r="E30" s="8"/>
       <c r="F30" s="11"/>
     </row>
-    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>7</v>
       </c>
@@ -2335,24 +2347,24 @@
         <v>37</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="E31" s="8"/>
       <c r="F31" s="11"/>
     </row>
-    <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B32" s="25"/>
       <c r="C32" s="25"/>
       <c r="D32" s="18" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="E32" s="8"/>
       <c r="F32" s="14"/>
     </row>
-    <row r="33" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>7</v>
       </c>
@@ -2361,12 +2373,12 @@
       </c>
       <c r="C33" s="25"/>
       <c r="D33" s="18" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="E33" s="8"/>
       <c r="F33" s="11"/>
     </row>
-    <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>7</v>
       </c>
@@ -2377,12 +2389,12 @@
         <v>40</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="E34" s="8"/>
       <c r="F34" s="11"/>
     </row>
-    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>7</v>
       </c>
@@ -2393,12 +2405,12 @@
         <v>41</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="E35" s="8"/>
       <c r="F35" s="11"/>
     </row>
-    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>7</v>
       </c>
@@ -2409,12 +2421,12 @@
         <v>42</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="E36" s="8"/>
       <c r="F36" s="11"/>
     </row>
-    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
         <v>7</v>
       </c>
@@ -2423,12 +2435,12 @@
       </c>
       <c r="C37" s="25"/>
       <c r="D37" s="18" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="E37" s="8"/>
       <c r="F37" s="11"/>
     </row>
-    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>7</v>
       </c>
@@ -2439,12 +2451,12 @@
         <v>44</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="E38" s="8"/>
       <c r="F38" s="11"/>
     </row>
-    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>7</v>
       </c>
@@ -2455,36 +2467,36 @@
         <v>45</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="E39" s="8"/>
       <c r="F39" s="11"/>
     </row>
-    <row r="40" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="25"/>
       <c r="B40" s="25"/>
       <c r="C40" s="7" t="s">
         <v>46</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="E40" s="8"/>
       <c r="F40" s="11"/>
     </row>
-    <row r="41" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>47</v>
       </c>
       <c r="B41" s="25"/>
       <c r="C41" s="25"/>
       <c r="D41" s="27" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="E41" s="8"/>
       <c r="F41" s="13"/>
     </row>
-    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>7</v>
       </c>
@@ -2493,12 +2505,12 @@
       </c>
       <c r="C42" s="25"/>
       <c r="D42" s="18" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="E42" s="8"/>
       <c r="F42" s="11"/>
     </row>
-    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>7</v>
       </c>
@@ -2509,12 +2521,12 @@
         <v>49</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="E43" s="8"/>
       <c r="F43" s="11"/>
     </row>
-    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>7</v>
       </c>
@@ -2525,12 +2537,12 @@
         <v>50</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="E44" s="8"/>
       <c r="F44" s="11"/>
     </row>
-    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
         <v>7</v>
       </c>
@@ -2541,12 +2553,12 @@
         <v>51</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="E45" s="8"/>
       <c r="F45" s="11"/>
     </row>
-    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
         <v>7</v>
       </c>
@@ -2557,12 +2569,12 @@
         <v>52</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="E46" s="8"/>
       <c r="F46" s="11"/>
     </row>
-    <row r="47" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
         <v>7</v>
       </c>
@@ -2573,12 +2585,12 @@
         <v>53</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="E47" s="8"/>
       <c r="F47" s="11"/>
     </row>
-    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>7</v>
       </c>
@@ -2587,12 +2599,12 @@
       </c>
       <c r="C48" s="25"/>
       <c r="D48" s="18" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="E48" s="8"/>
       <c r="F48" s="11"/>
     </row>
-    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>7</v>
       </c>
@@ -2603,12 +2615,12 @@
         <v>55</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="E49" s="8"/>
       <c r="F49" s="11"/>
     </row>
-    <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
         <v>7</v>
       </c>
@@ -2619,12 +2631,12 @@
         <v>56</v>
       </c>
       <c r="D50" s="18" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="E50" s="8"/>
       <c r="F50" s="11"/>
     </row>
-    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
         <v>7</v>
       </c>
@@ -2635,12 +2647,12 @@
         <v>57</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="E51" s="8"/>
       <c r="F51" s="11"/>
     </row>
-    <row r="52" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>7</v>
       </c>
@@ -2651,12 +2663,12 @@
         <v>58</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="E52" s="8"/>
       <c r="F52" s="11"/>
     </row>
-    <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
         <v>7</v>
       </c>
@@ -2667,12 +2679,12 @@
         <v>59</v>
       </c>
       <c r="D53" s="18" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E53" s="8"/>
       <c r="F53" s="11"/>
     </row>
-    <row r="54" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
         <v>7</v>
       </c>
@@ -2683,12 +2695,12 @@
         <v>60</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="E54" s="10"/>
       <c r="F54" s="11"/>
     </row>
-    <row r="55" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
         <v>7</v>
       </c>
@@ -2699,12 +2711,12 @@
         <v>61</v>
       </c>
       <c r="D55" s="27" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="E55" s="10"/>
       <c r="F55" s="11"/>
     </row>
-    <row r="56" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
         <v>7</v>
       </c>
@@ -2715,12 +2727,12 @@
         <v>62</v>
       </c>
       <c r="D56" s="27" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="E56" s="10"/>
       <c r="F56" s="11"/>
     </row>
-    <row r="57" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="s">
         <v>7</v>
       </c>
@@ -2729,12 +2741,12 @@
       </c>
       <c r="C57" s="25"/>
       <c r="D57" s="18" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="E57" s="8"/>
       <c r="F57" s="11"/>
     </row>
-    <row r="58" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
         <v>7</v>
       </c>
@@ -2745,12 +2757,12 @@
         <v>64</v>
       </c>
       <c r="D58" s="18" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="E58" s="10"/>
       <c r="F58" s="11"/>
     </row>
-    <row r="59" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
         <v>7</v>
       </c>
@@ -2761,12 +2773,12 @@
         <v>65</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="E59" s="10"/>
       <c r="F59" s="11"/>
     </row>
-    <row r="60" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
         <v>7</v>
       </c>
@@ -2777,12 +2789,12 @@
         <v>66</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="E60" s="8"/>
       <c r="F60" s="11"/>
     </row>
-    <row r="61" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
         <v>7</v>
       </c>
@@ -2791,12 +2803,12 @@
       </c>
       <c r="C61" s="25"/>
       <c r="D61" s="18" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="E61" s="8"/>
       <c r="F61" s="11"/>
     </row>
-    <row r="62" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A62" s="7" t="s">
         <v>7</v>
       </c>
@@ -2807,12 +2819,12 @@
         <v>68</v>
       </c>
       <c r="D62" s="19" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="E62" s="8"/>
       <c r="F62" s="11"/>
     </row>
-    <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
         <v>7</v>
       </c>
@@ -2821,12 +2833,12 @@
       </c>
       <c r="C63" s="25"/>
       <c r="D63" s="18" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="E63" s="8"/>
       <c r="F63" s="11"/>
     </row>
-    <row r="64" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="7" t="s">
         <v>7</v>
       </c>
@@ -2837,12 +2849,12 @@
         <v>70</v>
       </c>
       <c r="D64" s="18" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="E64" s="8"/>
       <c r="F64" s="11"/>
     </row>
-    <row r="65" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="7" t="s">
         <v>7</v>
       </c>
@@ -2858,7 +2870,7 @@
       <c r="E65" s="8"/>
       <c r="F65" s="11"/>
     </row>
-    <row r="66" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
         <v>7</v>
       </c>
@@ -2867,12 +2879,12 @@
       </c>
       <c r="C66" s="25"/>
       <c r="D66" s="18" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="E66" s="8"/>
       <c r="F66" s="11"/>
     </row>
-    <row r="67" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="7" t="s">
         <v>7</v>
       </c>
@@ -2883,24 +2895,24 @@
         <v>74</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="E67" s="10"/>
       <c r="F67" s="11"/>
     </row>
-    <row r="68" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A68" s="7" t="s">
         <v>75</v>
       </c>
       <c r="B68" s="25"/>
       <c r="C68" s="25"/>
       <c r="D68" s="18" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="E68" s="8"/>
       <c r="F68" s="11"/>
     </row>
-    <row r="69" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A69" s="7" t="s">
         <v>7</v>
       </c>
@@ -2909,12 +2921,12 @@
       </c>
       <c r="C69" s="25"/>
       <c r="D69" s="18" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="E69" s="8"/>
       <c r="F69" s="11"/>
     </row>
-    <row r="70" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A70" s="7" t="s">
         <v>7</v>
       </c>
@@ -2925,12 +2937,12 @@
         <v>77</v>
       </c>
       <c r="D70" s="18" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="E70" s="8"/>
       <c r="F70" s="11"/>
     </row>
-    <row r="71" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A71" s="7" t="s">
         <v>7</v>
       </c>
@@ -2941,12 +2953,12 @@
         <v>78</v>
       </c>
       <c r="D71" s="18" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="E71" s="8"/>
       <c r="F71" s="11"/>
     </row>
-    <row r="72" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" s="7" t="s">
         <v>7</v>
       </c>
@@ -2957,12 +2969,12 @@
         <v>79</v>
       </c>
       <c r="D72" s="18" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="E72" s="8"/>
       <c r="F72" s="11"/>
     </row>
-    <row r="73" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" s="7" t="s">
         <v>7</v>
       </c>
@@ -2976,7 +2988,7 @@
       <c r="E73" s="8"/>
       <c r="F73" s="11"/>
     </row>
-    <row r="74" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" s="7" t="s">
         <v>7</v>
       </c>
@@ -2987,12 +2999,12 @@
         <v>82</v>
       </c>
       <c r="D74" s="18" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="E74" s="8"/>
       <c r="F74" s="11"/>
     </row>
-    <row r="75" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A75" s="7" t="s">
         <v>7</v>
       </c>
@@ -3001,12 +3013,12 @@
       </c>
       <c r="C75" s="25"/>
       <c r="D75" s="18" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="E75" s="8"/>
       <c r="F75" s="11"/>
     </row>
-    <row r="76" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" s="7" t="s">
         <v>7</v>
       </c>
@@ -3022,19 +3034,19 @@
       <c r="E76" s="8"/>
       <c r="F76" s="11"/>
     </row>
-    <row r="77" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" s="7" t="s">
         <v>86</v>
       </c>
       <c r="B77" s="25"/>
       <c r="C77" s="25"/>
       <c r="D77" s="18" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E77" s="8"/>
       <c r="F77" s="11"/>
     </row>
-    <row r="78" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A78" s="7" t="s">
         <v>7</v>
       </c>
@@ -3043,12 +3055,12 @@
       </c>
       <c r="C78" s="25"/>
       <c r="D78" s="18" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="E78" s="8"/>
       <c r="F78" s="11"/>
     </row>
-    <row r="79" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A79" s="7" t="s">
         <v>7</v>
       </c>
@@ -3059,12 +3071,12 @@
         <v>88</v>
       </c>
       <c r="D79" s="18" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E79" s="8"/>
       <c r="F79" s="11"/>
     </row>
-    <row r="80" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A80" s="7" t="s">
         <v>7</v>
       </c>
@@ -3073,12 +3085,12 @@
       </c>
       <c r="C80" s="25"/>
       <c r="D80" s="18" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="E80" s="8"/>
       <c r="F80" s="11"/>
     </row>
-    <row r="81" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A81" s="7" t="s">
         <v>7</v>
       </c>
@@ -3094,7 +3106,7 @@
       <c r="E81" s="8"/>
       <c r="F81" s="11"/>
     </row>
-    <row r="82" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A82" s="7" t="s">
         <v>7</v>
       </c>
@@ -3110,7 +3122,7 @@
       <c r="E82" s="8"/>
       <c r="F82" s="11"/>
     </row>
-    <row r="83" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A83" s="7" t="s">
         <v>7</v>
       </c>
@@ -3121,12 +3133,12 @@
         <v>94</v>
       </c>
       <c r="D83" s="18" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="E83" s="8"/>
       <c r="F83" s="11"/>
     </row>
-    <row r="84" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A84" s="7" t="s">
         <v>7</v>
       </c>
@@ -3134,49 +3146,49 @@
         <v>7</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>95</v>
+        <v>403</v>
       </c>
       <c r="D84" s="18" t="s">
-        <v>409</v>
+        <v>396</v>
       </c>
       <c r="E84" s="8"/>
       <c r="F84" s="28" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A85" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>216</v>
+        <v>404</v>
       </c>
       <c r="C85" s="25"/>
       <c r="D85" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E85" s="8"/>
       <c r="F85" s="15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A86" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C86" s="7" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A86" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B86" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C86" s="7" t="s">
-        <v>98</v>
-      </c>
       <c r="D86" s="18" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="E86" s="8"/>
       <c r="F86" s="11"/>
     </row>
-    <row r="87" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A87" s="7" t="s">
         <v>7</v>
       </c>
@@ -3184,15 +3196,15 @@
         <v>7</v>
       </c>
       <c r="C87" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D87" s="19" t="s">
         <v>99</v>
-      </c>
-      <c r="D87" s="19" t="s">
-        <v>100</v>
       </c>
       <c r="E87" s="8"/>
       <c r="F87" s="11"/>
     </row>
-    <row r="88" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A88" s="7" t="s">
         <v>7</v>
       </c>
@@ -3200,29 +3212,29 @@
         <v>7</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D88" s="20" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="E88" s="8"/>
       <c r="F88" s="11"/>
     </row>
-    <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A89" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C89" s="25"/>
       <c r="D89" s="20" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="E89" s="8"/>
       <c r="F89" s="11"/>
     </row>
-    <row r="90" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A90" s="7" t="s">
         <v>7</v>
       </c>
@@ -3230,15 +3242,15 @@
         <v>7</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D90" s="20" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E90" s="8"/>
       <c r="F90" s="11"/>
     </row>
-    <row r="91" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A91" s="7" t="s">
         <v>7</v>
       </c>
@@ -3246,29 +3258,29 @@
         <v>7</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D91" s="20" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="E91" s="8"/>
       <c r="F91" s="11"/>
     </row>
-    <row r="92" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A92" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C92" s="25"/>
       <c r="D92" s="20" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="E92" s="8"/>
       <c r="F92" s="11"/>
     </row>
-    <row r="93" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A93" s="7" t="s">
         <v>7</v>
       </c>
@@ -3276,15 +3288,15 @@
         <v>7</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D93" s="20" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="E93" s="8"/>
       <c r="F93" s="11"/>
     </row>
-    <row r="94" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A94" s="7" t="s">
         <v>7</v>
       </c>
@@ -3292,15 +3304,15 @@
         <v>7</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D94" s="20" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="E94" s="8"/>
       <c r="F94" s="11"/>
     </row>
-    <row r="95" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A95" s="7" t="s">
         <v>7</v>
       </c>
@@ -3308,15 +3320,15 @@
         <v>7</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D95" s="20" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="E95" s="8"/>
       <c r="F95" s="11"/>
     </row>
-    <row r="96" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A96" s="7" t="s">
         <v>7</v>
       </c>
@@ -3324,15 +3336,15 @@
         <v>7</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D96" s="20" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="E96" s="8"/>
       <c r="F96" s="11"/>
     </row>
-    <row r="97" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A97" s="7" t="s">
         <v>7</v>
       </c>
@@ -3340,41 +3352,41 @@
         <v>7</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D97" s="20" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="E97" s="8"/>
       <c r="F97" s="11"/>
     </row>
-    <row r="98" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A98" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B98" s="25"/>
       <c r="C98" s="25"/>
       <c r="D98" s="19" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
       <c r="E98" s="8"/>
       <c r="F98" s="11"/>
     </row>
-    <row r="99" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C99" s="25"/>
       <c r="D99" s="19" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="E99" s="8"/>
       <c r="F99" s="11"/>
     </row>
-    <row r="100" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A100" s="7" t="s">
         <v>7</v>
       </c>
@@ -3382,15 +3394,15 @@
         <v>7</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D100" s="18" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
       <c r="E100" s="8"/>
       <c r="F100" s="11"/>
     </row>
-    <row r="101" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A101" s="7" t="s">
         <v>7</v>
       </c>
@@ -3398,29 +3410,29 @@
         <v>7</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D101" s="19" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="E101" s="10"/>
       <c r="F101" s="11"/>
     </row>
-    <row r="102" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A102" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B102" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C102" s="25"/>
       <c r="D102" s="19" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="E102" s="8"/>
       <c r="F102" s="11"/>
     </row>
-    <row r="103" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A103" s="7" t="s">
         <v>7</v>
       </c>
@@ -3428,79 +3440,79 @@
         <v>7</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D103" s="19" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="E103" s="8"/>
       <c r="F103" s="11"/>
     </row>
-    <row r="104" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A104" s="25"/>
       <c r="B104" s="16" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="C104" s="25"/>
       <c r="D104" s="19" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="E104" s="8"/>
       <c r="F104" s="11"/>
     </row>
-    <row r="105" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A105" s="25"/>
       <c r="B105" s="25"/>
       <c r="C105" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D105" s="19" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="E105" s="8"/>
       <c r="F105" s="11"/>
     </row>
-    <row r="106" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A106" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B106" s="25"/>
       <c r="C106" s="25"/>
       <c r="D106" s="19" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E106" s="8"/>
       <c r="F106" s="11"/>
     </row>
-    <row r="107" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A107" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C107" s="25"/>
       <c r="D107" s="19" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E107" s="8"/>
       <c r="F107" s="11"/>
     </row>
-    <row r="108" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A108" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C108" s="25"/>
       <c r="D108" s="19" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E108" s="8"/>
       <c r="F108" s="11"/>
     </row>
-    <row r="109" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109" s="7" t="s">
         <v>7</v>
       </c>
@@ -3508,29 +3520,29 @@
         <v>7</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D109" s="19" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E109" s="8"/>
       <c r="F109" s="11"/>
     </row>
-    <row r="110" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A110" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C110" s="25"/>
       <c r="D110" s="19" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E110" s="8"/>
       <c r="F110" s="11"/>
     </row>
-    <row r="111" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A111" s="7" t="s">
         <v>7</v>
       </c>
@@ -3538,41 +3550,41 @@
         <v>7</v>
       </c>
       <c r="C111" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D111" s="19" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="E111" s="8"/>
       <c r="F111" s="11"/>
     </row>
-    <row r="112" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A112" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B112" s="25"/>
       <c r="C112" s="25"/>
       <c r="D112" s="19" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="E112" s="8"/>
       <c r="F112" s="11"/>
     </row>
-    <row r="113" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A113" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C113" s="25"/>
       <c r="D113" s="19" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="E113" s="10"/>
       <c r="F113" s="11"/>
     </row>
-    <row r="114" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A114" s="7" t="s">
         <v>7</v>
       </c>
@@ -3580,55 +3592,55 @@
         <v>7</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D114" s="19" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="E114" s="8"/>
       <c r="F114" s="11"/>
     </row>
-    <row r="115" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A115" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C115" s="25"/>
       <c r="D115" s="19" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="E115" s="8"/>
       <c r="F115" s="11"/>
     </row>
-    <row r="116" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A116" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B116" s="25"/>
       <c r="C116" s="25"/>
       <c r="D116" s="19" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="E116" s="8"/>
       <c r="F116" s="11"/>
     </row>
-    <row r="117" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A117" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C117" s="25"/>
       <c r="D117" s="19" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="E117" s="8"/>
       <c r="F117" s="11"/>
     </row>
-    <row r="118" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A118" s="7" t="s">
         <v>7</v>
       </c>
@@ -3636,15 +3648,15 @@
         <v>7</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D118" s="19" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="E118" s="8"/>
       <c r="F118" s="11"/>
     </row>
-    <row r="119" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A119" s="7" t="s">
         <v>7</v>
       </c>
@@ -3652,29 +3664,29 @@
         <v>7</v>
       </c>
       <c r="C119" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D119" s="19" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E119" s="8"/>
       <c r="F119" s="11"/>
     </row>
-    <row r="120" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A120" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C120" s="25"/>
       <c r="D120" s="19" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="E120" s="8"/>
       <c r="F120" s="11"/>
     </row>
-    <row r="121" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A121" s="7" t="s">
         <v>7</v>
       </c>
@@ -3682,15 +3694,15 @@
         <v>7</v>
       </c>
       <c r="C121" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D121" s="19" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="E121" s="8"/>
       <c r="F121" s="11"/>
     </row>
-    <row r="122" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A122" s="7" t="s">
         <v>7</v>
       </c>
@@ -3698,29 +3710,29 @@
         <v>7</v>
       </c>
       <c r="C122" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D122" s="19" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="E122" s="10"/>
       <c r="F122" s="11"/>
     </row>
-    <row r="123" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A123" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B123" s="16" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="C123" s="25"/>
       <c r="D123" s="19" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="E123" s="8"/>
       <c r="F123" s="11"/>
     </row>
-    <row r="124" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A124" s="7" t="s">
         <v>7</v>
       </c>
@@ -3728,15 +3740,15 @@
         <v>7</v>
       </c>
       <c r="C124" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D124" s="19" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="E124" s="8"/>
       <c r="F124" s="11"/>
     </row>
-    <row r="125" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A125" s="7" t="s">
         <v>7</v>
       </c>
@@ -3744,15 +3756,15 @@
         <v>7</v>
       </c>
       <c r="C125" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D125" s="19" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="E125" s="8"/>
       <c r="F125" s="11"/>
     </row>
-    <row r="126" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A126" s="7" t="s">
         <v>7</v>
       </c>
@@ -3760,15 +3772,15 @@
         <v>7</v>
       </c>
       <c r="C126" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D126" s="19" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="E126" s="8"/>
       <c r="F126" s="11"/>
     </row>
-    <row r="127" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A127" s="7" t="s">
         <v>7</v>
       </c>
@@ -3776,15 +3788,15 @@
         <v>7</v>
       </c>
       <c r="C127" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D127" s="19" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="E127" s="8"/>
       <c r="F127" s="11"/>
     </row>
-    <row r="128" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A128" s="7" t="s">
         <v>7</v>
       </c>
@@ -3792,15 +3804,15 @@
         <v>7</v>
       </c>
       <c r="C128" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D128" s="19" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="E128" s="8"/>
       <c r="F128" s="11"/>
     </row>
-    <row r="129" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A129" s="7" t="s">
         <v>7</v>
       </c>
@@ -3808,41 +3820,41 @@
         <v>7</v>
       </c>
       <c r="C129" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D129" s="19" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="E129" s="8"/>
       <c r="F129" s="11"/>
     </row>
-    <row r="130" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A130" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B130" s="25"/>
       <c r="C130" s="25"/>
       <c r="D130" s="19" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="E130" s="8"/>
       <c r="F130" s="11"/>
     </row>
-    <row r="131" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A131" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B131" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C131" s="25"/>
       <c r="D131" s="19" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="E131" s="8"/>
       <c r="F131" s="11"/>
     </row>
-    <row r="132" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A132" s="7" t="s">
         <v>7</v>
       </c>
@@ -3850,15 +3862,15 @@
         <v>7</v>
       </c>
       <c r="C132" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D132" s="19" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="E132" s="8"/>
       <c r="F132" s="11"/>
     </row>
-    <row r="133" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A133" s="7" t="s">
         <v>7</v>
       </c>
@@ -3866,29 +3878,29 @@
         <v>7</v>
       </c>
       <c r="C133" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D133" s="19" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="E133" s="8"/>
       <c r="F133" s="11"/>
     </row>
-    <row r="134" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A134" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B134" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C134" s="25"/>
       <c r="D134" s="19" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="E134" s="8"/>
       <c r="F134" s="11"/>
     </row>
-    <row r="135" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A135" s="7" t="s">
         <v>7</v>
       </c>
@@ -3896,15 +3908,15 @@
         <v>7</v>
       </c>
       <c r="C135" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D135" s="19" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="E135" s="8"/>
       <c r="F135" s="11"/>
     </row>
-    <row r="136" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A136" s="7" t="s">
         <v>7</v>
       </c>
@@ -3912,41 +3924,41 @@
         <v>7</v>
       </c>
       <c r="C136" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D136" s="19" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="E136" s="8"/>
       <c r="F136" s="11"/>
     </row>
-    <row r="137" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A137" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B137" s="25"/>
       <c r="C137" s="25"/>
       <c r="D137" s="19" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="E137" s="8"/>
       <c r="F137" s="11"/>
     </row>
-    <row r="138" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A138" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B138" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C138" s="25"/>
       <c r="D138" s="19" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="E138" s="8"/>
       <c r="F138" s="11"/>
     </row>
-    <row r="139" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A139" s="7" t="s">
         <v>7</v>
       </c>
@@ -3954,15 +3966,15 @@
         <v>7</v>
       </c>
       <c r="C139" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D139" s="19" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="E139" s="8"/>
       <c r="F139" s="11"/>
     </row>
-    <row r="140" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A140" s="7" t="s">
         <v>7</v>
       </c>
@@ -3970,15 +3982,15 @@
         <v>7</v>
       </c>
       <c r="C140" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D140" s="19" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
       <c r="E140" s="8"/>
       <c r="F140" s="11"/>
     </row>
-    <row r="141" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A141" s="7" t="s">
         <v>7</v>
       </c>
@@ -3986,15 +3998,15 @@
         <v>7</v>
       </c>
       <c r="C141" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D141" s="19" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="E141" s="8"/>
       <c r="F141" s="11"/>
     </row>
-    <row r="142" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A142" s="7" t="s">
         <v>7</v>
       </c>
@@ -4002,29 +4014,29 @@
         <v>7</v>
       </c>
       <c r="C142" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D142" s="19" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="E142" s="8"/>
       <c r="F142" s="11"/>
     </row>
-    <row r="143" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A143" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B143" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C143" s="25"/>
       <c r="D143" s="19" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="E143" s="8"/>
       <c r="F143" s="11"/>
     </row>
-    <row r="144" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A144" s="7" t="s">
         <v>7</v>
       </c>
@@ -4032,15 +4044,15 @@
         <v>7</v>
       </c>
       <c r="C144" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D144" s="19" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="E144" s="8"/>
       <c r="F144" s="11"/>
     </row>
-    <row r="145" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A145" s="7" t="s">
         <v>7</v>
       </c>
@@ -4048,15 +4060,15 @@
         <v>7</v>
       </c>
       <c r="C145" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D145" s="19" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="E145" s="8"/>
       <c r="F145" s="11"/>
     </row>
-    <row r="146" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A146" s="7" t="s">
         <v>7</v>
       </c>
@@ -4064,15 +4076,15 @@
         <v>7</v>
       </c>
       <c r="C146" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D146" s="19" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="E146" s="8"/>
       <c r="F146" s="11"/>
     </row>
-    <row r="147" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A147" s="7" t="s">
         <v>7</v>
       </c>
@@ -4080,15 +4092,15 @@
         <v>7</v>
       </c>
       <c r="C147" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D147" s="19" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="E147" s="8"/>
       <c r="F147" s="11"/>
     </row>
-    <row r="148" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A148" s="7" t="s">
         <v>7</v>
       </c>
@@ -4096,29 +4108,29 @@
         <v>7</v>
       </c>
       <c r="C148" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D148" s="19" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="E148" s="8"/>
       <c r="F148" s="11"/>
     </row>
-    <row r="149" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A149" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B149" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C149" s="25"/>
       <c r="D149" s="19" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="E149" s="8"/>
       <c r="F149" s="11"/>
     </row>
-    <row r="150" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A150" s="7" t="s">
         <v>7</v>
       </c>
@@ -4126,15 +4138,15 @@
         <v>7</v>
       </c>
       <c r="C150" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D150" s="19" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E150" s="8"/>
       <c r="F150" s="11"/>
     </row>
-    <row r="151" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A151" s="7" t="s">
         <v>7</v>
       </c>
@@ -4142,15 +4154,15 @@
         <v>7</v>
       </c>
       <c r="C151" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D151" s="19" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="E151" s="8"/>
       <c r="F151" s="11"/>
     </row>
-    <row r="152" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A152" s="7" t="s">
         <v>7</v>
       </c>
@@ -4158,15 +4170,15 @@
         <v>7</v>
       </c>
       <c r="C152" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D152" s="19" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
       <c r="E152" s="10"/>
       <c r="F152" s="11"/>
     </row>
-    <row r="153" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A153" s="7" t="s">
         <v>7</v>
       </c>
@@ -4174,15 +4186,15 @@
         <v>7</v>
       </c>
       <c r="C153" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D153" s="19" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="E153" s="10"/>
       <c r="F153" s="11"/>
     </row>
-    <row r="154" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A154" s="7" t="s">
         <v>7</v>
       </c>
@@ -4190,15 +4202,15 @@
         <v>7</v>
       </c>
       <c r="C154" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D154" s="19" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="E154" s="8"/>
       <c r="F154" s="11"/>
     </row>
-    <row r="155" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A155" s="7" t="s">
         <v>7</v>
       </c>
@@ -4206,31 +4218,31 @@
         <v>7</v>
       </c>
       <c r="C155" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D155" s="19" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="E155" s="8"/>
       <c r="F155" s="11"/>
     </row>
-    <row r="156" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A156" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B156" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C156" s="25"/>
       <c r="D156" s="19" t="s">
-        <v>379</v>
+        <v>405</v>
       </c>
       <c r="E156" s="8"/>
       <c r="F156" s="28" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A157" s="7" t="s">
         <v>7</v>
       </c>
@@ -4238,17 +4250,17 @@
         <v>7</v>
       </c>
       <c r="C157" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D157" s="19" t="s">
-        <v>340</v>
+        <v>406</v>
       </c>
       <c r="E157" s="8"/>
       <c r="F157" s="28" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A158" s="7" t="s">
         <v>7</v>
       </c>
@@ -4256,17 +4268,17 @@
         <v>7</v>
       </c>
       <c r="C158" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D158" s="19" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="E158" s="8"/>
       <c r="F158" s="28" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A159" s="7" t="s">
         <v>7</v>
       </c>
@@ -4274,43 +4286,43 @@
         <v>7</v>
       </c>
       <c r="C159" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D159" s="19" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="E159" s="8"/>
       <c r="F159" s="28" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A160" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B160" s="25"/>
       <c r="C160" s="25"/>
       <c r="D160" s="19" t="s">
-        <v>394</v>
+        <v>409</v>
       </c>
       <c r="E160" s="8"/>
       <c r="F160" s="11"/>
     </row>
-    <row r="161" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A161" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B161" s="7" t="s">
-        <v>171</v>
+        <v>414</v>
       </c>
       <c r="C161" s="25"/>
       <c r="D161" s="19" t="s">
-        <v>330</v>
+        <v>415</v>
       </c>
       <c r="E161" s="8"/>
       <c r="F161" s="11"/>
     </row>
-    <row r="162" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A162" s="7" t="s">
         <v>7</v>
       </c>
@@ -4318,15 +4330,15 @@
         <v>7</v>
       </c>
       <c r="C162" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D162" s="19" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="E162" s="8"/>
       <c r="F162" s="11"/>
     </row>
-    <row r="163" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A163" s="7" t="s">
         <v>7</v>
       </c>
@@ -4334,15 +4346,15 @@
         <v>7</v>
       </c>
       <c r="C163" s="7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D163" s="19" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="E163" s="8"/>
       <c r="F163" s="11"/>
     </row>
-    <row r="164" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A164" s="7" t="s">
         <v>7</v>
       </c>
@@ -4350,15 +4362,15 @@
         <v>7</v>
       </c>
       <c r="C164" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D164" s="19" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="E164" s="8"/>
       <c r="F164" s="11"/>
     </row>
-    <row r="165" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A165" s="7" t="s">
         <v>7</v>
       </c>
@@ -4366,15 +4378,15 @@
         <v>7</v>
       </c>
       <c r="C165" s="7" t="s">
-        <v>175</v>
+        <v>412</v>
       </c>
       <c r="D165" s="19" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="E165" s="8"/>
       <c r="F165" s="11"/>
     </row>
-    <row r="166" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A166" s="7" t="s">
         <v>7</v>
       </c>
@@ -4382,29 +4394,29 @@
         <v>7</v>
       </c>
       <c r="C166" s="7" t="s">
-        <v>176</v>
+        <v>413</v>
       </c>
       <c r="D166" s="19" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="E166" s="8"/>
       <c r="F166" s="11"/>
     </row>
-    <row r="167" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A167" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B167" s="7" t="s">
-        <v>177</v>
+        <v>416</v>
       </c>
       <c r="C167" s="25"/>
       <c r="D167" s="19" t="s">
-        <v>336</v>
+        <v>419</v>
       </c>
       <c r="E167" s="8"/>
       <c r="F167" s="11"/>
     </row>
-    <row r="168" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A168" s="7" t="s">
         <v>7</v>
       </c>
@@ -4412,45 +4424,45 @@
         <v>7</v>
       </c>
       <c r="C168" s="7" t="s">
-        <v>178</v>
+        <v>417</v>
       </c>
       <c r="D168" s="19" t="s">
-        <v>337</v>
+        <v>418</v>
       </c>
       <c r="E168" s="8"/>
       <c r="F168" s="11"/>
     </row>
-    <row r="169" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A169" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B169" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C169" s="7" t="s">
-        <v>179</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="C169" s="25"/>
       <c r="D169" s="19" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="E169" s="8"/>
       <c r="F169" s="11"/>
     </row>
-    <row r="170" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A170" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B170" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="C170" s="25"/>
+        <v>7</v>
+      </c>
+      <c r="C170" s="7" t="s">
+        <v>174</v>
+      </c>
       <c r="D170" s="19" t="s">
-        <v>380</v>
+        <v>330</v>
       </c>
       <c r="E170" s="8"/>
-      <c r="F170" s="9"/>
-    </row>
-    <row r="171" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="F170" s="11"/>
+    </row>
+    <row r="171" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A171" s="7" t="s">
         <v>7</v>
       </c>
@@ -4458,33 +4470,29 @@
         <v>7</v>
       </c>
       <c r="C171" s="7" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="D171" s="19" t="s">
-        <v>339</v>
-      </c>
-      <c r="E171" s="10"/>
-      <c r="F171" s="12" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+      <c r="E171" s="8"/>
+      <c r="F171" s="11"/>
+    </row>
+    <row r="172" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A172" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B172" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C172" s="7" t="s">
-        <v>182</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="C172" s="25"/>
       <c r="D172" s="19" t="s">
-        <v>341</v>
+        <v>371</v>
       </c>
       <c r="E172" s="8"/>
-      <c r="F172" s="6"/>
-    </row>
-    <row r="173" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F172" s="9"/>
+    </row>
+    <row r="173" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A173" s="7" t="s">
         <v>7</v>
       </c>
@@ -4492,87 +4500,91 @@
         <v>7</v>
       </c>
       <c r="C173" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="D173" s="29" t="s">
-        <v>342</v>
-      </c>
-      <c r="E173" s="8"/>
-      <c r="F173" s="11"/>
-    </row>
-    <row r="174" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+      <c r="D173" s="19" t="s">
+        <v>332</v>
+      </c>
+      <c r="E173" s="10"/>
+      <c r="F173" s="12" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A174" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="B174" s="25"/>
-      <c r="C174" s="25"/>
+        <v>7</v>
+      </c>
+      <c r="B174" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C174" s="7" t="s">
+        <v>178</v>
+      </c>
       <c r="D174" s="19" t="s">
-        <v>365</v>
+        <v>333</v>
       </c>
       <c r="E174" s="8"/>
-      <c r="F174" s="11"/>
-    </row>
-    <row r="175" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F174" s="6"/>
+    </row>
+    <row r="175" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A175" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B175" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="C175" s="25"/>
-      <c r="D175" s="19" t="s">
-        <v>343</v>
+        <v>7</v>
+      </c>
+      <c r="C175" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D175" s="29" t="s">
+        <v>334</v>
       </c>
       <c r="E175" s="8"/>
       <c r="F175" s="11"/>
     </row>
-    <row r="176" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A176" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B176" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C176" s="7" t="s">
-        <v>186</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="B176" s="25"/>
+      <c r="C176" s="25"/>
       <c r="D176" s="19" t="s">
-        <v>344</v>
+        <v>357</v>
       </c>
       <c r="E176" s="8"/>
       <c r="F176" s="11"/>
     </row>
-    <row r="177" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A177" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B177" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C177" s="7" t="s">
-        <v>187</v>
-      </c>
+        <v>181</v>
+      </c>
+      <c r="C177" s="25"/>
       <c r="D177" s="19" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="E177" s="8"/>
       <c r="F177" s="11"/>
     </row>
-    <row r="178" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A178" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B178" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="C178" s="25"/>
+        <v>7</v>
+      </c>
+      <c r="C178" s="7" t="s">
+        <v>182</v>
+      </c>
       <c r="D178" s="19" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="E178" s="8"/>
       <c r="F178" s="11"/>
     </row>
-    <row r="179" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A179" s="7" t="s">
         <v>7</v>
       </c>
@@ -4580,101 +4592,101 @@
         <v>7</v>
       </c>
       <c r="C179" s="7" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="D179" s="19" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="E179" s="8"/>
       <c r="F179" s="11"/>
     </row>
-    <row r="180" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A180" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="B180" s="25"/>
+        <v>7</v>
+      </c>
+      <c r="B180" s="7" t="s">
+        <v>184</v>
+      </c>
       <c r="C180" s="25"/>
       <c r="D180" s="19" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="E180" s="8"/>
       <c r="F180" s="11"/>
     </row>
-    <row r="181" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A181" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B181" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="C181" s="25"/>
+        <v>7</v>
+      </c>
+      <c r="C181" s="7" t="s">
+        <v>185</v>
+      </c>
       <c r="D181" s="19" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="E181" s="8"/>
       <c r="F181" s="11"/>
     </row>
-    <row r="182" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A182" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B182" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C182" s="16" t="s">
-        <v>350</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="B182" s="25"/>
+      <c r="C182" s="25"/>
       <c r="D182" s="19" t="s">
-        <v>351</v>
-      </c>
-      <c r="E182" s="10"/>
+        <v>340</v>
+      </c>
+      <c r="E182" s="8"/>
       <c r="F182" s="11"/>
     </row>
-    <row r="183" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A183" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B183" s="7" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C183" s="25"/>
       <c r="D183" s="19" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
       <c r="E183" s="8"/>
       <c r="F183" s="11"/>
     </row>
-    <row r="184" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A184" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B184" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C184" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="D184" s="29" t="s">
-        <v>397</v>
-      </c>
-      <c r="E184" s="8"/>
+      <c r="C184" s="16" t="s">
+        <v>342</v>
+      </c>
+      <c r="D184" s="19" t="s">
+        <v>343</v>
+      </c>
+      <c r="E184" s="10"/>
       <c r="F184" s="11"/>
     </row>
-    <row r="185" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A185" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B185" s="7" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="C185" s="25"/>
       <c r="D185" s="19" t="s">
-        <v>398</v>
+        <v>344</v>
       </c>
       <c r="E185" s="8"/>
       <c r="F185" s="11"/>
     </row>
-    <row r="186" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A186" s="7" t="s">
         <v>7</v>
       </c>
@@ -4682,29 +4694,29 @@
         <v>7</v>
       </c>
       <c r="C186" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="D186" s="19" t="s">
-        <v>399</v>
+        <v>189</v>
+      </c>
+      <c r="D186" s="29" t="s">
+        <v>387</v>
       </c>
       <c r="E186" s="8"/>
       <c r="F186" s="11"/>
     </row>
-    <row r="187" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A187" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B187" s="7" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C187" s="25"/>
       <c r="D187" s="19" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
       <c r="E187" s="8"/>
       <c r="F187" s="11"/>
     </row>
-    <row r="188" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A188" s="7" t="s">
         <v>7</v>
       </c>
@@ -4712,103 +4724,103 @@
         <v>7</v>
       </c>
       <c r="C188" s="7" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="D188" s="19" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="E188" s="8"/>
       <c r="F188" s="11"/>
     </row>
-    <row r="189" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A189" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B189" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C189" s="7" t="s">
-        <v>198</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="C189" s="25"/>
       <c r="D189" s="19" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
       <c r="E189" s="8"/>
       <c r="F189" s="11"/>
     </row>
-    <row r="190" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A190" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="B190" s="25"/>
-      <c r="C190" s="25"/>
+        <v>7</v>
+      </c>
+      <c r="B190" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C190" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="D190" s="19" t="s">
-        <v>353</v>
+        <v>391</v>
       </c>
       <c r="E190" s="8"/>
       <c r="F190" s="11"/>
     </row>
-    <row r="191" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A191" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B191" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="C191" s="25"/>
+        <v>7</v>
+      </c>
+      <c r="C191" s="7" t="s">
+        <v>194</v>
+      </c>
       <c r="D191" s="19" t="s">
-        <v>354</v>
+        <v>392</v>
       </c>
       <c r="E191" s="8"/>
       <c r="F191" s="11"/>
     </row>
-    <row r="192" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A192" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B192" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C192" s="7" t="s">
-        <v>201</v>
-      </c>
+        <v>195</v>
+      </c>
+      <c r="B192" s="25"/>
+      <c r="C192" s="25"/>
       <c r="D192" s="19" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="E192" s="8"/>
       <c r="F192" s="11"/>
     </row>
-    <row r="193" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A193" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B193" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C193" s="7" t="s">
-        <v>202</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="C193" s="25"/>
       <c r="D193" s="19" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="E193" s="8"/>
       <c r="F193" s="11"/>
     </row>
-    <row r="194" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A194" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B194" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="C194" s="25"/>
-      <c r="D194" s="18" t="s">
-        <v>204</v>
+        <v>7</v>
+      </c>
+      <c r="C194" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="D194" s="19" t="s">
+        <v>347</v>
       </c>
       <c r="E194" s="8"/>
       <c r="F194" s="11"/>
     </row>
-    <row r="195" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A195" s="7" t="s">
         <v>7</v>
       </c>
@@ -4816,47 +4828,47 @@
         <v>7</v>
       </c>
       <c r="C195" s="7" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="D195" s="19" t="s">
-        <v>405</v>
+        <v>348</v>
       </c>
       <c r="E195" s="8"/>
-      <c r="F195" s="28" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="196" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F195" s="11"/>
+    </row>
+    <row r="196" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A196" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B196" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C196" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="D196" s="19" t="s">
-        <v>357</v>
+        <v>199</v>
+      </c>
+      <c r="C196" s="25"/>
+      <c r="D196" s="18" t="s">
+        <v>200</v>
       </c>
       <c r="E196" s="8"/>
       <c r="F196" s="11"/>
     </row>
-    <row r="197" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A197" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B197" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C197" s="25"/>
+        <v>7</v>
+      </c>
+      <c r="C197" s="7" t="s">
+        <v>410</v>
+      </c>
       <c r="D197" s="19" t="s">
-        <v>358</v>
+        <v>411</v>
       </c>
       <c r="E197" s="8"/>
-      <c r="F197" s="11"/>
-    </row>
-    <row r="198" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="F197" s="28" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A198" s="7" t="s">
         <v>7</v>
       </c>
@@ -4864,69 +4876,99 @@
         <v>7</v>
       </c>
       <c r="C198" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="D198" s="29" t="s">
-        <v>408</v>
+        <v>201</v>
+      </c>
+      <c r="D198" s="19" t="s">
+        <v>349</v>
       </c>
       <c r="E198" s="8"/>
       <c r="F198" s="11"/>
     </row>
-    <row r="199" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A199" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="B199" s="25"/>
+        <v>7</v>
+      </c>
+      <c r="B199" s="7" t="s">
+        <v>202</v>
+      </c>
       <c r="C199" s="25"/>
       <c r="D199" s="19" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="E199" s="8"/>
       <c r="F199" s="11"/>
     </row>
-    <row r="200" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A200" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B200" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="C200" s="25"/>
-      <c r="D200" s="19" t="s">
-        <v>360</v>
+        <v>7</v>
+      </c>
+      <c r="C200" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="D200" s="29" t="s">
+        <v>395</v>
       </c>
       <c r="E200" s="8"/>
       <c r="F200" s="11"/>
     </row>
-    <row r="201" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A201" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B201" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C201" s="7" t="s">
-        <v>211</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="B201" s="25"/>
+      <c r="C201" s="25"/>
       <c r="D201" s="19" t="s">
-        <v>212</v>
+        <v>351</v>
       </c>
       <c r="E201" s="8"/>
       <c r="F201" s="11"/>
     </row>
-    <row r="202" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A202" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B202" s="7" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="C202" s="25"/>
       <c r="D202" s="19" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="E202" s="8"/>
       <c r="F202" s="11"/>
+    </row>
+    <row r="203" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A203" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B203" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C203" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="D203" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="E203" s="8"/>
+      <c r="F203" s="11"/>
+    </row>
+    <row r="204" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A204" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B204" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C204" s="25"/>
+      <c r="D204" s="19" t="s">
+        <v>353</v>
+      </c>
+      <c r="E204" s="8"/>
+      <c r="F204" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
A few more updates under Spying
</commit_message>
<xml_diff>
--- a/mind_maps/malware_capabilities_descriptions.xlsx
+++ b/mind_maps/malware_capabilities_descriptions.xlsx
@@ -550,12 +550,6 @@
     <t xml:space="preserve"> Capture System Screenshot</t>
   </si>
   <si>
-    <t xml:space="preserve"> Capture System Memory Dump</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Capture File System Dump</t>
-  </si>
-  <si>
     <t>Destruction</t>
   </si>
   <si>
@@ -1012,15 +1006,6 @@
     <t>The 'capture gps data' value indicates that the malware instance is able to capture system GPS data.</t>
   </si>
   <si>
-    <t>The 'capture system screenshot' value indicates that the malware instance is able to capture images of what is currently being displayed on a system's screen.</t>
-  </si>
-  <si>
-    <t>The 'capture system memory dump' value indicates that the malware instance is able to capture data from a system's RAM.</t>
-  </si>
-  <si>
-    <t>The 'capture file system dump' value indicates that the malware instance is able to capture data from a system's file system.</t>
-  </si>
-  <si>
     <t>The 'destroy physical entity' value indicates that the malware instance is able to destroy a physical entity.</t>
   </si>
   <si>
@@ -1274,6 +1259,21 @@
   </si>
   <si>
     <t>The 'capture system output peripheral data' value indicates that the malware instance is able to capture data sent to a system's output peripheral devices.</t>
+  </si>
+  <si>
+    <t>The 'capture system screenshot' value indicates that the malware instance is able to capture images of what is currently being displayed on a system's screen, either locally or remotely via a remote desktop protocol.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Capture File System</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Capture System Memory</t>
+  </si>
+  <si>
+    <t>The 'capture system memory' value indicates that the malware instance is able to capture data from a system's RAM.</t>
+  </si>
+  <si>
+    <t>The 'capture file system' value indicates that the malware instance is able to capture data from a system's file system.</t>
   </si>
 </sst>
 </file>
@@ -1865,8 +1865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV204"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B160" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D170" sqref="D170"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B166" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D176" sqref="D176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.61328125" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1907,7 +1907,7 @@
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
       <c r="D2" s="22" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="6"/>
@@ -1921,7 +1921,7 @@
       </c>
       <c r="C3" s="25"/>
       <c r="D3" s="18" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="6"/>
@@ -1937,7 +1937,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="6"/>
@@ -1953,7 +1953,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="6"/>
@@ -1969,7 +1969,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="6"/>
@@ -1983,7 +1983,7 @@
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="18" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="11"/>
@@ -1999,7 +1999,7 @@
         <v>13</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="11"/>
@@ -2015,7 +2015,7 @@
         <v>14</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="11"/>
@@ -2027,7 +2027,7 @@
       <c r="B10" s="25"/>
       <c r="C10" s="25"/>
       <c r="D10" s="18" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="11"/>
@@ -2041,7 +2041,7 @@
       </c>
       <c r="C11" s="25"/>
       <c r="D11" s="18" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="11"/>
@@ -2057,7 +2057,7 @@
         <v>17</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
@@ -2073,7 +2073,7 @@
         <v>18</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="11"/>
@@ -2087,7 +2087,7 @@
       </c>
       <c r="C14" s="25"/>
       <c r="D14" s="18" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="11"/>
@@ -2103,7 +2103,7 @@
         <v>20</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="11"/>
@@ -2115,7 +2115,7 @@
         <v>21</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="11"/>
@@ -2131,7 +2131,7 @@
         <v>22</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="11"/>
@@ -2143,7 +2143,7 @@
       <c r="B18" s="25"/>
       <c r="C18" s="25"/>
       <c r="D18" s="18" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="11"/>
@@ -2157,7 +2157,7 @@
       </c>
       <c r="C19" s="25"/>
       <c r="D19" s="18" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="11"/>
@@ -2173,7 +2173,7 @@
         <v>25</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="11"/>
@@ -2189,7 +2189,7 @@
         <v>26</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="13"/>
@@ -2203,7 +2203,7 @@
       </c>
       <c r="C22" s="25"/>
       <c r="D22" s="18" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="13"/>
@@ -2219,7 +2219,7 @@
         <v>28</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="9"/>
@@ -2235,11 +2235,11 @@
         <v>29</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E24" s="10"/>
       <c r="F24" s="12" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2253,7 +2253,7 @@
         <v>30</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="6"/>
@@ -2269,7 +2269,7 @@
         <v>31</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E26" s="8"/>
       <c r="F26" s="13"/>
@@ -2285,7 +2285,7 @@
         <v>32</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="E27" s="8"/>
       <c r="F27" s="11"/>
@@ -2299,7 +2299,7 @@
       </c>
       <c r="C28" s="25"/>
       <c r="D28" s="18" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E28" s="8"/>
       <c r="F28" s="11"/>
@@ -2315,7 +2315,7 @@
         <v>34</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E29" s="8"/>
       <c r="F29" s="11"/>
@@ -2347,7 +2347,7 @@
         <v>37</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E31" s="8"/>
       <c r="F31" s="11"/>
@@ -2359,7 +2359,7 @@
       <c r="B32" s="25"/>
       <c r="C32" s="25"/>
       <c r="D32" s="18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E32" s="8"/>
       <c r="F32" s="14"/>
@@ -2373,7 +2373,7 @@
       </c>
       <c r="C33" s="25"/>
       <c r="D33" s="18" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E33" s="8"/>
       <c r="F33" s="11"/>
@@ -2389,7 +2389,7 @@
         <v>40</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E34" s="8"/>
       <c r="F34" s="11"/>
@@ -2405,7 +2405,7 @@
         <v>41</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E35" s="8"/>
       <c r="F35" s="11"/>
@@ -2421,7 +2421,7 @@
         <v>42</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E36" s="8"/>
       <c r="F36" s="11"/>
@@ -2435,7 +2435,7 @@
       </c>
       <c r="C37" s="25"/>
       <c r="D37" s="18" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E37" s="8"/>
       <c r="F37" s="11"/>
@@ -2451,7 +2451,7 @@
         <v>44</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E38" s="8"/>
       <c r="F38" s="11"/>
@@ -2467,7 +2467,7 @@
         <v>45</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E39" s="8"/>
       <c r="F39" s="11"/>
@@ -2479,7 +2479,7 @@
         <v>46</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E40" s="8"/>
       <c r="F40" s="11"/>
@@ -2491,7 +2491,7 @@
       <c r="B41" s="25"/>
       <c r="C41" s="25"/>
       <c r="D41" s="27" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E41" s="8"/>
       <c r="F41" s="13"/>
@@ -2505,7 +2505,7 @@
       </c>
       <c r="C42" s="25"/>
       <c r="D42" s="18" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E42" s="8"/>
       <c r="F42" s="11"/>
@@ -2521,7 +2521,7 @@
         <v>49</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E43" s="8"/>
       <c r="F43" s="11"/>
@@ -2537,7 +2537,7 @@
         <v>50</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E44" s="8"/>
       <c r="F44" s="11"/>
@@ -2553,7 +2553,7 @@
         <v>51</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E45" s="8"/>
       <c r="F45" s="11"/>
@@ -2569,7 +2569,7 @@
         <v>52</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E46" s="8"/>
       <c r="F46" s="11"/>
@@ -2585,7 +2585,7 @@
         <v>53</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="E47" s="8"/>
       <c r="F47" s="11"/>
@@ -2599,7 +2599,7 @@
       </c>
       <c r="C48" s="25"/>
       <c r="D48" s="18" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E48" s="8"/>
       <c r="F48" s="11"/>
@@ -2615,7 +2615,7 @@
         <v>55</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E49" s="8"/>
       <c r="F49" s="11"/>
@@ -2631,7 +2631,7 @@
         <v>56</v>
       </c>
       <c r="D50" s="18" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E50" s="8"/>
       <c r="F50" s="11"/>
@@ -2647,7 +2647,7 @@
         <v>57</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E51" s="8"/>
       <c r="F51" s="11"/>
@@ -2663,7 +2663,7 @@
         <v>58</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E52" s="8"/>
       <c r="F52" s="11"/>
@@ -2679,7 +2679,7 @@
         <v>59</v>
       </c>
       <c r="D53" s="18" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E53" s="8"/>
       <c r="F53" s="11"/>
@@ -2695,7 +2695,7 @@
         <v>60</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="E54" s="10"/>
       <c r="F54" s="11"/>
@@ -2711,7 +2711,7 @@
         <v>61</v>
       </c>
       <c r="D55" s="27" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="E55" s="10"/>
       <c r="F55" s="11"/>
@@ -2727,7 +2727,7 @@
         <v>62</v>
       </c>
       <c r="D56" s="27" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="E56" s="10"/>
       <c r="F56" s="11"/>
@@ -2741,7 +2741,7 @@
       </c>
       <c r="C57" s="25"/>
       <c r="D57" s="18" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E57" s="8"/>
       <c r="F57" s="11"/>
@@ -2757,7 +2757,7 @@
         <v>64</v>
       </c>
       <c r="D58" s="18" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E58" s="10"/>
       <c r="F58" s="11"/>
@@ -2773,7 +2773,7 @@
         <v>65</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E59" s="10"/>
       <c r="F59" s="11"/>
@@ -2789,7 +2789,7 @@
         <v>66</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E60" s="8"/>
       <c r="F60" s="11"/>
@@ -2803,7 +2803,7 @@
       </c>
       <c r="C61" s="25"/>
       <c r="D61" s="18" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="E61" s="8"/>
       <c r="F61" s="11"/>
@@ -2819,7 +2819,7 @@
         <v>68</v>
       </c>
       <c r="D62" s="19" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="E62" s="8"/>
       <c r="F62" s="11"/>
@@ -2833,7 +2833,7 @@
       </c>
       <c r="C63" s="25"/>
       <c r="D63" s="18" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="E63" s="8"/>
       <c r="F63" s="11"/>
@@ -2849,7 +2849,7 @@
         <v>70</v>
       </c>
       <c r="D64" s="18" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E64" s="8"/>
       <c r="F64" s="11"/>
@@ -2879,7 +2879,7 @@
       </c>
       <c r="C66" s="25"/>
       <c r="D66" s="18" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E66" s="8"/>
       <c r="F66" s="11"/>
@@ -2895,7 +2895,7 @@
         <v>74</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E67" s="10"/>
       <c r="F67" s="11"/>
@@ -2907,7 +2907,7 @@
       <c r="B68" s="25"/>
       <c r="C68" s="25"/>
       <c r="D68" s="18" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E68" s="8"/>
       <c r="F68" s="11"/>
@@ -2921,7 +2921,7 @@
       </c>
       <c r="C69" s="25"/>
       <c r="D69" s="18" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="E69" s="8"/>
       <c r="F69" s="11"/>
@@ -2937,7 +2937,7 @@
         <v>77</v>
       </c>
       <c r="D70" s="18" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E70" s="8"/>
       <c r="F70" s="11"/>
@@ -2953,7 +2953,7 @@
         <v>78</v>
       </c>
       <c r="D71" s="18" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E71" s="8"/>
       <c r="F71" s="11"/>
@@ -2969,7 +2969,7 @@
         <v>79</v>
       </c>
       <c r="D72" s="18" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E72" s="8"/>
       <c r="F72" s="11"/>
@@ -2999,7 +2999,7 @@
         <v>82</v>
       </c>
       <c r="D74" s="18" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="E74" s="8"/>
       <c r="F74" s="11"/>
@@ -3013,7 +3013,7 @@
       </c>
       <c r="C75" s="25"/>
       <c r="D75" s="18" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E75" s="8"/>
       <c r="F75" s="11"/>
@@ -3041,7 +3041,7 @@
       <c r="B77" s="25"/>
       <c r="C77" s="25"/>
       <c r="D77" s="18" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E77" s="8"/>
       <c r="F77" s="11"/>
@@ -3055,7 +3055,7 @@
       </c>
       <c r="C78" s="25"/>
       <c r="D78" s="18" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="E78" s="8"/>
       <c r="F78" s="11"/>
@@ -3071,7 +3071,7 @@
         <v>88</v>
       </c>
       <c r="D79" s="18" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E79" s="8"/>
       <c r="F79" s="11"/>
@@ -3085,7 +3085,7 @@
       </c>
       <c r="C80" s="25"/>
       <c r="D80" s="18" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="E80" s="8"/>
       <c r="F80" s="11"/>
@@ -3133,7 +3133,7 @@
         <v>94</v>
       </c>
       <c r="D83" s="18" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="E83" s="8"/>
       <c r="F83" s="11"/>
@@ -3146,14 +3146,14 @@
         <v>7</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="D84" s="18" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="E84" s="8"/>
       <c r="F84" s="28" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3161,7 +3161,7 @@
         <v>7</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="C85" s="25"/>
       <c r="D85" s="18" t="s">
@@ -3183,7 +3183,7 @@
         <v>97</v>
       </c>
       <c r="D86" s="18" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="E86" s="8"/>
       <c r="F86" s="11"/>
@@ -3215,7 +3215,7 @@
         <v>100</v>
       </c>
       <c r="D88" s="20" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E88" s="8"/>
       <c r="F88" s="11"/>
@@ -3229,7 +3229,7 @@
       </c>
       <c r="C89" s="25"/>
       <c r="D89" s="20" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E89" s="8"/>
       <c r="F89" s="11"/>
@@ -3245,7 +3245,7 @@
         <v>102</v>
       </c>
       <c r="D90" s="20" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E90" s="8"/>
       <c r="F90" s="11"/>
@@ -3261,7 +3261,7 @@
         <v>103</v>
       </c>
       <c r="D91" s="20" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E91" s="8"/>
       <c r="F91" s="11"/>
@@ -3275,7 +3275,7 @@
       </c>
       <c r="C92" s="25"/>
       <c r="D92" s="20" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E92" s="8"/>
       <c r="F92" s="11"/>
@@ -3291,7 +3291,7 @@
         <v>105</v>
       </c>
       <c r="D93" s="20" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E93" s="8"/>
       <c r="F93" s="11"/>
@@ -3307,7 +3307,7 @@
         <v>106</v>
       </c>
       <c r="D94" s="20" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E94" s="8"/>
       <c r="F94" s="11"/>
@@ -3323,7 +3323,7 @@
         <v>107</v>
       </c>
       <c r="D95" s="20" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="E95" s="8"/>
       <c r="F95" s="11"/>
@@ -3339,7 +3339,7 @@
         <v>108</v>
       </c>
       <c r="D96" s="20" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E96" s="8"/>
       <c r="F96" s="11"/>
@@ -3355,7 +3355,7 @@
         <v>109</v>
       </c>
       <c r="D97" s="20" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E97" s="8"/>
       <c r="F97" s="11"/>
@@ -3367,7 +3367,7 @@
       <c r="B98" s="25"/>
       <c r="C98" s="25"/>
       <c r="D98" s="19" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="E98" s="8"/>
       <c r="F98" s="11"/>
@@ -3381,7 +3381,7 @@
       </c>
       <c r="C99" s="25"/>
       <c r="D99" s="19" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E99" s="8"/>
       <c r="F99" s="11"/>
@@ -3397,7 +3397,7 @@
         <v>112</v>
       </c>
       <c r="D100" s="18" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="E100" s="8"/>
       <c r="F100" s="11"/>
@@ -3413,7 +3413,7 @@
         <v>113</v>
       </c>
       <c r="D101" s="19" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E101" s="10"/>
       <c r="F101" s="11"/>
@@ -3427,7 +3427,7 @@
       </c>
       <c r="C102" s="25"/>
       <c r="D102" s="19" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="E102" s="8"/>
       <c r="F102" s="11"/>
@@ -3443,7 +3443,7 @@
         <v>115</v>
       </c>
       <c r="D103" s="19" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="E103" s="8"/>
       <c r="F103" s="11"/>
@@ -3451,11 +3451,11 @@
     <row r="104" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A104" s="25"/>
       <c r="B104" s="16" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C104" s="25"/>
       <c r="D104" s="19" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="E104" s="8"/>
       <c r="F104" s="11"/>
@@ -3467,7 +3467,7 @@
         <v>116</v>
       </c>
       <c r="D105" s="19" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E105" s="8"/>
       <c r="F105" s="11"/>
@@ -3479,7 +3479,7 @@
       <c r="B106" s="25"/>
       <c r="C106" s="25"/>
       <c r="D106" s="19" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E106" s="8"/>
       <c r="F106" s="11"/>
@@ -3493,7 +3493,7 @@
       </c>
       <c r="C107" s="25"/>
       <c r="D107" s="19" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E107" s="8"/>
       <c r="F107" s="11"/>
@@ -3507,7 +3507,7 @@
       </c>
       <c r="C108" s="25"/>
       <c r="D108" s="19" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E108" s="8"/>
       <c r="F108" s="11"/>
@@ -3523,7 +3523,7 @@
         <v>120</v>
       </c>
       <c r="D109" s="19" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E109" s="8"/>
       <c r="F109" s="11"/>
@@ -3537,7 +3537,7 @@
       </c>
       <c r="C110" s="25"/>
       <c r="D110" s="19" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E110" s="8"/>
       <c r="F110" s="11"/>
@@ -3553,7 +3553,7 @@
         <v>116</v>
       </c>
       <c r="D111" s="19" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E111" s="8"/>
       <c r="F111" s="11"/>
@@ -3565,7 +3565,7 @@
       <c r="B112" s="25"/>
       <c r="C112" s="25"/>
       <c r="D112" s="19" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E112" s="8"/>
       <c r="F112" s="11"/>
@@ -3579,7 +3579,7 @@
       </c>
       <c r="C113" s="25"/>
       <c r="D113" s="19" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E113" s="10"/>
       <c r="F113" s="11"/>
@@ -3595,7 +3595,7 @@
         <v>124</v>
       </c>
       <c r="D114" s="19" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E114" s="8"/>
       <c r="F114" s="11"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="C115" s="25"/>
       <c r="D115" s="19" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E115" s="8"/>
       <c r="F115" s="11"/>
@@ -3621,7 +3621,7 @@
       <c r="B116" s="25"/>
       <c r="C116" s="25"/>
       <c r="D116" s="19" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E116" s="8"/>
       <c r="F116" s="11"/>
@@ -3635,7 +3635,7 @@
       </c>
       <c r="C117" s="25"/>
       <c r="D117" s="19" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E117" s="8"/>
       <c r="F117" s="11"/>
@@ -3651,7 +3651,7 @@
         <v>128</v>
       </c>
       <c r="D118" s="19" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E118" s="8"/>
       <c r="F118" s="11"/>
@@ -3667,7 +3667,7 @@
         <v>129</v>
       </c>
       <c r="D119" s="19" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E119" s="8"/>
       <c r="F119" s="11"/>
@@ -3681,7 +3681,7 @@
       </c>
       <c r="C120" s="25"/>
       <c r="D120" s="19" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E120" s="8"/>
       <c r="F120" s="11"/>
@@ -3697,7 +3697,7 @@
         <v>131</v>
       </c>
       <c r="D121" s="19" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E121" s="8"/>
       <c r="F121" s="11"/>
@@ -3713,7 +3713,7 @@
         <v>132</v>
       </c>
       <c r="D122" s="19" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E122" s="10"/>
       <c r="F122" s="11"/>
@@ -3723,11 +3723,11 @@
         <v>7</v>
       </c>
       <c r="B123" s="16" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C123" s="25"/>
       <c r="D123" s="19" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E123" s="8"/>
       <c r="F123" s="11"/>
@@ -3743,7 +3743,7 @@
         <v>133</v>
       </c>
       <c r="D124" s="19" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E124" s="8"/>
       <c r="F124" s="11"/>
@@ -3759,7 +3759,7 @@
         <v>134</v>
       </c>
       <c r="D125" s="19" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="E125" s="8"/>
       <c r="F125" s="11"/>
@@ -3775,7 +3775,7 @@
         <v>135</v>
       </c>
       <c r="D126" s="19" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E126" s="8"/>
       <c r="F126" s="11"/>
@@ -3791,7 +3791,7 @@
         <v>136</v>
       </c>
       <c r="D127" s="19" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E127" s="8"/>
       <c r="F127" s="11"/>
@@ -3807,7 +3807,7 @@
         <v>137</v>
       </c>
       <c r="D128" s="19" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E128" s="8"/>
       <c r="F128" s="11"/>
@@ -3823,7 +3823,7 @@
         <v>138</v>
       </c>
       <c r="D129" s="19" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E129" s="8"/>
       <c r="F129" s="11"/>
@@ -3835,7 +3835,7 @@
       <c r="B130" s="25"/>
       <c r="C130" s="25"/>
       <c r="D130" s="19" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E130" s="8"/>
       <c r="F130" s="11"/>
@@ -3849,7 +3849,7 @@
       </c>
       <c r="C131" s="25"/>
       <c r="D131" s="19" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E131" s="8"/>
       <c r="F131" s="11"/>
@@ -3865,7 +3865,7 @@
         <v>141</v>
       </c>
       <c r="D132" s="19" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E132" s="8"/>
       <c r="F132" s="11"/>
@@ -3881,7 +3881,7 @@
         <v>142</v>
       </c>
       <c r="D133" s="19" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E133" s="8"/>
       <c r="F133" s="11"/>
@@ -3895,7 +3895,7 @@
       </c>
       <c r="C134" s="25"/>
       <c r="D134" s="19" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E134" s="8"/>
       <c r="F134" s="11"/>
@@ -3911,7 +3911,7 @@
         <v>144</v>
       </c>
       <c r="D135" s="19" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E135" s="8"/>
       <c r="F135" s="11"/>
@@ -3927,7 +3927,7 @@
         <v>145</v>
       </c>
       <c r="D136" s="19" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E136" s="8"/>
       <c r="F136" s="11"/>
@@ -3939,7 +3939,7 @@
       <c r="B137" s="25"/>
       <c r="C137" s="25"/>
       <c r="D137" s="19" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E137" s="8"/>
       <c r="F137" s="11"/>
@@ -3953,7 +3953,7 @@
       </c>
       <c r="C138" s="25"/>
       <c r="D138" s="19" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E138" s="8"/>
       <c r="F138" s="11"/>
@@ -3969,7 +3969,7 @@
         <v>148</v>
       </c>
       <c r="D139" s="19" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E139" s="8"/>
       <c r="F139" s="11"/>
@@ -3985,7 +3985,7 @@
         <v>149</v>
       </c>
       <c r="D140" s="19" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="E140" s="8"/>
       <c r="F140" s="11"/>
@@ -4001,7 +4001,7 @@
         <v>150</v>
       </c>
       <c r="D141" s="19" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E141" s="8"/>
       <c r="F141" s="11"/>
@@ -4017,7 +4017,7 @@
         <v>151</v>
       </c>
       <c r="D142" s="19" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E142" s="8"/>
       <c r="F142" s="11"/>
@@ -4031,7 +4031,7 @@
       </c>
       <c r="C143" s="25"/>
       <c r="D143" s="19" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="E143" s="8"/>
       <c r="F143" s="11"/>
@@ -4047,7 +4047,7 @@
         <v>153</v>
       </c>
       <c r="D144" s="19" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E144" s="8"/>
       <c r="F144" s="11"/>
@@ -4063,7 +4063,7 @@
         <v>154</v>
       </c>
       <c r="D145" s="19" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E145" s="8"/>
       <c r="F145" s="11"/>
@@ -4079,7 +4079,7 @@
         <v>155</v>
       </c>
       <c r="D146" s="19" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E146" s="8"/>
       <c r="F146" s="11"/>
@@ -4095,7 +4095,7 @@
         <v>156</v>
       </c>
       <c r="D147" s="19" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E147" s="8"/>
       <c r="F147" s="11"/>
@@ -4111,7 +4111,7 @@
         <v>157</v>
       </c>
       <c r="D148" s="19" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="E148" s="8"/>
       <c r="F148" s="11"/>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="C149" s="25"/>
       <c r="D149" s="19" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="E149" s="8"/>
       <c r="F149" s="11"/>
@@ -4141,7 +4141,7 @@
         <v>159</v>
       </c>
       <c r="D150" s="19" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E150" s="8"/>
       <c r="F150" s="11"/>
@@ -4157,7 +4157,7 @@
         <v>160</v>
       </c>
       <c r="D151" s="19" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E151" s="8"/>
       <c r="F151" s="11"/>
@@ -4173,7 +4173,7 @@
         <v>161</v>
       </c>
       <c r="D152" s="19" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="E152" s="10"/>
       <c r="F152" s="11"/>
@@ -4189,7 +4189,7 @@
         <v>162</v>
       </c>
       <c r="D153" s="19" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E153" s="10"/>
       <c r="F153" s="11"/>
@@ -4205,7 +4205,7 @@
         <v>163</v>
       </c>
       <c r="D154" s="19" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E154" s="8"/>
       <c r="F154" s="11"/>
@@ -4221,7 +4221,7 @@
         <v>164</v>
       </c>
       <c r="D155" s="19" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E155" s="8"/>
       <c r="F155" s="11"/>
@@ -4235,11 +4235,11 @@
       </c>
       <c r="C156" s="25"/>
       <c r="D156" s="19" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="E156" s="8"/>
       <c r="F156" s="28" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
     </row>
     <row r="157" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4253,11 +4253,11 @@
         <v>166</v>
       </c>
       <c r="D157" s="19" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="E157" s="8"/>
       <c r="F157" s="28" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
     </row>
     <row r="158" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4271,11 +4271,11 @@
         <v>167</v>
       </c>
       <c r="D158" s="19" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="E158" s="8"/>
       <c r="F158" s="28" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
     </row>
     <row r="159" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4289,11 +4289,11 @@
         <v>168</v>
       </c>
       <c r="D159" s="19" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="E159" s="8"/>
       <c r="F159" s="28" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
     </row>
     <row r="160" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4303,7 +4303,7 @@
       <c r="B160" s="25"/>
       <c r="C160" s="25"/>
       <c r="D160" s="19" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="E160" s="8"/>
       <c r="F160" s="11"/>
@@ -4313,11 +4313,11 @@
         <v>7</v>
       </c>
       <c r="B161" s="7" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="C161" s="25"/>
       <c r="D161" s="19" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="E161" s="8"/>
       <c r="F161" s="11"/>
@@ -4333,7 +4333,7 @@
         <v>170</v>
       </c>
       <c r="D162" s="19" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E162" s="8"/>
       <c r="F162" s="11"/>
@@ -4349,7 +4349,7 @@
         <v>171</v>
       </c>
       <c r="D163" s="19" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E163" s="8"/>
       <c r="F163" s="11"/>
@@ -4365,7 +4365,7 @@
         <v>172</v>
       </c>
       <c r="D164" s="19" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E164" s="8"/>
       <c r="F164" s="11"/>
@@ -4378,10 +4378,10 @@
         <v>7</v>
       </c>
       <c r="C165" s="7" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="D165" s="19" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E165" s="8"/>
       <c r="F165" s="11"/>
@@ -4394,10 +4394,10 @@
         <v>7</v>
       </c>
       <c r="C166" s="7" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="D166" s="19" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E166" s="8"/>
       <c r="F166" s="11"/>
@@ -4407,11 +4407,11 @@
         <v>7</v>
       </c>
       <c r="B167" s="7" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="C167" s="25"/>
       <c r="D167" s="19" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="E167" s="8"/>
       <c r="F167" s="11"/>
@@ -4424,40 +4424,42 @@
         <v>7</v>
       </c>
       <c r="C168" s="7" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="D168" s="19" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="E168" s="8"/>
       <c r="F168" s="11"/>
     </row>
-    <row r="169" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A169" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B169" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="C169" s="25"/>
+        <v>7</v>
+      </c>
+      <c r="C169" s="7" t="s">
+        <v>177</v>
+      </c>
       <c r="D169" s="19" t="s">
-        <v>329</v>
-      </c>
-      <c r="E169" s="8"/>
-      <c r="F169" s="11"/>
+        <v>415</v>
+      </c>
+      <c r="E169" s="10"/>
+      <c r="F169" s="12" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="170" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A170" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B170" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C170" s="7" t="s">
-        <v>174</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="C170" s="25"/>
       <c r="D170" s="19" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="E170" s="8"/>
       <c r="F170" s="11"/>
@@ -4470,10 +4472,10 @@
         <v>7</v>
       </c>
       <c r="C171" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D171" s="19" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="E171" s="8"/>
       <c r="F171" s="11"/>
@@ -4483,32 +4485,30 @@
         <v>7</v>
       </c>
       <c r="B172" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C172" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D172" s="19" t="s">
+        <v>329</v>
+      </c>
+      <c r="E172" s="8"/>
+      <c r="F172" s="11"/>
+    </row>
+    <row r="173" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A173" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B173" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="C172" s="25"/>
-      <c r="D172" s="19" t="s">
-        <v>371</v>
-      </c>
-      <c r="E172" s="8"/>
-      <c r="F172" s="9"/>
-    </row>
-    <row r="173" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A173" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B173" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C173" s="7" t="s">
-        <v>177</v>
-      </c>
+      <c r="C173" s="25"/>
       <c r="D173" s="19" t="s">
-        <v>332</v>
-      </c>
-      <c r="E173" s="10"/>
-      <c r="F173" s="12" t="s">
-        <v>400</v>
-      </c>
+        <v>366</v>
+      </c>
+      <c r="E173" s="8"/>
+      <c r="F173" s="9"/>
     </row>
     <row r="174" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A174" s="7" t="s">
@@ -4518,10 +4518,10 @@
         <v>7</v>
       </c>
       <c r="C174" s="7" t="s">
-        <v>178</v>
+        <v>417</v>
       </c>
       <c r="D174" s="19" t="s">
-        <v>333</v>
+        <v>418</v>
       </c>
       <c r="E174" s="8"/>
       <c r="F174" s="6"/>
@@ -4534,22 +4534,22 @@
         <v>7</v>
       </c>
       <c r="C175" s="7" t="s">
-        <v>179</v>
+        <v>416</v>
       </c>
       <c r="D175" s="29" t="s">
-        <v>334</v>
+        <v>419</v>
       </c>
       <c r="E175" s="8"/>
       <c r="F175" s="11"/>
     </row>
     <row r="176" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A176" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B176" s="25"/>
       <c r="C176" s="25"/>
       <c r="D176" s="19" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="E176" s="8"/>
       <c r="F176" s="11"/>
@@ -4559,11 +4559,11 @@
         <v>7</v>
       </c>
       <c r="B177" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C177" s="25"/>
       <c r="D177" s="19" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="E177" s="8"/>
       <c r="F177" s="11"/>
@@ -4576,10 +4576,10 @@
         <v>7</v>
       </c>
       <c r="C178" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D178" s="19" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="E178" s="8"/>
       <c r="F178" s="11"/>
@@ -4592,10 +4592,10 @@
         <v>7</v>
       </c>
       <c r="C179" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D179" s="19" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="E179" s="8"/>
       <c r="F179" s="11"/>
@@ -4605,11 +4605,11 @@
         <v>7</v>
       </c>
       <c r="B180" s="7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C180" s="25"/>
       <c r="D180" s="19" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="E180" s="8"/>
       <c r="F180" s="11"/>
@@ -4622,22 +4622,22 @@
         <v>7</v>
       </c>
       <c r="C181" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D181" s="19" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="E181" s="8"/>
       <c r="F181" s="11"/>
     </row>
     <row r="182" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A182" s="7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B182" s="25"/>
       <c r="C182" s="25"/>
       <c r="D182" s="19" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="E182" s="8"/>
       <c r="F182" s="11"/>
@@ -4647,11 +4647,11 @@
         <v>7</v>
       </c>
       <c r="B183" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C183" s="25"/>
       <c r="D183" s="19" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="E183" s="8"/>
       <c r="F183" s="11"/>
@@ -4664,10 +4664,10 @@
         <v>7</v>
       </c>
       <c r="C184" s="16" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="D184" s="19" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="E184" s="10"/>
       <c r="F184" s="11"/>
@@ -4677,11 +4677,11 @@
         <v>7</v>
       </c>
       <c r="B185" s="7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C185" s="25"/>
       <c r="D185" s="19" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="E185" s="8"/>
       <c r="F185" s="11"/>
@@ -4694,10 +4694,10 @@
         <v>7</v>
       </c>
       <c r="C186" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D186" s="29" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="E186" s="8"/>
       <c r="F186" s="11"/>
@@ -4707,11 +4707,11 @@
         <v>7</v>
       </c>
       <c r="B187" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C187" s="25"/>
       <c r="D187" s="19" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="E187" s="8"/>
       <c r="F187" s="11"/>
@@ -4724,10 +4724,10 @@
         <v>7</v>
       </c>
       <c r="C188" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D188" s="19" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="E188" s="8"/>
       <c r="F188" s="11"/>
@@ -4737,11 +4737,11 @@
         <v>7</v>
       </c>
       <c r="B189" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C189" s="25"/>
       <c r="D189" s="19" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="E189" s="8"/>
       <c r="F189" s="11"/>
@@ -4754,10 +4754,10 @@
         <v>7</v>
       </c>
       <c r="C190" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D190" s="19" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="E190" s="8"/>
       <c r="F190" s="11"/>
@@ -4770,22 +4770,22 @@
         <v>7</v>
       </c>
       <c r="C191" s="7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D191" s="19" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="E191" s="8"/>
       <c r="F191" s="11"/>
     </row>
     <row r="192" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A192" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B192" s="25"/>
       <c r="C192" s="25"/>
       <c r="D192" s="19" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="E192" s="8"/>
       <c r="F192" s="11"/>
@@ -4795,11 +4795,11 @@
         <v>7</v>
       </c>
       <c r="B193" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C193" s="25"/>
       <c r="D193" s="19" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="E193" s="8"/>
       <c r="F193" s="11"/>
@@ -4812,10 +4812,10 @@
         <v>7</v>
       </c>
       <c r="C194" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D194" s="19" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="E194" s="8"/>
       <c r="F194" s="11"/>
@@ -4828,10 +4828,10 @@
         <v>7</v>
       </c>
       <c r="C195" s="7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D195" s="19" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="E195" s="8"/>
       <c r="F195" s="11"/>
@@ -4841,11 +4841,11 @@
         <v>7</v>
       </c>
       <c r="B196" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C196" s="25"/>
       <c r="D196" s="18" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E196" s="8"/>
       <c r="F196" s="11"/>
@@ -4858,14 +4858,14 @@
         <v>7</v>
       </c>
       <c r="C197" s="7" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="D197" s="19" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="E197" s="8"/>
       <c r="F197" s="28" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
     </row>
     <row r="198" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4876,10 +4876,10 @@
         <v>7</v>
       </c>
       <c r="C198" s="7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D198" s="19" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="E198" s="8"/>
       <c r="F198" s="11"/>
@@ -4889,11 +4889,11 @@
         <v>7</v>
       </c>
       <c r="B199" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C199" s="25"/>
       <c r="D199" s="19" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="E199" s="8"/>
       <c r="F199" s="11"/>
@@ -4906,22 +4906,22 @@
         <v>7</v>
       </c>
       <c r="C200" s="7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D200" s="29" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="E200" s="8"/>
       <c r="F200" s="11"/>
     </row>
     <row r="201" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A201" s="7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B201" s="25"/>
       <c r="C201" s="25"/>
       <c r="D201" s="19" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="E201" s="8"/>
       <c r="F201" s="11"/>
@@ -4931,11 +4931,11 @@
         <v>7</v>
       </c>
       <c r="B202" s="7" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C202" s="25"/>
       <c r="D202" s="19" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="E202" s="8"/>
       <c r="F202" s="11"/>
@@ -4948,10 +4948,10 @@
         <v>7</v>
       </c>
       <c r="C203" s="7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D203" s="19" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E203" s="8"/>
       <c r="F203" s="11"/>
@@ -4961,11 +4961,11 @@
         <v>7</v>
       </c>
       <c r="B204" s="7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C204" s="25"/>
       <c r="D204" s="19" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="E204" s="8"/>
       <c r="F204" s="11"/>

</xml_diff>

<commit_message>
Updated Data Theft annotation to account for stored data or application-data (e.g. entered into a web browser)
</commit_message>
<xml_diff>
--- a/mind_maps/malware_capabilities_descriptions.xlsx
+++ b/mind_maps/malware_capabilities_descriptions.xlsx
@@ -940,9 +940,6 @@
     <t>The 'remove system artifacts' value indicates that the malware instance is able to remove its artifacts from a system.</t>
   </si>
   <si>
-    <t>The 'data theft' Capability indicates that the malware instance is able to steal data from the system on which it executes.</t>
-  </si>
-  <si>
     <t>The 'steal authentication credentials' value indicates that the malware instance is able to steal authentication credentials.</t>
   </si>
   <si>
@@ -1274,6 +1271,9 @@
   </si>
   <si>
     <t>The 'capture file system' value indicates that the malware instance is able to capture data from a system's file system.</t>
+  </si>
+  <si>
+    <t>The 'data theft' Capability indicates that the malware instance is able to steal data from the system on which it executes. This includes data stored in some form, e.g. in a file, as well as data that may be entered into some application such as a web-browser.</t>
   </si>
 </sst>
 </file>
@@ -1865,8 +1865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV204"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B166" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D176" sqref="D176"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C133" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D140" sqref="D140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.61328125" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1937,7 +1937,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="6"/>
@@ -1953,7 +1953,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="6"/>
@@ -1969,7 +1969,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="6"/>
@@ -2131,7 +2131,7 @@
         <v>22</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="11"/>
@@ -2157,7 +2157,7 @@
       </c>
       <c r="C19" s="25"/>
       <c r="D19" s="18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="11"/>
@@ -2219,7 +2219,7 @@
         <v>28</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="9"/>
@@ -2239,7 +2239,7 @@
       </c>
       <c r="E24" s="10"/>
       <c r="F24" s="12" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2285,7 +2285,7 @@
         <v>32</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E27" s="8"/>
       <c r="F27" s="11"/>
@@ -2585,7 +2585,7 @@
         <v>53</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E47" s="8"/>
       <c r="F47" s="11"/>
@@ -2695,7 +2695,7 @@
         <v>60</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E54" s="10"/>
       <c r="F54" s="11"/>
@@ -2711,7 +2711,7 @@
         <v>61</v>
       </c>
       <c r="D55" s="27" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E55" s="10"/>
       <c r="F55" s="11"/>
@@ -2727,7 +2727,7 @@
         <v>62</v>
       </c>
       <c r="D56" s="27" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E56" s="10"/>
       <c r="F56" s="11"/>
@@ -2803,7 +2803,7 @@
       </c>
       <c r="C61" s="25"/>
       <c r="D61" s="18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E61" s="8"/>
       <c r="F61" s="11"/>
@@ -2819,7 +2819,7 @@
         <v>68</v>
       </c>
       <c r="D62" s="19" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E62" s="8"/>
       <c r="F62" s="11"/>
@@ -2833,7 +2833,7 @@
       </c>
       <c r="C63" s="25"/>
       <c r="D63" s="18" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E63" s="8"/>
       <c r="F63" s="11"/>
@@ -2921,7 +2921,7 @@
       </c>
       <c r="C69" s="25"/>
       <c r="D69" s="18" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E69" s="8"/>
       <c r="F69" s="11"/>
@@ -2999,7 +2999,7 @@
         <v>82</v>
       </c>
       <c r="D74" s="18" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E74" s="8"/>
       <c r="F74" s="11"/>
@@ -3055,7 +3055,7 @@
       </c>
       <c r="C78" s="25"/>
       <c r="D78" s="18" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E78" s="8"/>
       <c r="F78" s="11"/>
@@ -3085,7 +3085,7 @@
       </c>
       <c r="C80" s="25"/>
       <c r="D80" s="18" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E80" s="8"/>
       <c r="F80" s="11"/>
@@ -3133,7 +3133,7 @@
         <v>94</v>
       </c>
       <c r="D83" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E83" s="8"/>
       <c r="F83" s="11"/>
@@ -3146,14 +3146,14 @@
         <v>7</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D84" s="18" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E84" s="8"/>
       <c r="F84" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3161,7 +3161,7 @@
         <v>7</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C85" s="25"/>
       <c r="D85" s="18" t="s">
@@ -3183,7 +3183,7 @@
         <v>97</v>
       </c>
       <c r="D86" s="18" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E86" s="8"/>
       <c r="F86" s="11"/>
@@ -3323,7 +3323,7 @@
         <v>107</v>
       </c>
       <c r="D95" s="20" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E95" s="8"/>
       <c r="F95" s="11"/>
@@ -3367,7 +3367,7 @@
       <c r="B98" s="25"/>
       <c r="C98" s="25"/>
       <c r="D98" s="19" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E98" s="8"/>
       <c r="F98" s="11"/>
@@ -3397,7 +3397,7 @@
         <v>112</v>
       </c>
       <c r="D100" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E100" s="8"/>
       <c r="F100" s="11"/>
@@ -3427,7 +3427,7 @@
       </c>
       <c r="C102" s="25"/>
       <c r="D102" s="19" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E102" s="8"/>
       <c r="F102" s="11"/>
@@ -3443,7 +3443,7 @@
         <v>115</v>
       </c>
       <c r="D103" s="19" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E103" s="8"/>
       <c r="F103" s="11"/>
@@ -3455,7 +3455,7 @@
       </c>
       <c r="C104" s="25"/>
       <c r="D104" s="19" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E104" s="8"/>
       <c r="F104" s="11"/>
@@ -3759,7 +3759,7 @@
         <v>134</v>
       </c>
       <c r="D125" s="19" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E125" s="8"/>
       <c r="F125" s="11"/>
@@ -3932,14 +3932,14 @@
       <c r="E136" s="8"/>
       <c r="F136" s="11"/>
     </row>
-    <row r="137" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A137" s="7" t="s">
         <v>146</v>
       </c>
       <c r="B137" s="25"/>
       <c r="C137" s="25"/>
       <c r="D137" s="19" t="s">
-        <v>308</v>
+        <v>419</v>
       </c>
       <c r="E137" s="8"/>
       <c r="F137" s="11"/>
@@ -3953,7 +3953,7 @@
       </c>
       <c r="C138" s="25"/>
       <c r="D138" s="19" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E138" s="8"/>
       <c r="F138" s="11"/>
@@ -3969,7 +3969,7 @@
         <v>148</v>
       </c>
       <c r="D139" s="19" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E139" s="8"/>
       <c r="F139" s="11"/>
@@ -3985,7 +3985,7 @@
         <v>149</v>
       </c>
       <c r="D140" s="19" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E140" s="8"/>
       <c r="F140" s="11"/>
@@ -4001,7 +4001,7 @@
         <v>150</v>
       </c>
       <c r="D141" s="19" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E141" s="8"/>
       <c r="F141" s="11"/>
@@ -4017,7 +4017,7 @@
         <v>151</v>
       </c>
       <c r="D142" s="19" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E142" s="8"/>
       <c r="F142" s="11"/>
@@ -4031,7 +4031,7 @@
       </c>
       <c r="C143" s="25"/>
       <c r="D143" s="19" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E143" s="8"/>
       <c r="F143" s="11"/>
@@ -4047,7 +4047,7 @@
         <v>153</v>
       </c>
       <c r="D144" s="19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E144" s="8"/>
       <c r="F144" s="11"/>
@@ -4063,7 +4063,7 @@
         <v>154</v>
       </c>
       <c r="D145" s="19" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E145" s="8"/>
       <c r="F145" s="11"/>
@@ -4079,7 +4079,7 @@
         <v>155</v>
       </c>
       <c r="D146" s="19" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E146" s="8"/>
       <c r="F146" s="11"/>
@@ -4095,7 +4095,7 @@
         <v>156</v>
       </c>
       <c r="D147" s="19" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E147" s="8"/>
       <c r="F147" s="11"/>
@@ -4111,7 +4111,7 @@
         <v>157</v>
       </c>
       <c r="D148" s="19" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E148" s="8"/>
       <c r="F148" s="11"/>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="C149" s="25"/>
       <c r="D149" s="19" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E149" s="8"/>
       <c r="F149" s="11"/>
@@ -4141,7 +4141,7 @@
         <v>159</v>
       </c>
       <c r="D150" s="19" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E150" s="8"/>
       <c r="F150" s="11"/>
@@ -4157,7 +4157,7 @@
         <v>160</v>
       </c>
       <c r="D151" s="19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E151" s="8"/>
       <c r="F151" s="11"/>
@@ -4173,7 +4173,7 @@
         <v>161</v>
       </c>
       <c r="D152" s="19" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E152" s="10"/>
       <c r="F152" s="11"/>
@@ -4189,7 +4189,7 @@
         <v>162</v>
       </c>
       <c r="D153" s="19" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E153" s="10"/>
       <c r="F153" s="11"/>
@@ -4205,7 +4205,7 @@
         <v>163</v>
       </c>
       <c r="D154" s="19" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E154" s="8"/>
       <c r="F154" s="11"/>
@@ -4221,7 +4221,7 @@
         <v>164</v>
       </c>
       <c r="D155" s="19" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E155" s="8"/>
       <c r="F155" s="11"/>
@@ -4235,11 +4235,11 @@
       </c>
       <c r="C156" s="25"/>
       <c r="D156" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E156" s="8"/>
       <c r="F156" s="28" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="157" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4253,11 +4253,11 @@
         <v>166</v>
       </c>
       <c r="D157" s="19" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E157" s="8"/>
       <c r="F157" s="28" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="158" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4271,11 +4271,11 @@
         <v>167</v>
       </c>
       <c r="D158" s="19" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E158" s="8"/>
       <c r="F158" s="28" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="159" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4289,11 +4289,11 @@
         <v>168</v>
       </c>
       <c r="D159" s="19" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E159" s="8"/>
       <c r="F159" s="28" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="160" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4303,7 +4303,7 @@
       <c r="B160" s="25"/>
       <c r="C160" s="25"/>
       <c r="D160" s="19" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E160" s="8"/>
       <c r="F160" s="11"/>
@@ -4313,11 +4313,11 @@
         <v>7</v>
       </c>
       <c r="B161" s="7" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C161" s="25"/>
       <c r="D161" s="19" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E161" s="8"/>
       <c r="F161" s="11"/>
@@ -4333,7 +4333,7 @@
         <v>170</v>
       </c>
       <c r="D162" s="19" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E162" s="8"/>
       <c r="F162" s="11"/>
@@ -4349,7 +4349,7 @@
         <v>171</v>
       </c>
       <c r="D163" s="19" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E163" s="8"/>
       <c r="F163" s="11"/>
@@ -4365,7 +4365,7 @@
         <v>172</v>
       </c>
       <c r="D164" s="19" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E164" s="8"/>
       <c r="F164" s="11"/>
@@ -4378,10 +4378,10 @@
         <v>7</v>
       </c>
       <c r="C165" s="7" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D165" s="19" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E165" s="8"/>
       <c r="F165" s="11"/>
@@ -4394,10 +4394,10 @@
         <v>7</v>
       </c>
       <c r="C166" s="7" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D166" s="19" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E166" s="8"/>
       <c r="F166" s="11"/>
@@ -4407,11 +4407,11 @@
         <v>7</v>
       </c>
       <c r="B167" s="7" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C167" s="25"/>
       <c r="D167" s="19" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E167" s="8"/>
       <c r="F167" s="11"/>
@@ -4424,10 +4424,10 @@
         <v>7</v>
       </c>
       <c r="C168" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="D168" s="19" t="s">
         <v>412</v>
-      </c>
-      <c r="D168" s="19" t="s">
-        <v>413</v>
       </c>
       <c r="E168" s="8"/>
       <c r="F168" s="11"/>
@@ -4443,11 +4443,11 @@
         <v>177</v>
       </c>
       <c r="D169" s="19" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E169" s="10"/>
       <c r="F169" s="12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="170" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4459,7 +4459,7 @@
       </c>
       <c r="C170" s="25"/>
       <c r="D170" s="19" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E170" s="8"/>
       <c r="F170" s="11"/>
@@ -4475,7 +4475,7 @@
         <v>174</v>
       </c>
       <c r="D171" s="19" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E171" s="8"/>
       <c r="F171" s="11"/>
@@ -4491,7 +4491,7 @@
         <v>175</v>
       </c>
       <c r="D172" s="19" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E172" s="8"/>
       <c r="F172" s="11"/>
@@ -4505,7 +4505,7 @@
       </c>
       <c r="C173" s="25"/>
       <c r="D173" s="19" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E173" s="8"/>
       <c r="F173" s="9"/>
@@ -4518,10 +4518,10 @@
         <v>7</v>
       </c>
       <c r="C174" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="D174" s="19" t="s">
         <v>417</v>
-      </c>
-      <c r="D174" s="19" t="s">
-        <v>418</v>
       </c>
       <c r="E174" s="8"/>
       <c r="F174" s="6"/>
@@ -4534,10 +4534,10 @@
         <v>7</v>
       </c>
       <c r="C175" s="7" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D175" s="29" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E175" s="8"/>
       <c r="F175" s="11"/>
@@ -4549,7 +4549,7 @@
       <c r="B176" s="25"/>
       <c r="C176" s="25"/>
       <c r="D176" s="19" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E176" s="8"/>
       <c r="F176" s="11"/>
@@ -4563,7 +4563,7 @@
       </c>
       <c r="C177" s="25"/>
       <c r="D177" s="19" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E177" s="8"/>
       <c r="F177" s="11"/>
@@ -4579,7 +4579,7 @@
         <v>180</v>
       </c>
       <c r="D178" s="19" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E178" s="8"/>
       <c r="F178" s="11"/>
@@ -4595,7 +4595,7 @@
         <v>181</v>
       </c>
       <c r="D179" s="19" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E179" s="8"/>
       <c r="F179" s="11"/>
@@ -4609,7 +4609,7 @@
       </c>
       <c r="C180" s="25"/>
       <c r="D180" s="19" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E180" s="8"/>
       <c r="F180" s="11"/>
@@ -4625,7 +4625,7 @@
         <v>183</v>
       </c>
       <c r="D181" s="19" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E181" s="8"/>
       <c r="F181" s="11"/>
@@ -4637,7 +4637,7 @@
       <c r="B182" s="25"/>
       <c r="C182" s="25"/>
       <c r="D182" s="19" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E182" s="8"/>
       <c r="F182" s="11"/>
@@ -4651,7 +4651,7 @@
       </c>
       <c r="C183" s="25"/>
       <c r="D183" s="19" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E183" s="8"/>
       <c r="F183" s="11"/>
@@ -4664,10 +4664,10 @@
         <v>7</v>
       </c>
       <c r="C184" s="16" t="s">
+        <v>336</v>
+      </c>
+      <c r="D184" s="19" t="s">
         <v>337</v>
-      </c>
-      <c r="D184" s="19" t="s">
-        <v>338</v>
       </c>
       <c r="E184" s="10"/>
       <c r="F184" s="11"/>
@@ -4681,7 +4681,7 @@
       </c>
       <c r="C185" s="25"/>
       <c r="D185" s="19" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E185" s="8"/>
       <c r="F185" s="11"/>
@@ -4697,7 +4697,7 @@
         <v>187</v>
       </c>
       <c r="D186" s="29" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E186" s="8"/>
       <c r="F186" s="11"/>
@@ -4711,7 +4711,7 @@
       </c>
       <c r="C187" s="25"/>
       <c r="D187" s="19" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E187" s="8"/>
       <c r="F187" s="11"/>
@@ -4727,7 +4727,7 @@
         <v>189</v>
       </c>
       <c r="D188" s="19" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E188" s="8"/>
       <c r="F188" s="11"/>
@@ -4741,7 +4741,7 @@
       </c>
       <c r="C189" s="25"/>
       <c r="D189" s="19" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E189" s="8"/>
       <c r="F189" s="11"/>
@@ -4757,7 +4757,7 @@
         <v>191</v>
       </c>
       <c r="D190" s="19" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E190" s="8"/>
       <c r="F190" s="11"/>
@@ -4773,7 +4773,7 @@
         <v>192</v>
       </c>
       <c r="D191" s="19" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E191" s="8"/>
       <c r="F191" s="11"/>
@@ -4785,7 +4785,7 @@
       <c r="B192" s="25"/>
       <c r="C192" s="25"/>
       <c r="D192" s="19" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E192" s="8"/>
       <c r="F192" s="11"/>
@@ -4799,7 +4799,7 @@
       </c>
       <c r="C193" s="25"/>
       <c r="D193" s="19" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E193" s="8"/>
       <c r="F193" s="11"/>
@@ -4815,7 +4815,7 @@
         <v>195</v>
       </c>
       <c r="D194" s="19" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E194" s="8"/>
       <c r="F194" s="11"/>
@@ -4831,7 +4831,7 @@
         <v>196</v>
       </c>
       <c r="D195" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E195" s="8"/>
       <c r="F195" s="11"/>
@@ -4858,14 +4858,14 @@
         <v>7</v>
       </c>
       <c r="C197" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="D197" s="19" t="s">
         <v>405</v>
-      </c>
-      <c r="D197" s="19" t="s">
-        <v>406</v>
       </c>
       <c r="E197" s="8"/>
       <c r="F197" s="28" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="198" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4879,7 +4879,7 @@
         <v>199</v>
       </c>
       <c r="D198" s="19" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E198" s="8"/>
       <c r="F198" s="11"/>
@@ -4893,7 +4893,7 @@
       </c>
       <c r="C199" s="25"/>
       <c r="D199" s="19" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E199" s="8"/>
       <c r="F199" s="11"/>
@@ -4909,7 +4909,7 @@
         <v>201</v>
       </c>
       <c r="D200" s="29" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E200" s="8"/>
       <c r="F200" s="11"/>
@@ -4921,7 +4921,7 @@
       <c r="B201" s="25"/>
       <c r="C201" s="25"/>
       <c r="D201" s="19" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E201" s="8"/>
       <c r="F201" s="11"/>
@@ -4935,7 +4935,7 @@
       </c>
       <c r="C202" s="25"/>
       <c r="D202" s="19" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E202" s="8"/>
       <c r="F202" s="11"/>
@@ -4965,7 +4965,7 @@
       </c>
       <c r="C204" s="25"/>
       <c r="D204" s="19" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E204" s="8"/>
       <c r="F204" s="11"/>

</xml_diff>

<commit_message>
Updated based on C2/Send Data to C2 Server changes
</commit_message>
<xml_diff>
--- a/mind_maps/malware_capabilities_descriptions.xlsx
+++ b/mind_maps/malware_capabilities_descriptions.xlsx
@@ -4,18 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="15960" windowHeight="12816" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="36" windowWidth="15960" windowHeight="12816"/>
   </bookViews>
   <sheets>
     <sheet name="malware_capabilities" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="423">
   <si>
     <t>Capability</t>
   </si>
@@ -1265,12 +1264,6 @@
     <t>The 'update configuration' value indicates that the malware instance is able to update its configuration using data received from a command and control server.</t>
   </si>
   <si>
-    <t>Send System Information to C2 Server</t>
-  </si>
-  <si>
-    <t>Send Heartbeat Data to C2 Server</t>
-  </si>
-  <si>
     <t>The 'send system information to c2 server' value indicates that the malware instance is able to send data regarding the system on which it is executing to a command and control server.</t>
   </si>
   <si>
@@ -1284,6 +1277,12 @@
   </si>
   <si>
     <t>The 'send heartbeat data to c2 server' value indicates that the malware instance is able to send heartbeat data to a command and control server, also commonly referred to as beaconing.</t>
+  </si>
+  <si>
+    <t>Send System Information</t>
+  </si>
+  <si>
+    <t>Send Heartbeat Data</t>
   </si>
 </sst>
 </file>
@@ -1875,8 +1874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV205"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.61328125" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -3377,7 +3376,7 @@
       <c r="B98" s="25"/>
       <c r="C98" s="25"/>
       <c r="D98" s="19" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E98" s="8"/>
       <c r="F98" s="11"/>
@@ -3414,7 +3413,7 @@
       </c>
       <c r="C101" s="25"/>
       <c r="D101" s="19" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E101" s="8"/>
       <c r="F101" s="11"/>
@@ -3426,11 +3425,11 @@
       <c r="B102" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C102" s="7" t="s">
+      <c r="C102" s="16" t="s">
+        <v>421</v>
+      </c>
+      <c r="D102" s="19" t="s">
         <v>416</v>
-      </c>
-      <c r="D102" s="19" t="s">
-        <v>418</v>
       </c>
       <c r="E102" s="10"/>
       <c r="F102" s="11"/>
@@ -3442,11 +3441,11 @@
       <c r="B103" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C103" s="7" t="s">
-        <v>417</v>
+      <c r="C103" s="16" t="s">
+        <v>422</v>
       </c>
       <c r="D103" s="19" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="E103" s="10"/>
       <c r="F103" s="11"/>
@@ -3467,7 +3466,7 @@
       <c r="A105" s="25"/>
       <c r="B105" s="25"/>
       <c r="C105" s="7" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D105" s="19" t="s">
         <v>413</v>
@@ -4992,2663 +4991,4 @@
     <oddFooter>&amp;"Helvetica,Regular"&amp;11&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16.61328125" customWidth="1"/>
-    <col min="2" max="2" width="22.53515625" customWidth="1"/>
-    <col min="3" max="3" width="25.765625" customWidth="1"/>
-    <col min="4" max="4" width="19.765625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:256" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="1"/>
-      <c r="AD1" s="1"/>
-      <c r="AE1" s="1"/>
-      <c r="AF1" s="1"/>
-      <c r="AG1" s="1"/>
-      <c r="AH1" s="1"/>
-      <c r="AI1" s="1"/>
-      <c r="AJ1" s="1"/>
-      <c r="AK1" s="1"/>
-      <c r="AL1" s="1"/>
-      <c r="AM1" s="1"/>
-      <c r="AN1" s="1"/>
-      <c r="AO1" s="1"/>
-      <c r="AP1" s="1"/>
-      <c r="AQ1" s="1"/>
-      <c r="AR1" s="1"/>
-      <c r="AS1" s="1"/>
-      <c r="AT1" s="1"/>
-      <c r="AU1" s="1"/>
-      <c r="AV1" s="1"/>
-      <c r="AW1" s="1"/>
-      <c r="AX1" s="1"/>
-      <c r="AY1" s="1"/>
-      <c r="AZ1" s="1"/>
-      <c r="BA1" s="1"/>
-      <c r="BB1" s="1"/>
-      <c r="BC1" s="1"/>
-      <c r="BD1" s="1"/>
-      <c r="BE1" s="1"/>
-      <c r="BF1" s="1"/>
-      <c r="BG1" s="1"/>
-      <c r="BH1" s="1"/>
-      <c r="BI1" s="1"/>
-      <c r="BJ1" s="1"/>
-      <c r="BK1" s="1"/>
-      <c r="BL1" s="1"/>
-      <c r="BM1" s="1"/>
-      <c r="BN1" s="1"/>
-      <c r="BO1" s="1"/>
-      <c r="BP1" s="1"/>
-      <c r="BQ1" s="1"/>
-      <c r="BR1" s="1"/>
-      <c r="BS1" s="1"/>
-      <c r="BT1" s="1"/>
-      <c r="BU1" s="1"/>
-      <c r="BV1" s="1"/>
-      <c r="BW1" s="1"/>
-      <c r="BX1" s="1"/>
-      <c r="BY1" s="1"/>
-      <c r="BZ1" s="1"/>
-      <c r="CA1" s="1"/>
-      <c r="CB1" s="1"/>
-      <c r="CC1" s="1"/>
-      <c r="CD1" s="1"/>
-      <c r="CE1" s="1"/>
-      <c r="CF1" s="1"/>
-      <c r="CG1" s="1"/>
-      <c r="CH1" s="1"/>
-      <c r="CI1" s="1"/>
-      <c r="CJ1" s="1"/>
-      <c r="CK1" s="1"/>
-      <c r="CL1" s="1"/>
-      <c r="CM1" s="1"/>
-      <c r="CN1" s="1"/>
-      <c r="CO1" s="1"/>
-      <c r="CP1" s="1"/>
-      <c r="CQ1" s="1"/>
-      <c r="CR1" s="1"/>
-      <c r="CS1" s="1"/>
-      <c r="CT1" s="1"/>
-      <c r="CU1" s="1"/>
-      <c r="CV1" s="1"/>
-      <c r="CW1" s="1"/>
-      <c r="CX1" s="1"/>
-      <c r="CY1" s="1"/>
-      <c r="CZ1" s="1"/>
-      <c r="DA1" s="1"/>
-      <c r="DB1" s="1"/>
-      <c r="DC1" s="1"/>
-      <c r="DD1" s="1"/>
-      <c r="DE1" s="1"/>
-      <c r="DF1" s="1"/>
-      <c r="DG1" s="1"/>
-      <c r="DH1" s="1"/>
-      <c r="DI1" s="1"/>
-      <c r="DJ1" s="1"/>
-      <c r="DK1" s="1"/>
-      <c r="DL1" s="1"/>
-      <c r="DM1" s="1"/>
-      <c r="DN1" s="1"/>
-      <c r="DO1" s="1"/>
-      <c r="DP1" s="1"/>
-      <c r="DQ1" s="1"/>
-      <c r="DR1" s="1"/>
-      <c r="DS1" s="1"/>
-      <c r="DT1" s="1"/>
-      <c r="DU1" s="1"/>
-      <c r="DV1" s="1"/>
-      <c r="DW1" s="1"/>
-      <c r="DX1" s="1"/>
-      <c r="DY1" s="1"/>
-      <c r="DZ1" s="1"/>
-      <c r="EA1" s="1"/>
-      <c r="EB1" s="1"/>
-      <c r="EC1" s="1"/>
-      <c r="ED1" s="1"/>
-      <c r="EE1" s="1"/>
-      <c r="EF1" s="1"/>
-      <c r="EG1" s="1"/>
-      <c r="EH1" s="1"/>
-      <c r="EI1" s="1"/>
-      <c r="EJ1" s="1"/>
-      <c r="EK1" s="1"/>
-      <c r="EL1" s="1"/>
-      <c r="EM1" s="1"/>
-      <c r="EN1" s="1"/>
-      <c r="EO1" s="1"/>
-      <c r="EP1" s="1"/>
-      <c r="EQ1" s="1"/>
-      <c r="ER1" s="1"/>
-      <c r="ES1" s="1"/>
-      <c r="ET1" s="1"/>
-      <c r="EU1" s="1"/>
-      <c r="EV1" s="1"/>
-      <c r="EW1" s="1"/>
-      <c r="EX1" s="1"/>
-      <c r="EY1" s="1"/>
-      <c r="EZ1" s="1"/>
-      <c r="FA1" s="1"/>
-      <c r="FB1" s="1"/>
-      <c r="FC1" s="1"/>
-      <c r="FD1" s="1"/>
-      <c r="FE1" s="1"/>
-      <c r="FF1" s="1"/>
-      <c r="FG1" s="1"/>
-      <c r="FH1" s="1"/>
-      <c r="FI1" s="1"/>
-      <c r="FJ1" s="1"/>
-      <c r="FK1" s="1"/>
-      <c r="FL1" s="1"/>
-      <c r="FM1" s="1"/>
-      <c r="FN1" s="1"/>
-      <c r="FO1" s="1"/>
-      <c r="FP1" s="1"/>
-      <c r="FQ1" s="1"/>
-      <c r="FR1" s="1"/>
-      <c r="FS1" s="1"/>
-      <c r="FT1" s="1"/>
-      <c r="FU1" s="1"/>
-      <c r="FV1" s="1"/>
-      <c r="FW1" s="1"/>
-      <c r="FX1" s="1"/>
-      <c r="FY1" s="1"/>
-      <c r="FZ1" s="1"/>
-      <c r="GA1" s="1"/>
-      <c r="GB1" s="1"/>
-      <c r="GC1" s="1"/>
-      <c r="GD1" s="1"/>
-      <c r="GE1" s="1"/>
-      <c r="GF1" s="1"/>
-      <c r="GG1" s="1"/>
-      <c r="GH1" s="1"/>
-      <c r="GI1" s="1"/>
-      <c r="GJ1" s="1"/>
-      <c r="GK1" s="1"/>
-      <c r="GL1" s="1"/>
-      <c r="GM1" s="1"/>
-      <c r="GN1" s="1"/>
-      <c r="GO1" s="1"/>
-      <c r="GP1" s="1"/>
-      <c r="GQ1" s="1"/>
-      <c r="GR1" s="1"/>
-      <c r="GS1" s="1"/>
-      <c r="GT1" s="1"/>
-      <c r="GU1" s="1"/>
-      <c r="GV1" s="1"/>
-      <c r="GW1" s="1"/>
-      <c r="GX1" s="1"/>
-      <c r="GY1" s="1"/>
-      <c r="GZ1" s="1"/>
-      <c r="HA1" s="1"/>
-      <c r="HB1" s="1"/>
-      <c r="HC1" s="1"/>
-      <c r="HD1" s="1"/>
-      <c r="HE1" s="1"/>
-      <c r="HF1" s="1"/>
-      <c r="HG1" s="1"/>
-      <c r="HH1" s="1"/>
-      <c r="HI1" s="1"/>
-      <c r="HJ1" s="1"/>
-      <c r="HK1" s="1"/>
-      <c r="HL1" s="1"/>
-      <c r="HM1" s="1"/>
-      <c r="HN1" s="1"/>
-      <c r="HO1" s="1"/>
-      <c r="HP1" s="1"/>
-      <c r="HQ1" s="1"/>
-      <c r="HR1" s="1"/>
-      <c r="HS1" s="1"/>
-      <c r="HT1" s="1"/>
-      <c r="HU1" s="1"/>
-      <c r="HV1" s="1"/>
-      <c r="HW1" s="1"/>
-      <c r="HX1" s="1"/>
-      <c r="HY1" s="1"/>
-      <c r="HZ1" s="1"/>
-      <c r="IA1" s="1"/>
-      <c r="IB1" s="1"/>
-      <c r="IC1" s="1"/>
-      <c r="ID1" s="1"/>
-      <c r="IE1" s="1"/>
-      <c r="IF1" s="1"/>
-      <c r="IG1" s="1"/>
-      <c r="IH1" s="1"/>
-      <c r="II1" s="1"/>
-      <c r="IJ1" s="1"/>
-      <c r="IK1" s="1"/>
-      <c r="IL1" s="1"/>
-      <c r="IM1" s="1"/>
-      <c r="IN1" s="1"/>
-      <c r="IO1" s="1"/>
-      <c r="IP1" s="1"/>
-      <c r="IQ1" s="1"/>
-      <c r="IR1" s="1"/>
-      <c r="IS1" s="1"/>
-      <c r="IT1" s="1"/>
-      <c r="IU1" s="1"/>
-      <c r="IV1" s="1"/>
-    </row>
-    <row r="2" spans="1:256" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="19" t="s">
-        <v>420</v>
-      </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="1"/>
-      <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
-      <c r="AI2" s="1"/>
-      <c r="AJ2" s="1"/>
-      <c r="AK2" s="1"/>
-      <c r="AL2" s="1"/>
-      <c r="AM2" s="1"/>
-      <c r="AN2" s="1"/>
-      <c r="AO2" s="1"/>
-      <c r="AP2" s="1"/>
-      <c r="AQ2" s="1"/>
-      <c r="AR2" s="1"/>
-      <c r="AS2" s="1"/>
-      <c r="AT2" s="1"/>
-      <c r="AU2" s="1"/>
-      <c r="AV2" s="1"/>
-      <c r="AW2" s="1"/>
-      <c r="AX2" s="1"/>
-      <c r="AY2" s="1"/>
-      <c r="AZ2" s="1"/>
-      <c r="BA2" s="1"/>
-      <c r="BB2" s="1"/>
-      <c r="BC2" s="1"/>
-      <c r="BD2" s="1"/>
-      <c r="BE2" s="1"/>
-      <c r="BF2" s="1"/>
-      <c r="BG2" s="1"/>
-      <c r="BH2" s="1"/>
-      <c r="BI2" s="1"/>
-      <c r="BJ2" s="1"/>
-      <c r="BK2" s="1"/>
-      <c r="BL2" s="1"/>
-      <c r="BM2" s="1"/>
-      <c r="BN2" s="1"/>
-      <c r="BO2" s="1"/>
-      <c r="BP2" s="1"/>
-      <c r="BQ2" s="1"/>
-      <c r="BR2" s="1"/>
-      <c r="BS2" s="1"/>
-      <c r="BT2" s="1"/>
-      <c r="BU2" s="1"/>
-      <c r="BV2" s="1"/>
-      <c r="BW2" s="1"/>
-      <c r="BX2" s="1"/>
-      <c r="BY2" s="1"/>
-      <c r="BZ2" s="1"/>
-      <c r="CA2" s="1"/>
-      <c r="CB2" s="1"/>
-      <c r="CC2" s="1"/>
-      <c r="CD2" s="1"/>
-      <c r="CE2" s="1"/>
-      <c r="CF2" s="1"/>
-      <c r="CG2" s="1"/>
-      <c r="CH2" s="1"/>
-      <c r="CI2" s="1"/>
-      <c r="CJ2" s="1"/>
-      <c r="CK2" s="1"/>
-      <c r="CL2" s="1"/>
-      <c r="CM2" s="1"/>
-      <c r="CN2" s="1"/>
-      <c r="CO2" s="1"/>
-      <c r="CP2" s="1"/>
-      <c r="CQ2" s="1"/>
-      <c r="CR2" s="1"/>
-      <c r="CS2" s="1"/>
-      <c r="CT2" s="1"/>
-      <c r="CU2" s="1"/>
-      <c r="CV2" s="1"/>
-      <c r="CW2" s="1"/>
-      <c r="CX2" s="1"/>
-      <c r="CY2" s="1"/>
-      <c r="CZ2" s="1"/>
-      <c r="DA2" s="1"/>
-      <c r="DB2" s="1"/>
-      <c r="DC2" s="1"/>
-      <c r="DD2" s="1"/>
-      <c r="DE2" s="1"/>
-      <c r="DF2" s="1"/>
-      <c r="DG2" s="1"/>
-      <c r="DH2" s="1"/>
-      <c r="DI2" s="1"/>
-      <c r="DJ2" s="1"/>
-      <c r="DK2" s="1"/>
-      <c r="DL2" s="1"/>
-      <c r="DM2" s="1"/>
-      <c r="DN2" s="1"/>
-      <c r="DO2" s="1"/>
-      <c r="DP2" s="1"/>
-      <c r="DQ2" s="1"/>
-      <c r="DR2" s="1"/>
-      <c r="DS2" s="1"/>
-      <c r="DT2" s="1"/>
-      <c r="DU2" s="1"/>
-      <c r="DV2" s="1"/>
-      <c r="DW2" s="1"/>
-      <c r="DX2" s="1"/>
-      <c r="DY2" s="1"/>
-      <c r="DZ2" s="1"/>
-      <c r="EA2" s="1"/>
-      <c r="EB2" s="1"/>
-      <c r="EC2" s="1"/>
-      <c r="ED2" s="1"/>
-      <c r="EE2" s="1"/>
-      <c r="EF2" s="1"/>
-      <c r="EG2" s="1"/>
-      <c r="EH2" s="1"/>
-      <c r="EI2" s="1"/>
-      <c r="EJ2" s="1"/>
-      <c r="EK2" s="1"/>
-      <c r="EL2" s="1"/>
-      <c r="EM2" s="1"/>
-      <c r="EN2" s="1"/>
-      <c r="EO2" s="1"/>
-      <c r="EP2" s="1"/>
-      <c r="EQ2" s="1"/>
-      <c r="ER2" s="1"/>
-      <c r="ES2" s="1"/>
-      <c r="ET2" s="1"/>
-      <c r="EU2" s="1"/>
-      <c r="EV2" s="1"/>
-      <c r="EW2" s="1"/>
-      <c r="EX2" s="1"/>
-      <c r="EY2" s="1"/>
-      <c r="EZ2" s="1"/>
-      <c r="FA2" s="1"/>
-      <c r="FB2" s="1"/>
-      <c r="FC2" s="1"/>
-      <c r="FD2" s="1"/>
-      <c r="FE2" s="1"/>
-      <c r="FF2" s="1"/>
-      <c r="FG2" s="1"/>
-      <c r="FH2" s="1"/>
-      <c r="FI2" s="1"/>
-      <c r="FJ2" s="1"/>
-      <c r="FK2" s="1"/>
-      <c r="FL2" s="1"/>
-      <c r="FM2" s="1"/>
-      <c r="FN2" s="1"/>
-      <c r="FO2" s="1"/>
-      <c r="FP2" s="1"/>
-      <c r="FQ2" s="1"/>
-      <c r="FR2" s="1"/>
-      <c r="FS2" s="1"/>
-      <c r="FT2" s="1"/>
-      <c r="FU2" s="1"/>
-      <c r="FV2" s="1"/>
-      <c r="FW2" s="1"/>
-      <c r="FX2" s="1"/>
-      <c r="FY2" s="1"/>
-      <c r="FZ2" s="1"/>
-      <c r="GA2" s="1"/>
-      <c r="GB2" s="1"/>
-      <c r="GC2" s="1"/>
-      <c r="GD2" s="1"/>
-      <c r="GE2" s="1"/>
-      <c r="GF2" s="1"/>
-      <c r="GG2" s="1"/>
-      <c r="GH2" s="1"/>
-      <c r="GI2" s="1"/>
-      <c r="GJ2" s="1"/>
-      <c r="GK2" s="1"/>
-      <c r="GL2" s="1"/>
-      <c r="GM2" s="1"/>
-      <c r="GN2" s="1"/>
-      <c r="GO2" s="1"/>
-      <c r="GP2" s="1"/>
-      <c r="GQ2" s="1"/>
-      <c r="GR2" s="1"/>
-      <c r="GS2" s="1"/>
-      <c r="GT2" s="1"/>
-      <c r="GU2" s="1"/>
-      <c r="GV2" s="1"/>
-      <c r="GW2" s="1"/>
-      <c r="GX2" s="1"/>
-      <c r="GY2" s="1"/>
-      <c r="GZ2" s="1"/>
-      <c r="HA2" s="1"/>
-      <c r="HB2" s="1"/>
-      <c r="HC2" s="1"/>
-      <c r="HD2" s="1"/>
-      <c r="HE2" s="1"/>
-      <c r="HF2" s="1"/>
-      <c r="HG2" s="1"/>
-      <c r="HH2" s="1"/>
-      <c r="HI2" s="1"/>
-      <c r="HJ2" s="1"/>
-      <c r="HK2" s="1"/>
-      <c r="HL2" s="1"/>
-      <c r="HM2" s="1"/>
-      <c r="HN2" s="1"/>
-      <c r="HO2" s="1"/>
-      <c r="HP2" s="1"/>
-      <c r="HQ2" s="1"/>
-      <c r="HR2" s="1"/>
-      <c r="HS2" s="1"/>
-      <c r="HT2" s="1"/>
-      <c r="HU2" s="1"/>
-      <c r="HV2" s="1"/>
-      <c r="HW2" s="1"/>
-      <c r="HX2" s="1"/>
-      <c r="HY2" s="1"/>
-      <c r="HZ2" s="1"/>
-      <c r="IA2" s="1"/>
-      <c r="IB2" s="1"/>
-      <c r="IC2" s="1"/>
-      <c r="ID2" s="1"/>
-      <c r="IE2" s="1"/>
-      <c r="IF2" s="1"/>
-      <c r="IG2" s="1"/>
-      <c r="IH2" s="1"/>
-      <c r="II2" s="1"/>
-      <c r="IJ2" s="1"/>
-      <c r="IK2" s="1"/>
-      <c r="IL2" s="1"/>
-      <c r="IM2" s="1"/>
-      <c r="IN2" s="1"/>
-      <c r="IO2" s="1"/>
-      <c r="IP2" s="1"/>
-      <c r="IQ2" s="1"/>
-      <c r="IR2" s="1"/>
-      <c r="IS2" s="1"/>
-      <c r="IT2" s="1"/>
-      <c r="IU2" s="1"/>
-      <c r="IV2" s="1"/>
-    </row>
-    <row r="3" spans="1:256" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="19" t="s">
-        <v>366</v>
-      </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
-      <c r="AC3" s="1"/>
-      <c r="AD3" s="1"/>
-      <c r="AE3" s="1"/>
-      <c r="AF3" s="1"/>
-      <c r="AG3" s="1"/>
-      <c r="AH3" s="1"/>
-      <c r="AI3" s="1"/>
-      <c r="AJ3" s="1"/>
-      <c r="AK3" s="1"/>
-      <c r="AL3" s="1"/>
-      <c r="AM3" s="1"/>
-      <c r="AN3" s="1"/>
-      <c r="AO3" s="1"/>
-      <c r="AP3" s="1"/>
-      <c r="AQ3" s="1"/>
-      <c r="AR3" s="1"/>
-      <c r="AS3" s="1"/>
-      <c r="AT3" s="1"/>
-      <c r="AU3" s="1"/>
-      <c r="AV3" s="1"/>
-      <c r="AW3" s="1"/>
-      <c r="AX3" s="1"/>
-      <c r="AY3" s="1"/>
-      <c r="AZ3" s="1"/>
-      <c r="BA3" s="1"/>
-      <c r="BB3" s="1"/>
-      <c r="BC3" s="1"/>
-      <c r="BD3" s="1"/>
-      <c r="BE3" s="1"/>
-      <c r="BF3" s="1"/>
-      <c r="BG3" s="1"/>
-      <c r="BH3" s="1"/>
-      <c r="BI3" s="1"/>
-      <c r="BJ3" s="1"/>
-      <c r="BK3" s="1"/>
-      <c r="BL3" s="1"/>
-      <c r="BM3" s="1"/>
-      <c r="BN3" s="1"/>
-      <c r="BO3" s="1"/>
-      <c r="BP3" s="1"/>
-      <c r="BQ3" s="1"/>
-      <c r="BR3" s="1"/>
-      <c r="BS3" s="1"/>
-      <c r="BT3" s="1"/>
-      <c r="BU3" s="1"/>
-      <c r="BV3" s="1"/>
-      <c r="BW3" s="1"/>
-      <c r="BX3" s="1"/>
-      <c r="BY3" s="1"/>
-      <c r="BZ3" s="1"/>
-      <c r="CA3" s="1"/>
-      <c r="CB3" s="1"/>
-      <c r="CC3" s="1"/>
-      <c r="CD3" s="1"/>
-      <c r="CE3" s="1"/>
-      <c r="CF3" s="1"/>
-      <c r="CG3" s="1"/>
-      <c r="CH3" s="1"/>
-      <c r="CI3" s="1"/>
-      <c r="CJ3" s="1"/>
-      <c r="CK3" s="1"/>
-      <c r="CL3" s="1"/>
-      <c r="CM3" s="1"/>
-      <c r="CN3" s="1"/>
-      <c r="CO3" s="1"/>
-      <c r="CP3" s="1"/>
-      <c r="CQ3" s="1"/>
-      <c r="CR3" s="1"/>
-      <c r="CS3" s="1"/>
-      <c r="CT3" s="1"/>
-      <c r="CU3" s="1"/>
-      <c r="CV3" s="1"/>
-      <c r="CW3" s="1"/>
-      <c r="CX3" s="1"/>
-      <c r="CY3" s="1"/>
-      <c r="CZ3" s="1"/>
-      <c r="DA3" s="1"/>
-      <c r="DB3" s="1"/>
-      <c r="DC3" s="1"/>
-      <c r="DD3" s="1"/>
-      <c r="DE3" s="1"/>
-      <c r="DF3" s="1"/>
-      <c r="DG3" s="1"/>
-      <c r="DH3" s="1"/>
-      <c r="DI3" s="1"/>
-      <c r="DJ3" s="1"/>
-      <c r="DK3" s="1"/>
-      <c r="DL3" s="1"/>
-      <c r="DM3" s="1"/>
-      <c r="DN3" s="1"/>
-      <c r="DO3" s="1"/>
-      <c r="DP3" s="1"/>
-      <c r="DQ3" s="1"/>
-      <c r="DR3" s="1"/>
-      <c r="DS3" s="1"/>
-      <c r="DT3" s="1"/>
-      <c r="DU3" s="1"/>
-      <c r="DV3" s="1"/>
-      <c r="DW3" s="1"/>
-      <c r="DX3" s="1"/>
-      <c r="DY3" s="1"/>
-      <c r="DZ3" s="1"/>
-      <c r="EA3" s="1"/>
-      <c r="EB3" s="1"/>
-      <c r="EC3" s="1"/>
-      <c r="ED3" s="1"/>
-      <c r="EE3" s="1"/>
-      <c r="EF3" s="1"/>
-      <c r="EG3" s="1"/>
-      <c r="EH3" s="1"/>
-      <c r="EI3" s="1"/>
-      <c r="EJ3" s="1"/>
-      <c r="EK3" s="1"/>
-      <c r="EL3" s="1"/>
-      <c r="EM3" s="1"/>
-      <c r="EN3" s="1"/>
-      <c r="EO3" s="1"/>
-      <c r="EP3" s="1"/>
-      <c r="EQ3" s="1"/>
-      <c r="ER3" s="1"/>
-      <c r="ES3" s="1"/>
-      <c r="ET3" s="1"/>
-      <c r="EU3" s="1"/>
-      <c r="EV3" s="1"/>
-      <c r="EW3" s="1"/>
-      <c r="EX3" s="1"/>
-      <c r="EY3" s="1"/>
-      <c r="EZ3" s="1"/>
-      <c r="FA3" s="1"/>
-      <c r="FB3" s="1"/>
-      <c r="FC3" s="1"/>
-      <c r="FD3" s="1"/>
-      <c r="FE3" s="1"/>
-      <c r="FF3" s="1"/>
-      <c r="FG3" s="1"/>
-      <c r="FH3" s="1"/>
-      <c r="FI3" s="1"/>
-      <c r="FJ3" s="1"/>
-      <c r="FK3" s="1"/>
-      <c r="FL3" s="1"/>
-      <c r="FM3" s="1"/>
-      <c r="FN3" s="1"/>
-      <c r="FO3" s="1"/>
-      <c r="FP3" s="1"/>
-      <c r="FQ3" s="1"/>
-      <c r="FR3" s="1"/>
-      <c r="FS3" s="1"/>
-      <c r="FT3" s="1"/>
-      <c r="FU3" s="1"/>
-      <c r="FV3" s="1"/>
-      <c r="FW3" s="1"/>
-      <c r="FX3" s="1"/>
-      <c r="FY3" s="1"/>
-      <c r="FZ3" s="1"/>
-      <c r="GA3" s="1"/>
-      <c r="GB3" s="1"/>
-      <c r="GC3" s="1"/>
-      <c r="GD3" s="1"/>
-      <c r="GE3" s="1"/>
-      <c r="GF3" s="1"/>
-      <c r="GG3" s="1"/>
-      <c r="GH3" s="1"/>
-      <c r="GI3" s="1"/>
-      <c r="GJ3" s="1"/>
-      <c r="GK3" s="1"/>
-      <c r="GL3" s="1"/>
-      <c r="GM3" s="1"/>
-      <c r="GN3" s="1"/>
-      <c r="GO3" s="1"/>
-      <c r="GP3" s="1"/>
-      <c r="GQ3" s="1"/>
-      <c r="GR3" s="1"/>
-      <c r="GS3" s="1"/>
-      <c r="GT3" s="1"/>
-      <c r="GU3" s="1"/>
-      <c r="GV3" s="1"/>
-      <c r="GW3" s="1"/>
-      <c r="GX3" s="1"/>
-      <c r="GY3" s="1"/>
-      <c r="GZ3" s="1"/>
-      <c r="HA3" s="1"/>
-      <c r="HB3" s="1"/>
-      <c r="HC3" s="1"/>
-      <c r="HD3" s="1"/>
-      <c r="HE3" s="1"/>
-      <c r="HF3" s="1"/>
-      <c r="HG3" s="1"/>
-      <c r="HH3" s="1"/>
-      <c r="HI3" s="1"/>
-      <c r="HJ3" s="1"/>
-      <c r="HK3" s="1"/>
-      <c r="HL3" s="1"/>
-      <c r="HM3" s="1"/>
-      <c r="HN3" s="1"/>
-      <c r="HO3" s="1"/>
-      <c r="HP3" s="1"/>
-      <c r="HQ3" s="1"/>
-      <c r="HR3" s="1"/>
-      <c r="HS3" s="1"/>
-      <c r="HT3" s="1"/>
-      <c r="HU3" s="1"/>
-      <c r="HV3" s="1"/>
-      <c r="HW3" s="1"/>
-      <c r="HX3" s="1"/>
-      <c r="HY3" s="1"/>
-      <c r="HZ3" s="1"/>
-      <c r="IA3" s="1"/>
-      <c r="IB3" s="1"/>
-      <c r="IC3" s="1"/>
-      <c r="ID3" s="1"/>
-      <c r="IE3" s="1"/>
-      <c r="IF3" s="1"/>
-      <c r="IG3" s="1"/>
-      <c r="IH3" s="1"/>
-      <c r="II3" s="1"/>
-      <c r="IJ3" s="1"/>
-      <c r="IK3" s="1"/>
-      <c r="IL3" s="1"/>
-      <c r="IM3" s="1"/>
-      <c r="IN3" s="1"/>
-      <c r="IO3" s="1"/>
-      <c r="IP3" s="1"/>
-      <c r="IQ3" s="1"/>
-      <c r="IR3" s="1"/>
-      <c r="IS3" s="1"/>
-      <c r="IT3" s="1"/>
-      <c r="IU3" s="1"/>
-      <c r="IV3" s="1"/>
-    </row>
-    <row r="4" spans="1:256" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="19" t="s">
-        <v>410</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>411</v>
-      </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-      <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
-      <c r="AC4" s="1"/>
-      <c r="AD4" s="1"/>
-      <c r="AE4" s="1"/>
-      <c r="AF4" s="1"/>
-      <c r="AG4" s="1"/>
-      <c r="AH4" s="1"/>
-      <c r="AI4" s="1"/>
-      <c r="AJ4" s="1"/>
-      <c r="AK4" s="1"/>
-      <c r="AL4" s="1"/>
-      <c r="AM4" s="1"/>
-      <c r="AN4" s="1"/>
-      <c r="AO4" s="1"/>
-      <c r="AP4" s="1"/>
-      <c r="AQ4" s="1"/>
-      <c r="AR4" s="1"/>
-      <c r="AS4" s="1"/>
-      <c r="AT4" s="1"/>
-      <c r="AU4" s="1"/>
-      <c r="AV4" s="1"/>
-      <c r="AW4" s="1"/>
-      <c r="AX4" s="1"/>
-      <c r="AY4" s="1"/>
-      <c r="AZ4" s="1"/>
-      <c r="BA4" s="1"/>
-      <c r="BB4" s="1"/>
-      <c r="BC4" s="1"/>
-      <c r="BD4" s="1"/>
-      <c r="BE4" s="1"/>
-      <c r="BF4" s="1"/>
-      <c r="BG4" s="1"/>
-      <c r="BH4" s="1"/>
-      <c r="BI4" s="1"/>
-      <c r="BJ4" s="1"/>
-      <c r="BK4" s="1"/>
-      <c r="BL4" s="1"/>
-      <c r="BM4" s="1"/>
-      <c r="BN4" s="1"/>
-      <c r="BO4" s="1"/>
-      <c r="BP4" s="1"/>
-      <c r="BQ4" s="1"/>
-      <c r="BR4" s="1"/>
-      <c r="BS4" s="1"/>
-      <c r="BT4" s="1"/>
-      <c r="BU4" s="1"/>
-      <c r="BV4" s="1"/>
-      <c r="BW4" s="1"/>
-      <c r="BX4" s="1"/>
-      <c r="BY4" s="1"/>
-      <c r="BZ4" s="1"/>
-      <c r="CA4" s="1"/>
-      <c r="CB4" s="1"/>
-      <c r="CC4" s="1"/>
-      <c r="CD4" s="1"/>
-      <c r="CE4" s="1"/>
-      <c r="CF4" s="1"/>
-      <c r="CG4" s="1"/>
-      <c r="CH4" s="1"/>
-      <c r="CI4" s="1"/>
-      <c r="CJ4" s="1"/>
-      <c r="CK4" s="1"/>
-      <c r="CL4" s="1"/>
-      <c r="CM4" s="1"/>
-      <c r="CN4" s="1"/>
-      <c r="CO4" s="1"/>
-      <c r="CP4" s="1"/>
-      <c r="CQ4" s="1"/>
-      <c r="CR4" s="1"/>
-      <c r="CS4" s="1"/>
-      <c r="CT4" s="1"/>
-      <c r="CU4" s="1"/>
-      <c r="CV4" s="1"/>
-      <c r="CW4" s="1"/>
-      <c r="CX4" s="1"/>
-      <c r="CY4" s="1"/>
-      <c r="CZ4" s="1"/>
-      <c r="DA4" s="1"/>
-      <c r="DB4" s="1"/>
-      <c r="DC4" s="1"/>
-      <c r="DD4" s="1"/>
-      <c r="DE4" s="1"/>
-      <c r="DF4" s="1"/>
-      <c r="DG4" s="1"/>
-      <c r="DH4" s="1"/>
-      <c r="DI4" s="1"/>
-      <c r="DJ4" s="1"/>
-      <c r="DK4" s="1"/>
-      <c r="DL4" s="1"/>
-      <c r="DM4" s="1"/>
-      <c r="DN4" s="1"/>
-      <c r="DO4" s="1"/>
-      <c r="DP4" s="1"/>
-      <c r="DQ4" s="1"/>
-      <c r="DR4" s="1"/>
-      <c r="DS4" s="1"/>
-      <c r="DT4" s="1"/>
-      <c r="DU4" s="1"/>
-      <c r="DV4" s="1"/>
-      <c r="DW4" s="1"/>
-      <c r="DX4" s="1"/>
-      <c r="DY4" s="1"/>
-      <c r="DZ4" s="1"/>
-      <c r="EA4" s="1"/>
-      <c r="EB4" s="1"/>
-      <c r="EC4" s="1"/>
-      <c r="ED4" s="1"/>
-      <c r="EE4" s="1"/>
-      <c r="EF4" s="1"/>
-      <c r="EG4" s="1"/>
-      <c r="EH4" s="1"/>
-      <c r="EI4" s="1"/>
-      <c r="EJ4" s="1"/>
-      <c r="EK4" s="1"/>
-      <c r="EL4" s="1"/>
-      <c r="EM4" s="1"/>
-      <c r="EN4" s="1"/>
-      <c r="EO4" s="1"/>
-      <c r="EP4" s="1"/>
-      <c r="EQ4" s="1"/>
-      <c r="ER4" s="1"/>
-      <c r="ES4" s="1"/>
-      <c r="ET4" s="1"/>
-      <c r="EU4" s="1"/>
-      <c r="EV4" s="1"/>
-      <c r="EW4" s="1"/>
-      <c r="EX4" s="1"/>
-      <c r="EY4" s="1"/>
-      <c r="EZ4" s="1"/>
-      <c r="FA4" s="1"/>
-      <c r="FB4" s="1"/>
-      <c r="FC4" s="1"/>
-      <c r="FD4" s="1"/>
-      <c r="FE4" s="1"/>
-      <c r="FF4" s="1"/>
-      <c r="FG4" s="1"/>
-      <c r="FH4" s="1"/>
-      <c r="FI4" s="1"/>
-      <c r="FJ4" s="1"/>
-      <c r="FK4" s="1"/>
-      <c r="FL4" s="1"/>
-      <c r="FM4" s="1"/>
-      <c r="FN4" s="1"/>
-      <c r="FO4" s="1"/>
-      <c r="FP4" s="1"/>
-      <c r="FQ4" s="1"/>
-      <c r="FR4" s="1"/>
-      <c r="FS4" s="1"/>
-      <c r="FT4" s="1"/>
-      <c r="FU4" s="1"/>
-      <c r="FV4" s="1"/>
-      <c r="FW4" s="1"/>
-      <c r="FX4" s="1"/>
-      <c r="FY4" s="1"/>
-      <c r="FZ4" s="1"/>
-      <c r="GA4" s="1"/>
-      <c r="GB4" s="1"/>
-      <c r="GC4" s="1"/>
-      <c r="GD4" s="1"/>
-      <c r="GE4" s="1"/>
-      <c r="GF4" s="1"/>
-      <c r="GG4" s="1"/>
-      <c r="GH4" s="1"/>
-      <c r="GI4" s="1"/>
-      <c r="GJ4" s="1"/>
-      <c r="GK4" s="1"/>
-      <c r="GL4" s="1"/>
-      <c r="GM4" s="1"/>
-      <c r="GN4" s="1"/>
-      <c r="GO4" s="1"/>
-      <c r="GP4" s="1"/>
-      <c r="GQ4" s="1"/>
-      <c r="GR4" s="1"/>
-      <c r="GS4" s="1"/>
-      <c r="GT4" s="1"/>
-      <c r="GU4" s="1"/>
-      <c r="GV4" s="1"/>
-      <c r="GW4" s="1"/>
-      <c r="GX4" s="1"/>
-      <c r="GY4" s="1"/>
-      <c r="GZ4" s="1"/>
-      <c r="HA4" s="1"/>
-      <c r="HB4" s="1"/>
-      <c r="HC4" s="1"/>
-      <c r="HD4" s="1"/>
-      <c r="HE4" s="1"/>
-      <c r="HF4" s="1"/>
-      <c r="HG4" s="1"/>
-      <c r="HH4" s="1"/>
-      <c r="HI4" s="1"/>
-      <c r="HJ4" s="1"/>
-      <c r="HK4" s="1"/>
-      <c r="HL4" s="1"/>
-      <c r="HM4" s="1"/>
-      <c r="HN4" s="1"/>
-      <c r="HO4" s="1"/>
-      <c r="HP4" s="1"/>
-      <c r="HQ4" s="1"/>
-      <c r="HR4" s="1"/>
-      <c r="HS4" s="1"/>
-      <c r="HT4" s="1"/>
-      <c r="HU4" s="1"/>
-      <c r="HV4" s="1"/>
-      <c r="HW4" s="1"/>
-      <c r="HX4" s="1"/>
-      <c r="HY4" s="1"/>
-      <c r="HZ4" s="1"/>
-      <c r="IA4" s="1"/>
-      <c r="IB4" s="1"/>
-      <c r="IC4" s="1"/>
-      <c r="ID4" s="1"/>
-      <c r="IE4" s="1"/>
-      <c r="IF4" s="1"/>
-      <c r="IG4" s="1"/>
-      <c r="IH4" s="1"/>
-      <c r="II4" s="1"/>
-      <c r="IJ4" s="1"/>
-      <c r="IK4" s="1"/>
-      <c r="IL4" s="1"/>
-      <c r="IM4" s="1"/>
-      <c r="IN4" s="1"/>
-      <c r="IO4" s="1"/>
-      <c r="IP4" s="1"/>
-      <c r="IQ4" s="1"/>
-      <c r="IR4" s="1"/>
-      <c r="IS4" s="1"/>
-      <c r="IT4" s="1"/>
-      <c r="IU4" s="1"/>
-      <c r="IV4" s="1"/>
-    </row>
-    <row r="5" spans="1:256" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="19" t="s">
-        <v>419</v>
-      </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
-      <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
-      <c r="AC5" s="1"/>
-      <c r="AD5" s="1"/>
-      <c r="AE5" s="1"/>
-      <c r="AF5" s="1"/>
-      <c r="AG5" s="1"/>
-      <c r="AH5" s="1"/>
-      <c r="AI5" s="1"/>
-      <c r="AJ5" s="1"/>
-      <c r="AK5" s="1"/>
-      <c r="AL5" s="1"/>
-      <c r="AM5" s="1"/>
-      <c r="AN5" s="1"/>
-      <c r="AO5" s="1"/>
-      <c r="AP5" s="1"/>
-      <c r="AQ5" s="1"/>
-      <c r="AR5" s="1"/>
-      <c r="AS5" s="1"/>
-      <c r="AT5" s="1"/>
-      <c r="AU5" s="1"/>
-      <c r="AV5" s="1"/>
-      <c r="AW5" s="1"/>
-      <c r="AX5" s="1"/>
-      <c r="AY5" s="1"/>
-      <c r="AZ5" s="1"/>
-      <c r="BA5" s="1"/>
-      <c r="BB5" s="1"/>
-      <c r="BC5" s="1"/>
-      <c r="BD5" s="1"/>
-      <c r="BE5" s="1"/>
-      <c r="BF5" s="1"/>
-      <c r="BG5" s="1"/>
-      <c r="BH5" s="1"/>
-      <c r="BI5" s="1"/>
-      <c r="BJ5" s="1"/>
-      <c r="BK5" s="1"/>
-      <c r="BL5" s="1"/>
-      <c r="BM5" s="1"/>
-      <c r="BN5" s="1"/>
-      <c r="BO5" s="1"/>
-      <c r="BP5" s="1"/>
-      <c r="BQ5" s="1"/>
-      <c r="BR5" s="1"/>
-      <c r="BS5" s="1"/>
-      <c r="BT5" s="1"/>
-      <c r="BU5" s="1"/>
-      <c r="BV5" s="1"/>
-      <c r="BW5" s="1"/>
-      <c r="BX5" s="1"/>
-      <c r="BY5" s="1"/>
-      <c r="BZ5" s="1"/>
-      <c r="CA5" s="1"/>
-      <c r="CB5" s="1"/>
-      <c r="CC5" s="1"/>
-      <c r="CD5" s="1"/>
-      <c r="CE5" s="1"/>
-      <c r="CF5" s="1"/>
-      <c r="CG5" s="1"/>
-      <c r="CH5" s="1"/>
-      <c r="CI5" s="1"/>
-      <c r="CJ5" s="1"/>
-      <c r="CK5" s="1"/>
-      <c r="CL5" s="1"/>
-      <c r="CM5" s="1"/>
-      <c r="CN5" s="1"/>
-      <c r="CO5" s="1"/>
-      <c r="CP5" s="1"/>
-      <c r="CQ5" s="1"/>
-      <c r="CR5" s="1"/>
-      <c r="CS5" s="1"/>
-      <c r="CT5" s="1"/>
-      <c r="CU5" s="1"/>
-      <c r="CV5" s="1"/>
-      <c r="CW5" s="1"/>
-      <c r="CX5" s="1"/>
-      <c r="CY5" s="1"/>
-      <c r="CZ5" s="1"/>
-      <c r="DA5" s="1"/>
-      <c r="DB5" s="1"/>
-      <c r="DC5" s="1"/>
-      <c r="DD5" s="1"/>
-      <c r="DE5" s="1"/>
-      <c r="DF5" s="1"/>
-      <c r="DG5" s="1"/>
-      <c r="DH5" s="1"/>
-      <c r="DI5" s="1"/>
-      <c r="DJ5" s="1"/>
-      <c r="DK5" s="1"/>
-      <c r="DL5" s="1"/>
-      <c r="DM5" s="1"/>
-      <c r="DN5" s="1"/>
-      <c r="DO5" s="1"/>
-      <c r="DP5" s="1"/>
-      <c r="DQ5" s="1"/>
-      <c r="DR5" s="1"/>
-      <c r="DS5" s="1"/>
-      <c r="DT5" s="1"/>
-      <c r="DU5" s="1"/>
-      <c r="DV5" s="1"/>
-      <c r="DW5" s="1"/>
-      <c r="DX5" s="1"/>
-      <c r="DY5" s="1"/>
-      <c r="DZ5" s="1"/>
-      <c r="EA5" s="1"/>
-      <c r="EB5" s="1"/>
-      <c r="EC5" s="1"/>
-      <c r="ED5" s="1"/>
-      <c r="EE5" s="1"/>
-      <c r="EF5" s="1"/>
-      <c r="EG5" s="1"/>
-      <c r="EH5" s="1"/>
-      <c r="EI5" s="1"/>
-      <c r="EJ5" s="1"/>
-      <c r="EK5" s="1"/>
-      <c r="EL5" s="1"/>
-      <c r="EM5" s="1"/>
-      <c r="EN5" s="1"/>
-      <c r="EO5" s="1"/>
-      <c r="EP5" s="1"/>
-      <c r="EQ5" s="1"/>
-      <c r="ER5" s="1"/>
-      <c r="ES5" s="1"/>
-      <c r="ET5" s="1"/>
-      <c r="EU5" s="1"/>
-      <c r="EV5" s="1"/>
-      <c r="EW5" s="1"/>
-      <c r="EX5" s="1"/>
-      <c r="EY5" s="1"/>
-      <c r="EZ5" s="1"/>
-      <c r="FA5" s="1"/>
-      <c r="FB5" s="1"/>
-      <c r="FC5" s="1"/>
-      <c r="FD5" s="1"/>
-      <c r="FE5" s="1"/>
-      <c r="FF5" s="1"/>
-      <c r="FG5" s="1"/>
-      <c r="FH5" s="1"/>
-      <c r="FI5" s="1"/>
-      <c r="FJ5" s="1"/>
-      <c r="FK5" s="1"/>
-      <c r="FL5" s="1"/>
-      <c r="FM5" s="1"/>
-      <c r="FN5" s="1"/>
-      <c r="FO5" s="1"/>
-      <c r="FP5" s="1"/>
-      <c r="FQ5" s="1"/>
-      <c r="FR5" s="1"/>
-      <c r="FS5" s="1"/>
-      <c r="FT5" s="1"/>
-      <c r="FU5" s="1"/>
-      <c r="FV5" s="1"/>
-      <c r="FW5" s="1"/>
-      <c r="FX5" s="1"/>
-      <c r="FY5" s="1"/>
-      <c r="FZ5" s="1"/>
-      <c r="GA5" s="1"/>
-      <c r="GB5" s="1"/>
-      <c r="GC5" s="1"/>
-      <c r="GD5" s="1"/>
-      <c r="GE5" s="1"/>
-      <c r="GF5" s="1"/>
-      <c r="GG5" s="1"/>
-      <c r="GH5" s="1"/>
-      <c r="GI5" s="1"/>
-      <c r="GJ5" s="1"/>
-      <c r="GK5" s="1"/>
-      <c r="GL5" s="1"/>
-      <c r="GM5" s="1"/>
-      <c r="GN5" s="1"/>
-      <c r="GO5" s="1"/>
-      <c r="GP5" s="1"/>
-      <c r="GQ5" s="1"/>
-      <c r="GR5" s="1"/>
-      <c r="GS5" s="1"/>
-      <c r="GT5" s="1"/>
-      <c r="GU5" s="1"/>
-      <c r="GV5" s="1"/>
-      <c r="GW5" s="1"/>
-      <c r="GX5" s="1"/>
-      <c r="GY5" s="1"/>
-      <c r="GZ5" s="1"/>
-      <c r="HA5" s="1"/>
-      <c r="HB5" s="1"/>
-      <c r="HC5" s="1"/>
-      <c r="HD5" s="1"/>
-      <c r="HE5" s="1"/>
-      <c r="HF5" s="1"/>
-      <c r="HG5" s="1"/>
-      <c r="HH5" s="1"/>
-      <c r="HI5" s="1"/>
-      <c r="HJ5" s="1"/>
-      <c r="HK5" s="1"/>
-      <c r="HL5" s="1"/>
-      <c r="HM5" s="1"/>
-      <c r="HN5" s="1"/>
-      <c r="HO5" s="1"/>
-      <c r="HP5" s="1"/>
-      <c r="HQ5" s="1"/>
-      <c r="HR5" s="1"/>
-      <c r="HS5" s="1"/>
-      <c r="HT5" s="1"/>
-      <c r="HU5" s="1"/>
-      <c r="HV5" s="1"/>
-      <c r="HW5" s="1"/>
-      <c r="HX5" s="1"/>
-      <c r="HY5" s="1"/>
-      <c r="HZ5" s="1"/>
-      <c r="IA5" s="1"/>
-      <c r="IB5" s="1"/>
-      <c r="IC5" s="1"/>
-      <c r="ID5" s="1"/>
-      <c r="IE5" s="1"/>
-      <c r="IF5" s="1"/>
-      <c r="IG5" s="1"/>
-      <c r="IH5" s="1"/>
-      <c r="II5" s="1"/>
-      <c r="IJ5" s="1"/>
-      <c r="IK5" s="1"/>
-      <c r="IL5" s="1"/>
-      <c r="IM5" s="1"/>
-      <c r="IN5" s="1"/>
-      <c r="IO5" s="1"/>
-      <c r="IP5" s="1"/>
-      <c r="IQ5" s="1"/>
-      <c r="IR5" s="1"/>
-      <c r="IS5" s="1"/>
-      <c r="IT5" s="1"/>
-      <c r="IU5" s="1"/>
-      <c r="IV5" s="1"/>
-    </row>
-    <row r="6" spans="1:256" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>416</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>418</v>
-      </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
-      <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
-      <c r="AC6" s="1"/>
-      <c r="AD6" s="1"/>
-      <c r="AE6" s="1"/>
-      <c r="AF6" s="1"/>
-      <c r="AG6" s="1"/>
-      <c r="AH6" s="1"/>
-      <c r="AI6" s="1"/>
-      <c r="AJ6" s="1"/>
-      <c r="AK6" s="1"/>
-      <c r="AL6" s="1"/>
-      <c r="AM6" s="1"/>
-      <c r="AN6" s="1"/>
-      <c r="AO6" s="1"/>
-      <c r="AP6" s="1"/>
-      <c r="AQ6" s="1"/>
-      <c r="AR6" s="1"/>
-      <c r="AS6" s="1"/>
-      <c r="AT6" s="1"/>
-      <c r="AU6" s="1"/>
-      <c r="AV6" s="1"/>
-      <c r="AW6" s="1"/>
-      <c r="AX6" s="1"/>
-      <c r="AY6" s="1"/>
-      <c r="AZ6" s="1"/>
-      <c r="BA6" s="1"/>
-      <c r="BB6" s="1"/>
-      <c r="BC6" s="1"/>
-      <c r="BD6" s="1"/>
-      <c r="BE6" s="1"/>
-      <c r="BF6" s="1"/>
-      <c r="BG6" s="1"/>
-      <c r="BH6" s="1"/>
-      <c r="BI6" s="1"/>
-      <c r="BJ6" s="1"/>
-      <c r="BK6" s="1"/>
-      <c r="BL6" s="1"/>
-      <c r="BM6" s="1"/>
-      <c r="BN6" s="1"/>
-      <c r="BO6" s="1"/>
-      <c r="BP6" s="1"/>
-      <c r="BQ6" s="1"/>
-      <c r="BR6" s="1"/>
-      <c r="BS6" s="1"/>
-      <c r="BT6" s="1"/>
-      <c r="BU6" s="1"/>
-      <c r="BV6" s="1"/>
-      <c r="BW6" s="1"/>
-      <c r="BX6" s="1"/>
-      <c r="BY6" s="1"/>
-      <c r="BZ6" s="1"/>
-      <c r="CA6" s="1"/>
-      <c r="CB6" s="1"/>
-      <c r="CC6" s="1"/>
-      <c r="CD6" s="1"/>
-      <c r="CE6" s="1"/>
-      <c r="CF6" s="1"/>
-      <c r="CG6" s="1"/>
-      <c r="CH6" s="1"/>
-      <c r="CI6" s="1"/>
-      <c r="CJ6" s="1"/>
-      <c r="CK6" s="1"/>
-      <c r="CL6" s="1"/>
-      <c r="CM6" s="1"/>
-      <c r="CN6" s="1"/>
-      <c r="CO6" s="1"/>
-      <c r="CP6" s="1"/>
-      <c r="CQ6" s="1"/>
-      <c r="CR6" s="1"/>
-      <c r="CS6" s="1"/>
-      <c r="CT6" s="1"/>
-      <c r="CU6" s="1"/>
-      <c r="CV6" s="1"/>
-      <c r="CW6" s="1"/>
-      <c r="CX6" s="1"/>
-      <c r="CY6" s="1"/>
-      <c r="CZ6" s="1"/>
-      <c r="DA6" s="1"/>
-      <c r="DB6" s="1"/>
-      <c r="DC6" s="1"/>
-      <c r="DD6" s="1"/>
-      <c r="DE6" s="1"/>
-      <c r="DF6" s="1"/>
-      <c r="DG6" s="1"/>
-      <c r="DH6" s="1"/>
-      <c r="DI6" s="1"/>
-      <c r="DJ6" s="1"/>
-      <c r="DK6" s="1"/>
-      <c r="DL6" s="1"/>
-      <c r="DM6" s="1"/>
-      <c r="DN6" s="1"/>
-      <c r="DO6" s="1"/>
-      <c r="DP6" s="1"/>
-      <c r="DQ6" s="1"/>
-      <c r="DR6" s="1"/>
-      <c r="DS6" s="1"/>
-      <c r="DT6" s="1"/>
-      <c r="DU6" s="1"/>
-      <c r="DV6" s="1"/>
-      <c r="DW6" s="1"/>
-      <c r="DX6" s="1"/>
-      <c r="DY6" s="1"/>
-      <c r="DZ6" s="1"/>
-      <c r="EA6" s="1"/>
-      <c r="EB6" s="1"/>
-      <c r="EC6" s="1"/>
-      <c r="ED6" s="1"/>
-      <c r="EE6" s="1"/>
-      <c r="EF6" s="1"/>
-      <c r="EG6" s="1"/>
-      <c r="EH6" s="1"/>
-      <c r="EI6" s="1"/>
-      <c r="EJ6" s="1"/>
-      <c r="EK6" s="1"/>
-      <c r="EL6" s="1"/>
-      <c r="EM6" s="1"/>
-      <c r="EN6" s="1"/>
-      <c r="EO6" s="1"/>
-      <c r="EP6" s="1"/>
-      <c r="EQ6" s="1"/>
-      <c r="ER6" s="1"/>
-      <c r="ES6" s="1"/>
-      <c r="ET6" s="1"/>
-      <c r="EU6" s="1"/>
-      <c r="EV6" s="1"/>
-      <c r="EW6" s="1"/>
-      <c r="EX6" s="1"/>
-      <c r="EY6" s="1"/>
-      <c r="EZ6" s="1"/>
-      <c r="FA6" s="1"/>
-      <c r="FB6" s="1"/>
-      <c r="FC6" s="1"/>
-      <c r="FD6" s="1"/>
-      <c r="FE6" s="1"/>
-      <c r="FF6" s="1"/>
-      <c r="FG6" s="1"/>
-      <c r="FH6" s="1"/>
-      <c r="FI6" s="1"/>
-      <c r="FJ6" s="1"/>
-      <c r="FK6" s="1"/>
-      <c r="FL6" s="1"/>
-      <c r="FM6" s="1"/>
-      <c r="FN6" s="1"/>
-      <c r="FO6" s="1"/>
-      <c r="FP6" s="1"/>
-      <c r="FQ6" s="1"/>
-      <c r="FR6" s="1"/>
-      <c r="FS6" s="1"/>
-      <c r="FT6" s="1"/>
-      <c r="FU6" s="1"/>
-      <c r="FV6" s="1"/>
-      <c r="FW6" s="1"/>
-      <c r="FX6" s="1"/>
-      <c r="FY6" s="1"/>
-      <c r="FZ6" s="1"/>
-      <c r="GA6" s="1"/>
-      <c r="GB6" s="1"/>
-      <c r="GC6" s="1"/>
-      <c r="GD6" s="1"/>
-      <c r="GE6" s="1"/>
-      <c r="GF6" s="1"/>
-      <c r="GG6" s="1"/>
-      <c r="GH6" s="1"/>
-      <c r="GI6" s="1"/>
-      <c r="GJ6" s="1"/>
-      <c r="GK6" s="1"/>
-      <c r="GL6" s="1"/>
-      <c r="GM6" s="1"/>
-      <c r="GN6" s="1"/>
-      <c r="GO6" s="1"/>
-      <c r="GP6" s="1"/>
-      <c r="GQ6" s="1"/>
-      <c r="GR6" s="1"/>
-      <c r="GS6" s="1"/>
-      <c r="GT6" s="1"/>
-      <c r="GU6" s="1"/>
-      <c r="GV6" s="1"/>
-      <c r="GW6" s="1"/>
-      <c r="GX6" s="1"/>
-      <c r="GY6" s="1"/>
-      <c r="GZ6" s="1"/>
-      <c r="HA6" s="1"/>
-      <c r="HB6" s="1"/>
-      <c r="HC6" s="1"/>
-      <c r="HD6" s="1"/>
-      <c r="HE6" s="1"/>
-      <c r="HF6" s="1"/>
-      <c r="HG6" s="1"/>
-      <c r="HH6" s="1"/>
-      <c r="HI6" s="1"/>
-      <c r="HJ6" s="1"/>
-      <c r="HK6" s="1"/>
-      <c r="HL6" s="1"/>
-      <c r="HM6" s="1"/>
-      <c r="HN6" s="1"/>
-      <c r="HO6" s="1"/>
-      <c r="HP6" s="1"/>
-      <c r="HQ6" s="1"/>
-      <c r="HR6" s="1"/>
-      <c r="HS6" s="1"/>
-      <c r="HT6" s="1"/>
-      <c r="HU6" s="1"/>
-      <c r="HV6" s="1"/>
-      <c r="HW6" s="1"/>
-      <c r="HX6" s="1"/>
-      <c r="HY6" s="1"/>
-      <c r="HZ6" s="1"/>
-      <c r="IA6" s="1"/>
-      <c r="IB6" s="1"/>
-      <c r="IC6" s="1"/>
-      <c r="ID6" s="1"/>
-      <c r="IE6" s="1"/>
-      <c r="IF6" s="1"/>
-      <c r="IG6" s="1"/>
-      <c r="IH6" s="1"/>
-      <c r="II6" s="1"/>
-      <c r="IJ6" s="1"/>
-      <c r="IK6" s="1"/>
-      <c r="IL6" s="1"/>
-      <c r="IM6" s="1"/>
-      <c r="IN6" s="1"/>
-      <c r="IO6" s="1"/>
-      <c r="IP6" s="1"/>
-      <c r="IQ6" s="1"/>
-      <c r="IR6" s="1"/>
-      <c r="IS6" s="1"/>
-      <c r="IT6" s="1"/>
-      <c r="IU6" s="1"/>
-      <c r="IV6" s="1"/>
-    </row>
-    <row r="7" spans="1:256" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>417</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>422</v>
-      </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
-      <c r="W7" s="1"/>
-      <c r="X7" s="1"/>
-      <c r="Y7" s="1"/>
-      <c r="Z7" s="1"/>
-      <c r="AA7" s="1"/>
-      <c r="AB7" s="1"/>
-      <c r="AC7" s="1"/>
-      <c r="AD7" s="1"/>
-      <c r="AE7" s="1"/>
-      <c r="AF7" s="1"/>
-      <c r="AG7" s="1"/>
-      <c r="AH7" s="1"/>
-      <c r="AI7" s="1"/>
-      <c r="AJ7" s="1"/>
-      <c r="AK7" s="1"/>
-      <c r="AL7" s="1"/>
-      <c r="AM7" s="1"/>
-      <c r="AN7" s="1"/>
-      <c r="AO7" s="1"/>
-      <c r="AP7" s="1"/>
-      <c r="AQ7" s="1"/>
-      <c r="AR7" s="1"/>
-      <c r="AS7" s="1"/>
-      <c r="AT7" s="1"/>
-      <c r="AU7" s="1"/>
-      <c r="AV7" s="1"/>
-      <c r="AW7" s="1"/>
-      <c r="AX7" s="1"/>
-      <c r="AY7" s="1"/>
-      <c r="AZ7" s="1"/>
-      <c r="BA7" s="1"/>
-      <c r="BB7" s="1"/>
-      <c r="BC7" s="1"/>
-      <c r="BD7" s="1"/>
-      <c r="BE7" s="1"/>
-      <c r="BF7" s="1"/>
-      <c r="BG7" s="1"/>
-      <c r="BH7" s="1"/>
-      <c r="BI7" s="1"/>
-      <c r="BJ7" s="1"/>
-      <c r="BK7" s="1"/>
-      <c r="BL7" s="1"/>
-      <c r="BM7" s="1"/>
-      <c r="BN7" s="1"/>
-      <c r="BO7" s="1"/>
-      <c r="BP7" s="1"/>
-      <c r="BQ7" s="1"/>
-      <c r="BR7" s="1"/>
-      <c r="BS7" s="1"/>
-      <c r="BT7" s="1"/>
-      <c r="BU7" s="1"/>
-      <c r="BV7" s="1"/>
-      <c r="BW7" s="1"/>
-      <c r="BX7" s="1"/>
-      <c r="BY7" s="1"/>
-      <c r="BZ7" s="1"/>
-      <c r="CA7" s="1"/>
-      <c r="CB7" s="1"/>
-      <c r="CC7" s="1"/>
-      <c r="CD7" s="1"/>
-      <c r="CE7" s="1"/>
-      <c r="CF7" s="1"/>
-      <c r="CG7" s="1"/>
-      <c r="CH7" s="1"/>
-      <c r="CI7" s="1"/>
-      <c r="CJ7" s="1"/>
-      <c r="CK7" s="1"/>
-      <c r="CL7" s="1"/>
-      <c r="CM7" s="1"/>
-      <c r="CN7" s="1"/>
-      <c r="CO7" s="1"/>
-      <c r="CP7" s="1"/>
-      <c r="CQ7" s="1"/>
-      <c r="CR7" s="1"/>
-      <c r="CS7" s="1"/>
-      <c r="CT7" s="1"/>
-      <c r="CU7" s="1"/>
-      <c r="CV7" s="1"/>
-      <c r="CW7" s="1"/>
-      <c r="CX7" s="1"/>
-      <c r="CY7" s="1"/>
-      <c r="CZ7" s="1"/>
-      <c r="DA7" s="1"/>
-      <c r="DB7" s="1"/>
-      <c r="DC7" s="1"/>
-      <c r="DD7" s="1"/>
-      <c r="DE7" s="1"/>
-      <c r="DF7" s="1"/>
-      <c r="DG7" s="1"/>
-      <c r="DH7" s="1"/>
-      <c r="DI7" s="1"/>
-      <c r="DJ7" s="1"/>
-      <c r="DK7" s="1"/>
-      <c r="DL7" s="1"/>
-      <c r="DM7" s="1"/>
-      <c r="DN7" s="1"/>
-      <c r="DO7" s="1"/>
-      <c r="DP7" s="1"/>
-      <c r="DQ7" s="1"/>
-      <c r="DR7" s="1"/>
-      <c r="DS7" s="1"/>
-      <c r="DT7" s="1"/>
-      <c r="DU7" s="1"/>
-      <c r="DV7" s="1"/>
-      <c r="DW7" s="1"/>
-      <c r="DX7" s="1"/>
-      <c r="DY7" s="1"/>
-      <c r="DZ7" s="1"/>
-      <c r="EA7" s="1"/>
-      <c r="EB7" s="1"/>
-      <c r="EC7" s="1"/>
-      <c r="ED7" s="1"/>
-      <c r="EE7" s="1"/>
-      <c r="EF7" s="1"/>
-      <c r="EG7" s="1"/>
-      <c r="EH7" s="1"/>
-      <c r="EI7" s="1"/>
-      <c r="EJ7" s="1"/>
-      <c r="EK7" s="1"/>
-      <c r="EL7" s="1"/>
-      <c r="EM7" s="1"/>
-      <c r="EN7" s="1"/>
-      <c r="EO7" s="1"/>
-      <c r="EP7" s="1"/>
-      <c r="EQ7" s="1"/>
-      <c r="ER7" s="1"/>
-      <c r="ES7" s="1"/>
-      <c r="ET7" s="1"/>
-      <c r="EU7" s="1"/>
-      <c r="EV7" s="1"/>
-      <c r="EW7" s="1"/>
-      <c r="EX7" s="1"/>
-      <c r="EY7" s="1"/>
-      <c r="EZ7" s="1"/>
-      <c r="FA7" s="1"/>
-      <c r="FB7" s="1"/>
-      <c r="FC7" s="1"/>
-      <c r="FD7" s="1"/>
-      <c r="FE7" s="1"/>
-      <c r="FF7" s="1"/>
-      <c r="FG7" s="1"/>
-      <c r="FH7" s="1"/>
-      <c r="FI7" s="1"/>
-      <c r="FJ7" s="1"/>
-      <c r="FK7" s="1"/>
-      <c r="FL7" s="1"/>
-      <c r="FM7" s="1"/>
-      <c r="FN7" s="1"/>
-      <c r="FO7" s="1"/>
-      <c r="FP7" s="1"/>
-      <c r="FQ7" s="1"/>
-      <c r="FR7" s="1"/>
-      <c r="FS7" s="1"/>
-      <c r="FT7" s="1"/>
-      <c r="FU7" s="1"/>
-      <c r="FV7" s="1"/>
-      <c r="FW7" s="1"/>
-      <c r="FX7" s="1"/>
-      <c r="FY7" s="1"/>
-      <c r="FZ7" s="1"/>
-      <c r="GA7" s="1"/>
-      <c r="GB7" s="1"/>
-      <c r="GC7" s="1"/>
-      <c r="GD7" s="1"/>
-      <c r="GE7" s="1"/>
-      <c r="GF7" s="1"/>
-      <c r="GG7" s="1"/>
-      <c r="GH7" s="1"/>
-      <c r="GI7" s="1"/>
-      <c r="GJ7" s="1"/>
-      <c r="GK7" s="1"/>
-      <c r="GL7" s="1"/>
-      <c r="GM7" s="1"/>
-      <c r="GN7" s="1"/>
-      <c r="GO7" s="1"/>
-      <c r="GP7" s="1"/>
-      <c r="GQ7" s="1"/>
-      <c r="GR7" s="1"/>
-      <c r="GS7" s="1"/>
-      <c r="GT7" s="1"/>
-      <c r="GU7" s="1"/>
-      <c r="GV7" s="1"/>
-      <c r="GW7" s="1"/>
-      <c r="GX7" s="1"/>
-      <c r="GY7" s="1"/>
-      <c r="GZ7" s="1"/>
-      <c r="HA7" s="1"/>
-      <c r="HB7" s="1"/>
-      <c r="HC7" s="1"/>
-      <c r="HD7" s="1"/>
-      <c r="HE7" s="1"/>
-      <c r="HF7" s="1"/>
-      <c r="HG7" s="1"/>
-      <c r="HH7" s="1"/>
-      <c r="HI7" s="1"/>
-      <c r="HJ7" s="1"/>
-      <c r="HK7" s="1"/>
-      <c r="HL7" s="1"/>
-      <c r="HM7" s="1"/>
-      <c r="HN7" s="1"/>
-      <c r="HO7" s="1"/>
-      <c r="HP7" s="1"/>
-      <c r="HQ7" s="1"/>
-      <c r="HR7" s="1"/>
-      <c r="HS7" s="1"/>
-      <c r="HT7" s="1"/>
-      <c r="HU7" s="1"/>
-      <c r="HV7" s="1"/>
-      <c r="HW7" s="1"/>
-      <c r="HX7" s="1"/>
-      <c r="HY7" s="1"/>
-      <c r="HZ7" s="1"/>
-      <c r="IA7" s="1"/>
-      <c r="IB7" s="1"/>
-      <c r="IC7" s="1"/>
-      <c r="ID7" s="1"/>
-      <c r="IE7" s="1"/>
-      <c r="IF7" s="1"/>
-      <c r="IG7" s="1"/>
-      <c r="IH7" s="1"/>
-      <c r="II7" s="1"/>
-      <c r="IJ7" s="1"/>
-      <c r="IK7" s="1"/>
-      <c r="IL7" s="1"/>
-      <c r="IM7" s="1"/>
-      <c r="IN7" s="1"/>
-      <c r="IO7" s="1"/>
-      <c r="IP7" s="1"/>
-      <c r="IQ7" s="1"/>
-      <c r="IR7" s="1"/>
-      <c r="IS7" s="1"/>
-      <c r="IT7" s="1"/>
-      <c r="IU7" s="1"/>
-      <c r="IV7" s="1"/>
-    </row>
-    <row r="8" spans="1:256" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="25"/>
-      <c r="B8" s="16" t="s">
-        <v>412</v>
-      </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="19" t="s">
-        <v>352</v>
-      </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
-      <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
-      <c r="W8" s="1"/>
-      <c r="X8" s="1"/>
-      <c r="Y8" s="1"/>
-      <c r="Z8" s="1"/>
-      <c r="AA8" s="1"/>
-      <c r="AB8" s="1"/>
-      <c r="AC8" s="1"/>
-      <c r="AD8" s="1"/>
-      <c r="AE8" s="1"/>
-      <c r="AF8" s="1"/>
-      <c r="AG8" s="1"/>
-      <c r="AH8" s="1"/>
-      <c r="AI8" s="1"/>
-      <c r="AJ8" s="1"/>
-      <c r="AK8" s="1"/>
-      <c r="AL8" s="1"/>
-      <c r="AM8" s="1"/>
-      <c r="AN8" s="1"/>
-      <c r="AO8" s="1"/>
-      <c r="AP8" s="1"/>
-      <c r="AQ8" s="1"/>
-      <c r="AR8" s="1"/>
-      <c r="AS8" s="1"/>
-      <c r="AT8" s="1"/>
-      <c r="AU8" s="1"/>
-      <c r="AV8" s="1"/>
-      <c r="AW8" s="1"/>
-      <c r="AX8" s="1"/>
-      <c r="AY8" s="1"/>
-      <c r="AZ8" s="1"/>
-      <c r="BA8" s="1"/>
-      <c r="BB8" s="1"/>
-      <c r="BC8" s="1"/>
-      <c r="BD8" s="1"/>
-      <c r="BE8" s="1"/>
-      <c r="BF8" s="1"/>
-      <c r="BG8" s="1"/>
-      <c r="BH8" s="1"/>
-      <c r="BI8" s="1"/>
-      <c r="BJ8" s="1"/>
-      <c r="BK8" s="1"/>
-      <c r="BL8" s="1"/>
-      <c r="BM8" s="1"/>
-      <c r="BN8" s="1"/>
-      <c r="BO8" s="1"/>
-      <c r="BP8" s="1"/>
-      <c r="BQ8" s="1"/>
-      <c r="BR8" s="1"/>
-      <c r="BS8" s="1"/>
-      <c r="BT8" s="1"/>
-      <c r="BU8" s="1"/>
-      <c r="BV8" s="1"/>
-      <c r="BW8" s="1"/>
-      <c r="BX8" s="1"/>
-      <c r="BY8" s="1"/>
-      <c r="BZ8" s="1"/>
-      <c r="CA8" s="1"/>
-      <c r="CB8" s="1"/>
-      <c r="CC8" s="1"/>
-      <c r="CD8" s="1"/>
-      <c r="CE8" s="1"/>
-      <c r="CF8" s="1"/>
-      <c r="CG8" s="1"/>
-      <c r="CH8" s="1"/>
-      <c r="CI8" s="1"/>
-      <c r="CJ8" s="1"/>
-      <c r="CK8" s="1"/>
-      <c r="CL8" s="1"/>
-      <c r="CM8" s="1"/>
-      <c r="CN8" s="1"/>
-      <c r="CO8" s="1"/>
-      <c r="CP8" s="1"/>
-      <c r="CQ8" s="1"/>
-      <c r="CR8" s="1"/>
-      <c r="CS8" s="1"/>
-      <c r="CT8" s="1"/>
-      <c r="CU8" s="1"/>
-      <c r="CV8" s="1"/>
-      <c r="CW8" s="1"/>
-      <c r="CX8" s="1"/>
-      <c r="CY8" s="1"/>
-      <c r="CZ8" s="1"/>
-      <c r="DA8" s="1"/>
-      <c r="DB8" s="1"/>
-      <c r="DC8" s="1"/>
-      <c r="DD8" s="1"/>
-      <c r="DE8" s="1"/>
-      <c r="DF8" s="1"/>
-      <c r="DG8" s="1"/>
-      <c r="DH8" s="1"/>
-      <c r="DI8" s="1"/>
-      <c r="DJ8" s="1"/>
-      <c r="DK8" s="1"/>
-      <c r="DL8" s="1"/>
-      <c r="DM8" s="1"/>
-      <c r="DN8" s="1"/>
-      <c r="DO8" s="1"/>
-      <c r="DP8" s="1"/>
-      <c r="DQ8" s="1"/>
-      <c r="DR8" s="1"/>
-      <c r="DS8" s="1"/>
-      <c r="DT8" s="1"/>
-      <c r="DU8" s="1"/>
-      <c r="DV8" s="1"/>
-      <c r="DW8" s="1"/>
-      <c r="DX8" s="1"/>
-      <c r="DY8" s="1"/>
-      <c r="DZ8" s="1"/>
-      <c r="EA8" s="1"/>
-      <c r="EB8" s="1"/>
-      <c r="EC8" s="1"/>
-      <c r="ED8" s="1"/>
-      <c r="EE8" s="1"/>
-      <c r="EF8" s="1"/>
-      <c r="EG8" s="1"/>
-      <c r="EH8" s="1"/>
-      <c r="EI8" s="1"/>
-      <c r="EJ8" s="1"/>
-      <c r="EK8" s="1"/>
-      <c r="EL8" s="1"/>
-      <c r="EM8" s="1"/>
-      <c r="EN8" s="1"/>
-      <c r="EO8" s="1"/>
-      <c r="EP8" s="1"/>
-      <c r="EQ8" s="1"/>
-      <c r="ER8" s="1"/>
-      <c r="ES8" s="1"/>
-      <c r="ET8" s="1"/>
-      <c r="EU8" s="1"/>
-      <c r="EV8" s="1"/>
-      <c r="EW8" s="1"/>
-      <c r="EX8" s="1"/>
-      <c r="EY8" s="1"/>
-      <c r="EZ8" s="1"/>
-      <c r="FA8" s="1"/>
-      <c r="FB8" s="1"/>
-      <c r="FC8" s="1"/>
-      <c r="FD8" s="1"/>
-      <c r="FE8" s="1"/>
-      <c r="FF8" s="1"/>
-      <c r="FG8" s="1"/>
-      <c r="FH8" s="1"/>
-      <c r="FI8" s="1"/>
-      <c r="FJ8" s="1"/>
-      <c r="FK8" s="1"/>
-      <c r="FL8" s="1"/>
-      <c r="FM8" s="1"/>
-      <c r="FN8" s="1"/>
-      <c r="FO8" s="1"/>
-      <c r="FP8" s="1"/>
-      <c r="FQ8" s="1"/>
-      <c r="FR8" s="1"/>
-      <c r="FS8" s="1"/>
-      <c r="FT8" s="1"/>
-      <c r="FU8" s="1"/>
-      <c r="FV8" s="1"/>
-      <c r="FW8" s="1"/>
-      <c r="FX8" s="1"/>
-      <c r="FY8" s="1"/>
-      <c r="FZ8" s="1"/>
-      <c r="GA8" s="1"/>
-      <c r="GB8" s="1"/>
-      <c r="GC8" s="1"/>
-      <c r="GD8" s="1"/>
-      <c r="GE8" s="1"/>
-      <c r="GF8" s="1"/>
-      <c r="GG8" s="1"/>
-      <c r="GH8" s="1"/>
-      <c r="GI8" s="1"/>
-      <c r="GJ8" s="1"/>
-      <c r="GK8" s="1"/>
-      <c r="GL8" s="1"/>
-      <c r="GM8" s="1"/>
-      <c r="GN8" s="1"/>
-      <c r="GO8" s="1"/>
-      <c r="GP8" s="1"/>
-      <c r="GQ8" s="1"/>
-      <c r="GR8" s="1"/>
-      <c r="GS8" s="1"/>
-      <c r="GT8" s="1"/>
-      <c r="GU8" s="1"/>
-      <c r="GV8" s="1"/>
-      <c r="GW8" s="1"/>
-      <c r="GX8" s="1"/>
-      <c r="GY8" s="1"/>
-      <c r="GZ8" s="1"/>
-      <c r="HA8" s="1"/>
-      <c r="HB8" s="1"/>
-      <c r="HC8" s="1"/>
-      <c r="HD8" s="1"/>
-      <c r="HE8" s="1"/>
-      <c r="HF8" s="1"/>
-      <c r="HG8" s="1"/>
-      <c r="HH8" s="1"/>
-      <c r="HI8" s="1"/>
-      <c r="HJ8" s="1"/>
-      <c r="HK8" s="1"/>
-      <c r="HL8" s="1"/>
-      <c r="HM8" s="1"/>
-      <c r="HN8" s="1"/>
-      <c r="HO8" s="1"/>
-      <c r="HP8" s="1"/>
-      <c r="HQ8" s="1"/>
-      <c r="HR8" s="1"/>
-      <c r="HS8" s="1"/>
-      <c r="HT8" s="1"/>
-      <c r="HU8" s="1"/>
-      <c r="HV8" s="1"/>
-      <c r="HW8" s="1"/>
-      <c r="HX8" s="1"/>
-      <c r="HY8" s="1"/>
-      <c r="HZ8" s="1"/>
-      <c r="IA8" s="1"/>
-      <c r="IB8" s="1"/>
-      <c r="IC8" s="1"/>
-      <c r="ID8" s="1"/>
-      <c r="IE8" s="1"/>
-      <c r="IF8" s="1"/>
-      <c r="IG8" s="1"/>
-      <c r="IH8" s="1"/>
-      <c r="II8" s="1"/>
-      <c r="IJ8" s="1"/>
-      <c r="IK8" s="1"/>
-      <c r="IL8" s="1"/>
-      <c r="IM8" s="1"/>
-      <c r="IN8" s="1"/>
-      <c r="IO8" s="1"/>
-      <c r="IP8" s="1"/>
-      <c r="IQ8" s="1"/>
-      <c r="IR8" s="1"/>
-      <c r="IS8" s="1"/>
-      <c r="IT8" s="1"/>
-      <c r="IU8" s="1"/>
-      <c r="IV8" s="1"/>
-    </row>
-    <row r="9" spans="1:256" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="25"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="7" t="s">
-        <v>421</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>413</v>
-      </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
-      <c r="W9" s="1"/>
-      <c r="X9" s="1"/>
-      <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
-      <c r="AA9" s="1"/>
-      <c r="AB9" s="1"/>
-      <c r="AC9" s="1"/>
-      <c r="AD9" s="1"/>
-      <c r="AE9" s="1"/>
-      <c r="AF9" s="1"/>
-      <c r="AG9" s="1"/>
-      <c r="AH9" s="1"/>
-      <c r="AI9" s="1"/>
-      <c r="AJ9" s="1"/>
-      <c r="AK9" s="1"/>
-      <c r="AL9" s="1"/>
-      <c r="AM9" s="1"/>
-      <c r="AN9" s="1"/>
-      <c r="AO9" s="1"/>
-      <c r="AP9" s="1"/>
-      <c r="AQ9" s="1"/>
-      <c r="AR9" s="1"/>
-      <c r="AS9" s="1"/>
-      <c r="AT9" s="1"/>
-      <c r="AU9" s="1"/>
-      <c r="AV9" s="1"/>
-      <c r="AW9" s="1"/>
-      <c r="AX9" s="1"/>
-      <c r="AY9" s="1"/>
-      <c r="AZ9" s="1"/>
-      <c r="BA9" s="1"/>
-      <c r="BB9" s="1"/>
-      <c r="BC9" s="1"/>
-      <c r="BD9" s="1"/>
-      <c r="BE9" s="1"/>
-      <c r="BF9" s="1"/>
-      <c r="BG9" s="1"/>
-      <c r="BH9" s="1"/>
-      <c r="BI9" s="1"/>
-      <c r="BJ9" s="1"/>
-      <c r="BK9" s="1"/>
-      <c r="BL9" s="1"/>
-      <c r="BM9" s="1"/>
-      <c r="BN9" s="1"/>
-      <c r="BO9" s="1"/>
-      <c r="BP9" s="1"/>
-      <c r="BQ9" s="1"/>
-      <c r="BR9" s="1"/>
-      <c r="BS9" s="1"/>
-      <c r="BT9" s="1"/>
-      <c r="BU9" s="1"/>
-      <c r="BV9" s="1"/>
-      <c r="BW9" s="1"/>
-      <c r="BX9" s="1"/>
-      <c r="BY9" s="1"/>
-      <c r="BZ9" s="1"/>
-      <c r="CA9" s="1"/>
-      <c r="CB9" s="1"/>
-      <c r="CC9" s="1"/>
-      <c r="CD9" s="1"/>
-      <c r="CE9" s="1"/>
-      <c r="CF9" s="1"/>
-      <c r="CG9" s="1"/>
-      <c r="CH9" s="1"/>
-      <c r="CI9" s="1"/>
-      <c r="CJ9" s="1"/>
-      <c r="CK9" s="1"/>
-      <c r="CL9" s="1"/>
-      <c r="CM9" s="1"/>
-      <c r="CN9" s="1"/>
-      <c r="CO9" s="1"/>
-      <c r="CP9" s="1"/>
-      <c r="CQ9" s="1"/>
-      <c r="CR9" s="1"/>
-      <c r="CS9" s="1"/>
-      <c r="CT9" s="1"/>
-      <c r="CU9" s="1"/>
-      <c r="CV9" s="1"/>
-      <c r="CW9" s="1"/>
-      <c r="CX9" s="1"/>
-      <c r="CY9" s="1"/>
-      <c r="CZ9" s="1"/>
-      <c r="DA9" s="1"/>
-      <c r="DB9" s="1"/>
-      <c r="DC9" s="1"/>
-      <c r="DD9" s="1"/>
-      <c r="DE9" s="1"/>
-      <c r="DF9" s="1"/>
-      <c r="DG9" s="1"/>
-      <c r="DH9" s="1"/>
-      <c r="DI9" s="1"/>
-      <c r="DJ9" s="1"/>
-      <c r="DK9" s="1"/>
-      <c r="DL9" s="1"/>
-      <c r="DM9" s="1"/>
-      <c r="DN9" s="1"/>
-      <c r="DO9" s="1"/>
-      <c r="DP9" s="1"/>
-      <c r="DQ9" s="1"/>
-      <c r="DR9" s="1"/>
-      <c r="DS9" s="1"/>
-      <c r="DT9" s="1"/>
-      <c r="DU9" s="1"/>
-      <c r="DV9" s="1"/>
-      <c r="DW9" s="1"/>
-      <c r="DX9" s="1"/>
-      <c r="DY9" s="1"/>
-      <c r="DZ9" s="1"/>
-      <c r="EA9" s="1"/>
-      <c r="EB9" s="1"/>
-      <c r="EC9" s="1"/>
-      <c r="ED9" s="1"/>
-      <c r="EE9" s="1"/>
-      <c r="EF9" s="1"/>
-      <c r="EG9" s="1"/>
-      <c r="EH9" s="1"/>
-      <c r="EI9" s="1"/>
-      <c r="EJ9" s="1"/>
-      <c r="EK9" s="1"/>
-      <c r="EL9" s="1"/>
-      <c r="EM9" s="1"/>
-      <c r="EN9" s="1"/>
-      <c r="EO9" s="1"/>
-      <c r="EP9" s="1"/>
-      <c r="EQ9" s="1"/>
-      <c r="ER9" s="1"/>
-      <c r="ES9" s="1"/>
-      <c r="ET9" s="1"/>
-      <c r="EU9" s="1"/>
-      <c r="EV9" s="1"/>
-      <c r="EW9" s="1"/>
-      <c r="EX9" s="1"/>
-      <c r="EY9" s="1"/>
-      <c r="EZ9" s="1"/>
-      <c r="FA9" s="1"/>
-      <c r="FB9" s="1"/>
-      <c r="FC9" s="1"/>
-      <c r="FD9" s="1"/>
-      <c r="FE9" s="1"/>
-      <c r="FF9" s="1"/>
-      <c r="FG9" s="1"/>
-      <c r="FH9" s="1"/>
-      <c r="FI9" s="1"/>
-      <c r="FJ9" s="1"/>
-      <c r="FK9" s="1"/>
-      <c r="FL9" s="1"/>
-      <c r="FM9" s="1"/>
-      <c r="FN9" s="1"/>
-      <c r="FO9" s="1"/>
-      <c r="FP9" s="1"/>
-      <c r="FQ9" s="1"/>
-      <c r="FR9" s="1"/>
-      <c r="FS9" s="1"/>
-      <c r="FT9" s="1"/>
-      <c r="FU9" s="1"/>
-      <c r="FV9" s="1"/>
-      <c r="FW9" s="1"/>
-      <c r="FX9" s="1"/>
-      <c r="FY9" s="1"/>
-      <c r="FZ9" s="1"/>
-      <c r="GA9" s="1"/>
-      <c r="GB9" s="1"/>
-      <c r="GC9" s="1"/>
-      <c r="GD9" s="1"/>
-      <c r="GE9" s="1"/>
-      <c r="GF9" s="1"/>
-      <c r="GG9" s="1"/>
-      <c r="GH9" s="1"/>
-      <c r="GI9" s="1"/>
-      <c r="GJ9" s="1"/>
-      <c r="GK9" s="1"/>
-      <c r="GL9" s="1"/>
-      <c r="GM9" s="1"/>
-      <c r="GN9" s="1"/>
-      <c r="GO9" s="1"/>
-      <c r="GP9" s="1"/>
-      <c r="GQ9" s="1"/>
-      <c r="GR9" s="1"/>
-      <c r="GS9" s="1"/>
-      <c r="GT9" s="1"/>
-      <c r="GU9" s="1"/>
-      <c r="GV9" s="1"/>
-      <c r="GW9" s="1"/>
-      <c r="GX9" s="1"/>
-      <c r="GY9" s="1"/>
-      <c r="GZ9" s="1"/>
-      <c r="HA9" s="1"/>
-      <c r="HB9" s="1"/>
-      <c r="HC9" s="1"/>
-      <c r="HD9" s="1"/>
-      <c r="HE9" s="1"/>
-      <c r="HF9" s="1"/>
-      <c r="HG9" s="1"/>
-      <c r="HH9" s="1"/>
-      <c r="HI9" s="1"/>
-      <c r="HJ9" s="1"/>
-      <c r="HK9" s="1"/>
-      <c r="HL9" s="1"/>
-      <c r="HM9" s="1"/>
-      <c r="HN9" s="1"/>
-      <c r="HO9" s="1"/>
-      <c r="HP9" s="1"/>
-      <c r="HQ9" s="1"/>
-      <c r="HR9" s="1"/>
-      <c r="HS9" s="1"/>
-      <c r="HT9" s="1"/>
-      <c r="HU9" s="1"/>
-      <c r="HV9" s="1"/>
-      <c r="HW9" s="1"/>
-      <c r="HX9" s="1"/>
-      <c r="HY9" s="1"/>
-      <c r="HZ9" s="1"/>
-      <c r="IA9" s="1"/>
-      <c r="IB9" s="1"/>
-      <c r="IC9" s="1"/>
-      <c r="ID9" s="1"/>
-      <c r="IE9" s="1"/>
-      <c r="IF9" s="1"/>
-      <c r="IG9" s="1"/>
-      <c r="IH9" s="1"/>
-      <c r="II9" s="1"/>
-      <c r="IJ9" s="1"/>
-      <c r="IK9" s="1"/>
-      <c r="IL9" s="1"/>
-      <c r="IM9" s="1"/>
-      <c r="IN9" s="1"/>
-      <c r="IO9" s="1"/>
-      <c r="IP9" s="1"/>
-      <c r="IQ9" s="1"/>
-      <c r="IR9" s="1"/>
-      <c r="IS9" s="1"/>
-      <c r="IT9" s="1"/>
-      <c r="IU9" s="1"/>
-      <c r="IV9" s="1"/>
-    </row>
-    <row r="10" spans="1:256" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="25"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="7" t="s">
-        <v>414</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>415</v>
-      </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
-      <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
-      <c r="AA10" s="1"/>
-      <c r="AB10" s="1"/>
-      <c r="AC10" s="1"/>
-      <c r="AD10" s="1"/>
-      <c r="AE10" s="1"/>
-      <c r="AF10" s="1"/>
-      <c r="AG10" s="1"/>
-      <c r="AH10" s="1"/>
-      <c r="AI10" s="1"/>
-      <c r="AJ10" s="1"/>
-      <c r="AK10" s="1"/>
-      <c r="AL10" s="1"/>
-      <c r="AM10" s="1"/>
-      <c r="AN10" s="1"/>
-      <c r="AO10" s="1"/>
-      <c r="AP10" s="1"/>
-      <c r="AQ10" s="1"/>
-      <c r="AR10" s="1"/>
-      <c r="AS10" s="1"/>
-      <c r="AT10" s="1"/>
-      <c r="AU10" s="1"/>
-      <c r="AV10" s="1"/>
-      <c r="AW10" s="1"/>
-      <c r="AX10" s="1"/>
-      <c r="AY10" s="1"/>
-      <c r="AZ10" s="1"/>
-      <c r="BA10" s="1"/>
-      <c r="BB10" s="1"/>
-      <c r="BC10" s="1"/>
-      <c r="BD10" s="1"/>
-      <c r="BE10" s="1"/>
-      <c r="BF10" s="1"/>
-      <c r="BG10" s="1"/>
-      <c r="BH10" s="1"/>
-      <c r="BI10" s="1"/>
-      <c r="BJ10" s="1"/>
-      <c r="BK10" s="1"/>
-      <c r="BL10" s="1"/>
-      <c r="BM10" s="1"/>
-      <c r="BN10" s="1"/>
-      <c r="BO10" s="1"/>
-      <c r="BP10" s="1"/>
-      <c r="BQ10" s="1"/>
-      <c r="BR10" s="1"/>
-      <c r="BS10" s="1"/>
-      <c r="BT10" s="1"/>
-      <c r="BU10" s="1"/>
-      <c r="BV10" s="1"/>
-      <c r="BW10" s="1"/>
-      <c r="BX10" s="1"/>
-      <c r="BY10" s="1"/>
-      <c r="BZ10" s="1"/>
-      <c r="CA10" s="1"/>
-      <c r="CB10" s="1"/>
-      <c r="CC10" s="1"/>
-      <c r="CD10" s="1"/>
-      <c r="CE10" s="1"/>
-      <c r="CF10" s="1"/>
-      <c r="CG10" s="1"/>
-      <c r="CH10" s="1"/>
-      <c r="CI10" s="1"/>
-      <c r="CJ10" s="1"/>
-      <c r="CK10" s="1"/>
-      <c r="CL10" s="1"/>
-      <c r="CM10" s="1"/>
-      <c r="CN10" s="1"/>
-      <c r="CO10" s="1"/>
-      <c r="CP10" s="1"/>
-      <c r="CQ10" s="1"/>
-      <c r="CR10" s="1"/>
-      <c r="CS10" s="1"/>
-      <c r="CT10" s="1"/>
-      <c r="CU10" s="1"/>
-      <c r="CV10" s="1"/>
-      <c r="CW10" s="1"/>
-      <c r="CX10" s="1"/>
-      <c r="CY10" s="1"/>
-      <c r="CZ10" s="1"/>
-      <c r="DA10" s="1"/>
-      <c r="DB10" s="1"/>
-      <c r="DC10" s="1"/>
-      <c r="DD10" s="1"/>
-      <c r="DE10" s="1"/>
-      <c r="DF10" s="1"/>
-      <c r="DG10" s="1"/>
-      <c r="DH10" s="1"/>
-      <c r="DI10" s="1"/>
-      <c r="DJ10" s="1"/>
-      <c r="DK10" s="1"/>
-      <c r="DL10" s="1"/>
-      <c r="DM10" s="1"/>
-      <c r="DN10" s="1"/>
-      <c r="DO10" s="1"/>
-      <c r="DP10" s="1"/>
-      <c r="DQ10" s="1"/>
-      <c r="DR10" s="1"/>
-      <c r="DS10" s="1"/>
-      <c r="DT10" s="1"/>
-      <c r="DU10" s="1"/>
-      <c r="DV10" s="1"/>
-      <c r="DW10" s="1"/>
-      <c r="DX10" s="1"/>
-      <c r="DY10" s="1"/>
-      <c r="DZ10" s="1"/>
-      <c r="EA10" s="1"/>
-      <c r="EB10" s="1"/>
-      <c r="EC10" s="1"/>
-      <c r="ED10" s="1"/>
-      <c r="EE10" s="1"/>
-      <c r="EF10" s="1"/>
-      <c r="EG10" s="1"/>
-      <c r="EH10" s="1"/>
-      <c r="EI10" s="1"/>
-      <c r="EJ10" s="1"/>
-      <c r="EK10" s="1"/>
-      <c r="EL10" s="1"/>
-      <c r="EM10" s="1"/>
-      <c r="EN10" s="1"/>
-      <c r="EO10" s="1"/>
-      <c r="EP10" s="1"/>
-      <c r="EQ10" s="1"/>
-      <c r="ER10" s="1"/>
-      <c r="ES10" s="1"/>
-      <c r="ET10" s="1"/>
-      <c r="EU10" s="1"/>
-      <c r="EV10" s="1"/>
-      <c r="EW10" s="1"/>
-      <c r="EX10" s="1"/>
-      <c r="EY10" s="1"/>
-      <c r="EZ10" s="1"/>
-      <c r="FA10" s="1"/>
-      <c r="FB10" s="1"/>
-      <c r="FC10" s="1"/>
-      <c r="FD10" s="1"/>
-      <c r="FE10" s="1"/>
-      <c r="FF10" s="1"/>
-      <c r="FG10" s="1"/>
-      <c r="FH10" s="1"/>
-      <c r="FI10" s="1"/>
-      <c r="FJ10" s="1"/>
-      <c r="FK10" s="1"/>
-      <c r="FL10" s="1"/>
-      <c r="FM10" s="1"/>
-      <c r="FN10" s="1"/>
-      <c r="FO10" s="1"/>
-      <c r="FP10" s="1"/>
-      <c r="FQ10" s="1"/>
-      <c r="FR10" s="1"/>
-      <c r="FS10" s="1"/>
-      <c r="FT10" s="1"/>
-      <c r="FU10" s="1"/>
-      <c r="FV10" s="1"/>
-      <c r="FW10" s="1"/>
-      <c r="FX10" s="1"/>
-      <c r="FY10" s="1"/>
-      <c r="FZ10" s="1"/>
-      <c r="GA10" s="1"/>
-      <c r="GB10" s="1"/>
-      <c r="GC10" s="1"/>
-      <c r="GD10" s="1"/>
-      <c r="GE10" s="1"/>
-      <c r="GF10" s="1"/>
-      <c r="GG10" s="1"/>
-      <c r="GH10" s="1"/>
-      <c r="GI10" s="1"/>
-      <c r="GJ10" s="1"/>
-      <c r="GK10" s="1"/>
-      <c r="GL10" s="1"/>
-      <c r="GM10" s="1"/>
-      <c r="GN10" s="1"/>
-      <c r="GO10" s="1"/>
-      <c r="GP10" s="1"/>
-      <c r="GQ10" s="1"/>
-      <c r="GR10" s="1"/>
-      <c r="GS10" s="1"/>
-      <c r="GT10" s="1"/>
-      <c r="GU10" s="1"/>
-      <c r="GV10" s="1"/>
-      <c r="GW10" s="1"/>
-      <c r="GX10" s="1"/>
-      <c r="GY10" s="1"/>
-      <c r="GZ10" s="1"/>
-      <c r="HA10" s="1"/>
-      <c r="HB10" s="1"/>
-      <c r="HC10" s="1"/>
-      <c r="HD10" s="1"/>
-      <c r="HE10" s="1"/>
-      <c r="HF10" s="1"/>
-      <c r="HG10" s="1"/>
-      <c r="HH10" s="1"/>
-      <c r="HI10" s="1"/>
-      <c r="HJ10" s="1"/>
-      <c r="HK10" s="1"/>
-      <c r="HL10" s="1"/>
-      <c r="HM10" s="1"/>
-      <c r="HN10" s="1"/>
-      <c r="HO10" s="1"/>
-      <c r="HP10" s="1"/>
-      <c r="HQ10" s="1"/>
-      <c r="HR10" s="1"/>
-      <c r="HS10" s="1"/>
-      <c r="HT10" s="1"/>
-      <c r="HU10" s="1"/>
-      <c r="HV10" s="1"/>
-      <c r="HW10" s="1"/>
-      <c r="HX10" s="1"/>
-      <c r="HY10" s="1"/>
-      <c r="HZ10" s="1"/>
-      <c r="IA10" s="1"/>
-      <c r="IB10" s="1"/>
-      <c r="IC10" s="1"/>
-      <c r="ID10" s="1"/>
-      <c r="IE10" s="1"/>
-      <c r="IF10" s="1"/>
-      <c r="IG10" s="1"/>
-      <c r="IH10" s="1"/>
-      <c r="II10" s="1"/>
-      <c r="IJ10" s="1"/>
-      <c r="IK10" s="1"/>
-      <c r="IL10" s="1"/>
-      <c r="IM10" s="1"/>
-      <c r="IN10" s="1"/>
-      <c r="IO10" s="1"/>
-      <c r="IP10" s="1"/>
-      <c r="IQ10" s="1"/>
-      <c r="IR10" s="1"/>
-      <c r="IS10" s="1"/>
-      <c r="IT10" s="1"/>
-      <c r="IU10" s="1"/>
-      <c r="IV10" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Probing capability and child objectives
</commit_message>
<xml_diff>
--- a/mind_maps/malware_capabilities_descriptions.xlsx
+++ b/mind_maps/malware_capabilities_descriptions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="439">
   <si>
     <t>Capability</t>
   </si>
@@ -1283,6 +1283,54 @@
   </si>
   <si>
     <t>The 'send heartbeat data' value indicates that the malware instance is able to send heartbeat data to a command and control server, also commonly referred to as beaconing.</t>
+  </si>
+  <si>
+    <t>Probing</t>
+  </si>
+  <si>
+    <t>The 'probing' Capability indicates that the malware instance is able to probe its host system or network environment; most often this is done to support other Capabilities and their Objectives.</t>
+  </si>
+  <si>
+    <t>Probe Network Environment</t>
+  </si>
+  <si>
+    <t>The 'probe network environment' value indicates that the malware instance is able to probe the properties of its network environment, e.g. to determine whether it funnels traffic through a proxy.</t>
+  </si>
+  <si>
+    <t>Check for Internet Connectivity</t>
+  </si>
+  <si>
+    <t>The 'check for internet connectivity' value indicates that the malware instance is able to check whether the network environment in which it executes is connected to the internet.</t>
+  </si>
+  <si>
+    <t>Check for Firewall</t>
+  </si>
+  <si>
+    <t>The 'check for firewall' value indicates that the malware instance is able to check whether the network environment in which it executes contains a hardware or software firewall.</t>
+  </si>
+  <si>
+    <t>Check for Proxy</t>
+  </si>
+  <si>
+    <t>The 'check for proxy' value indicates that the malware instance is able to check whether the network environment in which it executes contains a hardware or software proxy.</t>
+  </si>
+  <si>
+    <t>Map Local Network</t>
+  </si>
+  <si>
+    <t>The 'map local network' value indicates that the malware instance is able to map the layout of the local network environment in which it executes.</t>
+  </si>
+  <si>
+    <t>Probe Host Configuration</t>
+  </si>
+  <si>
+    <t>The 'probe host configuration' value indicates that the malware instance is able to probe the configuration of the host system on which it executes.</t>
+  </si>
+  <si>
+    <t>Check Language</t>
+  </si>
+  <si>
+    <t>The 'check language' value indicates that the malware instance is able to check the language of the host system on which it executes.</t>
   </si>
 </sst>
 </file>
@@ -1299,12 +1347,14 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1872,10 +1922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV205"/>
+  <dimension ref="A1:IV213"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D104" sqref="D104"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.61328125" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -4984,6 +5034,118 @@
       <c r="E205" s="8"/>
       <c r="F205" s="11"/>
     </row>
+    <row r="206" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A206" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="B206" s="25"/>
+      <c r="C206" s="25"/>
+      <c r="D206" s="18" t="s">
+        <v>424</v>
+      </c>
+      <c r="E206" s="8"/>
+      <c r="F206" s="11"/>
+    </row>
+    <row r="207" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A207" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B207" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="C207" s="25"/>
+      <c r="D207" s="18" t="s">
+        <v>426</v>
+      </c>
+      <c r="E207" s="8"/>
+      <c r="F207" s="11"/>
+    </row>
+    <row r="208" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A208" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B208" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C208" s="7" t="s">
+        <v>427</v>
+      </c>
+      <c r="D208" s="18" t="s">
+        <v>428</v>
+      </c>
+      <c r="E208" s="8"/>
+      <c r="F208" s="11"/>
+    </row>
+    <row r="209" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A209" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B209" s="7"/>
+      <c r="C209" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="D209" s="18" t="s">
+        <v>430</v>
+      </c>
+      <c r="E209" s="8"/>
+      <c r="F209" s="11"/>
+    </row>
+    <row r="210" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A210" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B210" s="7"/>
+      <c r="C210" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="D210" s="18" t="s">
+        <v>432</v>
+      </c>
+      <c r="E210" s="8"/>
+      <c r="F210" s="11"/>
+    </row>
+    <row r="211" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A211" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B211" s="7"/>
+      <c r="C211" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="D211" s="18" t="s">
+        <v>434</v>
+      </c>
+      <c r="E211" s="8"/>
+      <c r="F211" s="11"/>
+    </row>
+    <row r="212" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A212" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B212" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="C212" s="25"/>
+      <c r="D212" s="18" t="s">
+        <v>436</v>
+      </c>
+      <c r="E212" s="8"/>
+      <c r="F212" s="11"/>
+    </row>
+    <row r="213" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A213" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B213" s="7"/>
+      <c r="C213" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="D213" s="18" t="s">
+        <v>438</v>
+      </c>
+      <c r="E213" s="8"/>
+      <c r="F213" s="11"/>
+    </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add new nodes under Persistence & annotations
</commit_message>
<xml_diff>
--- a/mind_maps/malware_capabilities_descriptions.xlsx
+++ b/mind_maps/malware_capabilities_descriptions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="96" windowWidth="15960" windowHeight="9576" tabRatio="543"/>
+    <workbookView xWindow="0" yWindow="156" windowWidth="15960" windowHeight="9516" tabRatio="543"/>
   </bookViews>
   <sheets>
     <sheet name="malware_capabilities" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="479">
   <si>
     <t>Capability</t>
   </si>
@@ -1193,9 +1193,6 @@
     <t>Receive Data from C2 Server</t>
   </si>
   <si>
-    <t>The 'execute remote command' value indicates that the malware instance is able to execute commands issued to it from a remote source such as a command and control server, for the purpose of controlling its behavior.</t>
-  </si>
-  <si>
     <t>Update Configuration</t>
   </si>
   <si>
@@ -1503,10 +1500,25 @@
     <t>Control Machine via Remote Command</t>
   </si>
   <si>
-    <t>The 'Control Machine via Remote Command' value indicates that the malware instance executes commands issued to it from a remote source, for the purpose of controlling the machine on which it is resident.</t>
+    <t>Control Malware via Remote Command</t>
   </si>
   <si>
-    <t>Control Malware via Remote Command</t>
+    <t>The 'control machine via remote command' value indicates that the malware instance executes commands issued to it from a remote source, for the purpose of controlling the machine on which it is resident.</t>
+  </si>
+  <si>
+    <t>The 'control malware via remote command' value indicates that the malware instance is able to execute commands issued to it from a remote source such as a command and control server, for the purpose of controlling its behavior.</t>
+  </si>
+  <si>
+    <t>Ensure Compatibility</t>
+  </si>
+  <si>
+    <t>The 'ensure compatibility' value indicates that the malware instance is able to manipulate or modify the system on which it executes to ensure that it is able to continue executing.</t>
+  </si>
+  <si>
+    <t>Limit Application Type/Version</t>
+  </si>
+  <si>
+    <t>The 'limit application type/version' value indicates that the malware instance is able to limit the type or version of an application that runs on a system in order to ensure that it is able to continue executing.</t>
   </si>
 </sst>
 </file>
@@ -2074,10 +2086,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IT239"/>
+  <dimension ref="A1:IT241"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D109" sqref="D109"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.61328125" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -2893,10 +2905,10 @@
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="24" t="s">
+        <v>439</v>
+      </c>
+      <c r="D5" s="14" t="s">
         <v>440</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>441</v>
       </c>
       <c r="E5" s="22"/>
       <c r="F5" s="22"/>
@@ -4471,10 +4483,10 @@
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="20" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
@@ -22355,14 +22367,16 @@
       <c r="IS78" s="22"/>
       <c r="IT78" s="22"/>
     </row>
-    <row r="79" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A79" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="B79" s="15"/>
+        <v>5</v>
+      </c>
+      <c r="B79" s="13" t="s">
+        <v>475</v>
+      </c>
       <c r="C79" s="15"/>
       <c r="D79" s="16" t="s">
-        <v>196</v>
+        <v>476</v>
       </c>
       <c r="E79" s="22"/>
       <c r="F79" s="22"/>
@@ -22620,11 +22634,13 @@
         <v>5</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="C80" s="15"/>
+        <v>5</v>
+      </c>
+      <c r="C80" s="13" t="s">
+        <v>477</v>
+      </c>
       <c r="D80" s="16" t="s">
-        <v>349</v>
+        <v>478</v>
       </c>
       <c r="E80" s="22"/>
       <c r="F80" s="22"/>
@@ -22877,18 +22893,14 @@
       <c r="IS80" s="22"/>
       <c r="IT80" s="22"/>
     </row>
-    <row r="81" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B81" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C81" s="13" t="s">
-        <v>86</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="B81" s="15"/>
+      <c r="C81" s="15"/>
       <c r="D81" s="16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E81" s="22"/>
       <c r="F81" s="22"/>
@@ -23146,11 +23158,11 @@
         <v>5</v>
       </c>
       <c r="B82" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C82" s="15"/>
       <c r="D82" s="16" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E82" s="22"/>
       <c r="F82" s="22"/>
@@ -23411,10 +23423,10 @@
         <v>5</v>
       </c>
       <c r="C83" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D83" s="16" t="s">
-        <v>89</v>
+        <v>197</v>
       </c>
       <c r="E83" s="22"/>
       <c r="F83" s="22"/>
@@ -23672,13 +23684,11 @@
         <v>5</v>
       </c>
       <c r="B84" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C84" s="13" t="s">
-        <v>90</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="C84" s="15"/>
       <c r="D84" s="16" t="s">
-        <v>91</v>
+        <v>350</v>
       </c>
       <c r="E84" s="22"/>
       <c r="F84" s="22"/>
@@ -23939,10 +23949,10 @@
         <v>5</v>
       </c>
       <c r="C85" s="13" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D85" s="16" t="s">
-        <v>351</v>
+        <v>89</v>
       </c>
       <c r="E85" s="22"/>
       <c r="F85" s="22"/>
@@ -24203,10 +24213,10 @@
         <v>5</v>
       </c>
       <c r="C86" s="13" t="s">
-        <v>367</v>
+        <v>90</v>
       </c>
       <c r="D86" s="16" t="s">
-        <v>366</v>
+        <v>91</v>
       </c>
       <c r="E86" s="22"/>
       <c r="F86" s="22"/>
@@ -24464,11 +24474,13 @@
         <v>5</v>
       </c>
       <c r="B87" s="13" t="s">
-        <v>368</v>
-      </c>
-      <c r="C87" s="15"/>
+        <v>5</v>
+      </c>
+      <c r="C87" s="13" t="s">
+        <v>92</v>
+      </c>
       <c r="D87" s="16" t="s">
-        <v>93</v>
+        <v>351</v>
       </c>
       <c r="E87" s="22"/>
       <c r="F87" s="22"/>
@@ -24729,10 +24741,10 @@
         <v>5</v>
       </c>
       <c r="C88" s="13" t="s">
-        <v>94</v>
+        <v>367</v>
       </c>
       <c r="D88" s="16" t="s">
-        <v>352</v>
+        <v>366</v>
       </c>
       <c r="E88" s="22"/>
       <c r="F88" s="22"/>
@@ -24985,18 +24997,16 @@
       <c r="IS88" s="22"/>
       <c r="IT88" s="22"/>
     </row>
-    <row r="89" spans="1:254" s="23" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A89" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B89" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C89" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="D89" s="14" t="s">
-        <v>96</v>
+        <v>368</v>
+      </c>
+      <c r="C89" s="15"/>
+      <c r="D89" s="16" t="s">
+        <v>93</v>
       </c>
       <c r="E89" s="22"/>
       <c r="F89" s="22"/>
@@ -25257,10 +25267,10 @@
         <v>5</v>
       </c>
       <c r="C90" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="D90" s="21" t="s">
-        <v>253</v>
+        <v>94</v>
+      </c>
+      <c r="D90" s="16" t="s">
+        <v>352</v>
       </c>
       <c r="E90" s="22"/>
       <c r="F90" s="22"/>
@@ -25513,16 +25523,18 @@
       <c r="IS90" s="22"/>
       <c r="IT90" s="22"/>
     </row>
-    <row r="91" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:254" s="23" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A91" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B91" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="C91" s="15"/>
-      <c r="D91" s="21" t="s">
-        <v>254</v>
+        <v>5</v>
+      </c>
+      <c r="C91" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D91" s="14" t="s">
+        <v>96</v>
       </c>
       <c r="E91" s="22"/>
       <c r="F91" s="22"/>
@@ -25783,10 +25795,10 @@
         <v>5</v>
       </c>
       <c r="C92" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D92" s="21" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E92" s="22"/>
       <c r="F92" s="22"/>
@@ -26039,18 +26051,16 @@
       <c r="IS92" s="22"/>
       <c r="IT92" s="22"/>
     </row>
-    <row r="93" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A93" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B93" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C93" s="13" t="s">
-        <v>100</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="C93" s="15"/>
       <c r="D93" s="21" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E93" s="22"/>
       <c r="F93" s="22"/>
@@ -26303,16 +26313,18 @@
       <c r="IS93" s="22"/>
       <c r="IT93" s="22"/>
     </row>
-    <row r="94" spans="1:254" s="23" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A94" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B94" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="C94" s="15"/>
+        <v>5</v>
+      </c>
+      <c r="C94" s="13" t="s">
+        <v>99</v>
+      </c>
       <c r="D94" s="21" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E94" s="22"/>
       <c r="F94" s="22"/>
@@ -26573,10 +26585,10 @@
         <v>5</v>
       </c>
       <c r="C95" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D95" s="21" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E95" s="22"/>
       <c r="F95" s="22"/>
@@ -26829,18 +26841,16 @@
       <c r="IS95" s="22"/>
       <c r="IT95" s="22"/>
     </row>
-    <row r="96" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:254" s="23" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A96" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B96" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C96" s="13" t="s">
-        <v>103</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="C96" s="15"/>
       <c r="D96" s="21" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E96" s="22"/>
       <c r="F96" s="22"/>
@@ -27093,7 +27103,7 @@
       <c r="IS96" s="22"/>
       <c r="IT96" s="22"/>
     </row>
-    <row r="97" spans="1:254" s="23" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A97" s="13" t="s">
         <v>5</v>
       </c>
@@ -27101,10 +27111,10 @@
         <v>5</v>
       </c>
       <c r="C97" s="13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D97" s="21" t="s">
-        <v>353</v>
+        <v>258</v>
       </c>
       <c r="E97" s="22"/>
       <c r="F97" s="22"/>
@@ -27365,10 +27375,10 @@
         <v>5</v>
       </c>
       <c r="C98" s="13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D98" s="21" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E98" s="22"/>
       <c r="F98" s="22"/>
@@ -27621,7 +27631,7 @@
       <c r="IS98" s="22"/>
       <c r="IT98" s="22"/>
     </row>
-    <row r="99" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:254" s="23" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A99" s="13" t="s">
         <v>5</v>
       </c>
@@ -27629,10 +27639,10 @@
         <v>5</v>
       </c>
       <c r="C99" s="13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D99" s="21" t="s">
-        <v>261</v>
+        <v>353</v>
       </c>
       <c r="E99" s="22"/>
       <c r="F99" s="22"/>
@@ -27885,14 +27895,18 @@
       <c r="IS99" s="22"/>
       <c r="IT99" s="22"/>
     </row>
-    <row r="100" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A100" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="B100" s="15"/>
-      <c r="C100" s="15"/>
-      <c r="D100" s="14" t="s">
-        <v>396</v>
+        <v>5</v>
+      </c>
+      <c r="B100" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C100" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="D100" s="21" t="s">
+        <v>260</v>
       </c>
       <c r="E100" s="22"/>
       <c r="F100" s="22"/>
@@ -28146,13 +28160,17 @@
       <c r="IT100" s="22"/>
     </row>
     <row r="101" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A101" s="13"/>
+      <c r="A101" s="13" t="s">
+        <v>5</v>
+      </c>
       <c r="B101" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="C101" s="13"/>
-      <c r="D101" s="14" t="s">
-        <v>354</v>
+        <v>5</v>
+      </c>
+      <c r="C101" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="D101" s="21" t="s">
+        <v>261</v>
       </c>
       <c r="E101" s="22"/>
       <c r="F101" s="22"/>
@@ -28405,14 +28423,14 @@
       <c r="IS101" s="22"/>
       <c r="IT101" s="22"/>
     </row>
-    <row r="102" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A102" s="13"/>
-      <c r="B102" s="13"/>
-      <c r="C102" s="14" t="s">
-        <v>437</v>
-      </c>
+    <row r="102" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A102" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B102" s="15"/>
+      <c r="C102" s="15"/>
       <c r="D102" s="14" t="s">
-        <v>421</v>
+        <v>395</v>
       </c>
       <c r="E102" s="22"/>
       <c r="F102" s="22"/>
@@ -28665,16 +28683,14 @@
       <c r="IS102" s="22"/>
       <c r="IT102" s="22"/>
     </row>
-    <row r="103" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A103" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B103" s="20" t="s">
-        <v>390</v>
-      </c>
-      <c r="C103" s="15"/>
+    <row r="103" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A103" s="13"/>
+      <c r="B103" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C103" s="13"/>
       <c r="D103" s="14" t="s">
-        <v>395</v>
+        <v>354</v>
       </c>
       <c r="E103" s="22"/>
       <c r="F103" s="22"/>
@@ -28928,17 +28944,13 @@
       <c r="IT103" s="22"/>
     </row>
     <row r="104" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A104" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B104" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C104" s="20" t="s">
-        <v>397</v>
+      <c r="A104" s="13"/>
+      <c r="B104" s="13"/>
+      <c r="C104" s="14" t="s">
+        <v>436</v>
       </c>
       <c r="D104" s="14" t="s">
-        <v>399</v>
+        <v>420</v>
       </c>
       <c r="E104" s="22"/>
       <c r="F104" s="22"/>
@@ -29191,18 +29203,16 @@
       <c r="IS104" s="22"/>
       <c r="IT104" s="22"/>
     </row>
-    <row r="105" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A105" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B105" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C105" s="20" t="s">
-        <v>398</v>
-      </c>
+      <c r="B105" s="20" t="s">
+        <v>390</v>
+      </c>
+      <c r="C105" s="15"/>
       <c r="D105" s="14" t="s">
-        <v>443</v>
+        <v>394</v>
       </c>
       <c r="E105" s="22"/>
       <c r="F105" s="22"/>
@@ -29456,13 +29466,17 @@
       <c r="IT105" s="22"/>
     </row>
     <row r="106" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A106" s="15"/>
-      <c r="B106" s="20"/>
-      <c r="C106" s="25" t="s">
-        <v>444</v>
+      <c r="A106" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B106" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C106" s="20" t="s">
+        <v>396</v>
       </c>
       <c r="D106" s="14" t="s">
-        <v>445</v>
+        <v>398</v>
       </c>
       <c r="E106" s="22"/>
       <c r="F106" s="22"/>
@@ -29716,13 +29730,17 @@
       <c r="IT106" s="22"/>
     </row>
     <row r="107" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A107" s="15"/>
-      <c r="B107" s="20" t="s">
-        <v>391</v>
-      </c>
-      <c r="C107" s="15"/>
+      <c r="A107" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B107" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C107" s="20" t="s">
+        <v>397</v>
+      </c>
       <c r="D107" s="14" t="s">
-        <v>340</v>
+        <v>442</v>
       </c>
       <c r="E107" s="22"/>
       <c r="F107" s="22"/>
@@ -29977,12 +29995,12 @@
     </row>
     <row r="108" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A108" s="15"/>
-      <c r="B108" s="15"/>
-      <c r="C108" s="13" t="s">
-        <v>474</v>
+      <c r="B108" s="20"/>
+      <c r="C108" s="25" t="s">
+        <v>443</v>
       </c>
       <c r="D108" s="14" t="s">
-        <v>392</v>
+        <v>444</v>
       </c>
       <c r="E108" s="22"/>
       <c r="F108" s="22"/>
@@ -30237,12 +30255,12 @@
     </row>
     <row r="109" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A109" s="15"/>
-      <c r="B109" s="15"/>
-      <c r="C109" s="13" t="s">
-        <v>393</v>
-      </c>
+      <c r="B109" s="20" t="s">
+        <v>391</v>
+      </c>
+      <c r="C109" s="15"/>
       <c r="D109" s="14" t="s">
-        <v>394</v>
+        <v>340</v>
       </c>
       <c r="E109" s="22"/>
       <c r="F109" s="22"/>
@@ -30495,14 +30513,14 @@
       <c r="IS109" s="22"/>
       <c r="IT109" s="22"/>
     </row>
-    <row r="110" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A110" s="15"/>
       <c r="B110" s="15"/>
-      <c r="C110" s="20" t="s">
-        <v>422</v>
+      <c r="C110" s="13" t="s">
+        <v>472</v>
       </c>
       <c r="D110" s="14" t="s">
-        <v>446</v>
+        <v>474</v>
       </c>
       <c r="E110" s="22"/>
       <c r="F110" s="22"/>
@@ -30756,13 +30774,13 @@
       <c r="IT110" s="22"/>
     </row>
     <row r="111" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A111" s="20" t="s">
-        <v>455</v>
-      </c>
+      <c r="A111" s="15"/>
       <c r="B111" s="15"/>
-      <c r="C111" s="15"/>
+      <c r="C111" s="13" t="s">
+        <v>392</v>
+      </c>
       <c r="D111" s="14" t="s">
-        <v>456</v>
+        <v>393</v>
       </c>
       <c r="E111" s="22"/>
       <c r="F111" s="22"/>
@@ -31015,14 +31033,14 @@
       <c r="IS111" s="22"/>
       <c r="IT111" s="22"/>
     </row>
-    <row r="112" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A112" s="13"/>
-      <c r="B112" s="20" t="s">
-        <v>451</v>
-      </c>
-      <c r="C112" s="13"/>
+    <row r="112" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A112" s="15"/>
+      <c r="B112" s="15"/>
+      <c r="C112" s="20" t="s">
+        <v>421</v>
+      </c>
       <c r="D112" s="14" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
       <c r="E112" s="22"/>
       <c r="F112" s="22"/>
@@ -31276,15 +31294,13 @@
       <c r="IT112" s="22"/>
     </row>
     <row r="113" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A113" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B113" s="20" t="s">
-        <v>457</v>
-      </c>
+      <c r="A113" s="20" t="s">
+        <v>454</v>
+      </c>
+      <c r="B113" s="15"/>
       <c r="C113" s="15"/>
       <c r="D113" s="14" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="E113" s="22"/>
       <c r="F113" s="22"/>
@@ -31538,17 +31554,13 @@
       <c r="IT113" s="22"/>
     </row>
     <row r="114" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A114" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B114" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C114" s="13" t="s">
-        <v>472</v>
-      </c>
+      <c r="A114" s="13"/>
+      <c r="B114" s="20" t="s">
+        <v>450</v>
+      </c>
+      <c r="C114" s="13"/>
       <c r="D114" s="14" t="s">
-        <v>473</v>
+        <v>452</v>
       </c>
       <c r="E114" s="22"/>
       <c r="F114" s="22"/>
@@ -31801,14 +31813,16 @@
       <c r="IS114" s="22"/>
       <c r="IT114" s="22"/>
     </row>
-    <row r="115" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A115" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="B115" s="15"/>
+    <row r="115" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A115" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B115" s="20" t="s">
+        <v>456</v>
+      </c>
       <c r="C115" s="15"/>
       <c r="D115" s="14" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="E115" s="22"/>
       <c r="F115" s="22"/>
@@ -32061,16 +32075,18 @@
       <c r="IS115" s="22"/>
       <c r="IT115" s="22"/>
     </row>
-    <row r="116" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A116" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B116" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="C116" s="15"/>
+        <v>5</v>
+      </c>
+      <c r="C116" s="13" t="s">
+        <v>471</v>
+      </c>
       <c r="D116" s="14" t="s">
-        <v>454</v>
+        <v>473</v>
       </c>
       <c r="E116" s="22"/>
       <c r="F116" s="22"/>
@@ -32324,15 +32340,13 @@
       <c r="IT116" s="22"/>
     </row>
     <row r="117" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A117" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B117" s="13" t="s">
-        <v>111</v>
-      </c>
+      <c r="A117" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="B117" s="15"/>
       <c r="C117" s="15"/>
       <c r="D117" s="14" t="s">
-        <v>262</v>
+        <v>457</v>
       </c>
       <c r="E117" s="22"/>
       <c r="F117" s="22"/>
@@ -32590,13 +32604,11 @@
         <v>5</v>
       </c>
       <c r="B118" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C118" s="13" t="s">
-        <v>112</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="C118" s="15"/>
       <c r="D118" s="14" t="s">
-        <v>263</v>
+        <v>453</v>
       </c>
       <c r="E118" s="22"/>
       <c r="F118" s="22"/>
@@ -32851,12 +32863,14 @@
     </row>
     <row r="119" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A119" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="B119" s="15"/>
+        <v>5</v>
+      </c>
+      <c r="B119" s="13" t="s">
+        <v>111</v>
+      </c>
       <c r="C119" s="15"/>
       <c r="D119" s="14" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E119" s="22"/>
       <c r="F119" s="22"/>
@@ -33109,16 +33123,18 @@
       <c r="IS119" s="22"/>
       <c r="IT119" s="22"/>
     </row>
-    <row r="120" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A120" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B120" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="C120" s="15"/>
+        <v>5</v>
+      </c>
+      <c r="C120" s="13" t="s">
+        <v>112</v>
+      </c>
       <c r="D120" s="14" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E120" s="22"/>
       <c r="F120" s="22"/>
@@ -33373,16 +33389,12 @@
     </row>
     <row r="121" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A121" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B121" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C121" s="13" t="s">
-        <v>115</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="B121" s="15"/>
+      <c r="C121" s="15"/>
       <c r="D121" s="14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E121" s="22"/>
       <c r="F121" s="22"/>
@@ -33640,11 +33652,11 @@
         <v>5</v>
       </c>
       <c r="B122" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C122" s="15"/>
       <c r="D122" s="14" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E122" s="22"/>
       <c r="F122" s="22"/>
@@ -33899,12 +33911,16 @@
     </row>
     <row r="123" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A123" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B123" s="15"/>
-      <c r="C123" s="15"/>
+        <v>5</v>
+      </c>
+      <c r="B123" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C123" s="13" t="s">
+        <v>115</v>
+      </c>
       <c r="D123" s="14" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="E123" s="22"/>
       <c r="F123" s="22"/>
@@ -34157,16 +34173,16 @@
       <c r="IS123" s="22"/>
       <c r="IT123" s="22"/>
     </row>
-    <row r="124" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A124" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B124" s="13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C124" s="15"/>
       <c r="D124" s="14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E124" s="22"/>
       <c r="F124" s="22"/>
@@ -34419,18 +34435,14 @@
       <c r="IS124" s="22"/>
       <c r="IT124" s="22"/>
     </row>
-    <row r="125" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A125" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B125" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C125" s="13" t="s">
-        <v>119</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="B125" s="15"/>
+      <c r="C125" s="15"/>
       <c r="D125" s="14" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="E125" s="22"/>
       <c r="F125" s="22"/>
@@ -34688,13 +34700,11 @@
         <v>5</v>
       </c>
       <c r="B126" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C126" s="13" t="s">
-        <v>120</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="C126" s="15"/>
       <c r="D126" s="14" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E126" s="22"/>
       <c r="F126" s="22"/>
@@ -34947,16 +34957,18 @@
       <c r="IS126" s="22"/>
       <c r="IT126" s="22"/>
     </row>
-    <row r="127" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A127" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B127" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="C127" s="15"/>
+        <v>5</v>
+      </c>
+      <c r="C127" s="13" t="s">
+        <v>119</v>
+      </c>
       <c r="D127" s="14" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E127" s="22"/>
       <c r="F127" s="22"/>
@@ -35217,10 +35229,10 @@
         <v>5</v>
       </c>
       <c r="C128" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D128" s="14" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E128" s="22"/>
       <c r="F128" s="22"/>
@@ -35473,18 +35485,16 @@
       <c r="IS128" s="22"/>
       <c r="IT128" s="22"/>
     </row>
-    <row r="129" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A129" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B129" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C129" s="13" t="s">
-        <v>123</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="C129" s="15"/>
       <c r="D129" s="14" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E129" s="22"/>
       <c r="F129" s="22"/>
@@ -35741,12 +35751,14 @@
       <c r="A130" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B130" s="20" t="s">
-        <v>275</v>
-      </c>
-      <c r="C130" s="15"/>
+      <c r="B130" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C130" s="13" t="s">
+        <v>122</v>
+      </c>
       <c r="D130" s="14" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E130" s="22"/>
       <c r="F130" s="22"/>
@@ -35999,7 +36011,7 @@
       <c r="IS130" s="22"/>
       <c r="IT130" s="22"/>
     </row>
-    <row r="131" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A131" s="13" t="s">
         <v>5</v>
       </c>
@@ -36007,10 +36019,10 @@
         <v>5</v>
       </c>
       <c r="C131" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D131" s="14" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="E131" s="22"/>
       <c r="F131" s="22"/>
@@ -36267,14 +36279,12 @@
       <c r="A132" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B132" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C132" s="13" t="s">
-        <v>125</v>
-      </c>
+      <c r="B132" s="20" t="s">
+        <v>275</v>
+      </c>
+      <c r="C132" s="15"/>
       <c r="D132" s="14" t="s">
-        <v>341</v>
+        <v>276</v>
       </c>
       <c r="E132" s="22"/>
       <c r="F132" s="22"/>
@@ -36535,10 +36545,10 @@
         <v>5</v>
       </c>
       <c r="C133" s="13" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D133" s="14" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E133" s="22"/>
       <c r="F133" s="22"/>
@@ -36791,7 +36801,7 @@
       <c r="IS133" s="22"/>
       <c r="IT133" s="22"/>
     </row>
-    <row r="134" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A134" s="13" t="s">
         <v>5</v>
       </c>
@@ -36799,10 +36809,10 @@
         <v>5</v>
       </c>
       <c r="C134" s="13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D134" s="14" t="s">
-        <v>279</v>
+        <v>341</v>
       </c>
       <c r="E134" s="22"/>
       <c r="F134" s="22"/>
@@ -37063,10 +37073,10 @@
         <v>5</v>
       </c>
       <c r="C135" s="13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D135" s="14" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="E135" s="22"/>
       <c r="F135" s="22"/>
@@ -37319,7 +37329,7 @@
       <c r="IS135" s="22"/>
       <c r="IT135" s="22"/>
     </row>
-    <row r="136" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A136" s="13" t="s">
         <v>5</v>
       </c>
@@ -37327,10 +37337,10 @@
         <v>5</v>
       </c>
       <c r="C136" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D136" s="14" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E136" s="22"/>
       <c r="F136" s="22"/>
@@ -37583,14 +37593,18 @@
       <c r="IS136" s="22"/>
       <c r="IT136" s="22"/>
     </row>
-    <row r="137" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A137" s="26" t="s">
-        <v>436</v>
-      </c>
-      <c r="B137" s="15"/>
-      <c r="C137" s="15"/>
+    <row r="137" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A137" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B137" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C137" s="13" t="s">
+        <v>128</v>
+      </c>
       <c r="D137" s="14" t="s">
-        <v>439</v>
+        <v>280</v>
       </c>
       <c r="E137" s="22"/>
       <c r="F137" s="22"/>
@@ -37843,16 +37857,18 @@
       <c r="IS137" s="22"/>
       <c r="IT137" s="22"/>
     </row>
-    <row r="138" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A138" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B138" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="C138" s="15"/>
+        <v>5</v>
+      </c>
+      <c r="C138" s="13" t="s">
+        <v>129</v>
+      </c>
       <c r="D138" s="14" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E138" s="22"/>
       <c r="F138" s="22"/>
@@ -38105,18 +38121,14 @@
       <c r="IS138" s="22"/>
       <c r="IT138" s="22"/>
     </row>
-    <row r="139" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A139" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B139" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C139" s="13" t="s">
-        <v>131</v>
-      </c>
+    <row r="139" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A139" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="B139" s="15"/>
+      <c r="C139" s="15"/>
       <c r="D139" s="14" t="s">
-        <v>283</v>
+        <v>438</v>
       </c>
       <c r="E139" s="22"/>
       <c r="F139" s="22"/>
@@ -38369,18 +38381,16 @@
       <c r="IS139" s="22"/>
       <c r="IT139" s="22"/>
     </row>
-    <row r="140" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A140" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B140" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C140" s="13" t="s">
-        <v>132</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="C140" s="15"/>
       <c r="D140" s="14" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E140" s="22"/>
       <c r="F140" s="22"/>
@@ -38634,13 +38644,17 @@
       <c r="IT140" s="22"/>
     </row>
     <row r="141" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A141" s="13"/>
-      <c r="B141" s="13"/>
-      <c r="C141" s="26" t="s">
-        <v>438</v>
+      <c r="A141" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B141" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C141" s="13" t="s">
+        <v>131</v>
       </c>
       <c r="D141" s="14" t="s">
-        <v>447</v>
+        <v>283</v>
       </c>
       <c r="E141" s="22"/>
       <c r="F141" s="22"/>
@@ -38898,11 +38912,13 @@
         <v>5</v>
       </c>
       <c r="B142" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="C142" s="15"/>
+        <v>5</v>
+      </c>
+      <c r="C142" s="13" t="s">
+        <v>132</v>
+      </c>
       <c r="D142" s="14" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E142" s="22"/>
       <c r="F142" s="22"/>
@@ -39156,17 +39172,13 @@
       <c r="IT142" s="22"/>
     </row>
     <row r="143" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A143" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B143" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C143" s="13" t="s">
-        <v>134</v>
+      <c r="A143" s="13"/>
+      <c r="B143" s="13"/>
+      <c r="C143" s="26" t="s">
+        <v>437</v>
       </c>
       <c r="D143" s="14" t="s">
-        <v>286</v>
+        <v>446</v>
       </c>
       <c r="E143" s="22"/>
       <c r="F143" s="22"/>
@@ -39424,13 +39436,11 @@
         <v>5</v>
       </c>
       <c r="B144" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C144" s="13" t="s">
-        <v>135</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="C144" s="15"/>
       <c r="D144" s="14" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E144" s="22"/>
       <c r="F144" s="22"/>
@@ -39683,14 +39693,18 @@
       <c r="IS144" s="22"/>
       <c r="IT144" s="22"/>
     </row>
-    <row r="145" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A145" s="13"/>
-      <c r="B145" s="20" t="s">
-        <v>468</v>
-      </c>
-      <c r="C145" s="13"/>
+    <row r="145" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A145" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B145" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C145" s="13" t="s">
+        <v>134</v>
+      </c>
       <c r="D145" s="14" t="s">
-        <v>469</v>
+        <v>286</v>
       </c>
       <c r="E145" s="22"/>
       <c r="F145" s="22"/>
@@ -39944,13 +39958,17 @@
       <c r="IT145" s="22"/>
     </row>
     <row r="146" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A146" s="13"/>
-      <c r="B146" s="20" t="s">
-        <v>418</v>
-      </c>
-      <c r="C146" s="13"/>
+      <c r="A146" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B146" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C146" s="13" t="s">
+        <v>135</v>
+      </c>
       <c r="D146" s="14" t="s">
-        <v>448</v>
+        <v>287</v>
       </c>
       <c r="E146" s="22"/>
       <c r="F146" s="22"/>
@@ -40203,14 +40221,14 @@
       <c r="IS146" s="22"/>
       <c r="IT146" s="22"/>
     </row>
-    <row r="147" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A147" s="13"/>
       <c r="B147" s="20" t="s">
-        <v>420</v>
-      </c>
-      <c r="C147" s="20"/>
+        <v>467</v>
+      </c>
+      <c r="C147" s="13"/>
       <c r="D147" s="14" t="s">
-        <v>449</v>
+        <v>468</v>
       </c>
       <c r="E147" s="22"/>
       <c r="F147" s="22"/>
@@ -40466,11 +40484,11 @@
     <row r="148" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A148" s="13"/>
       <c r="B148" s="20" t="s">
-        <v>429</v>
-      </c>
-      <c r="C148" s="20"/>
+        <v>417</v>
+      </c>
+      <c r="C148" s="13"/>
       <c r="D148" s="14" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="E148" s="22"/>
       <c r="F148" s="22"/>
@@ -40723,14 +40741,14 @@
       <c r="IS148" s="22"/>
       <c r="IT148" s="22"/>
     </row>
-    <row r="149" spans="1:254" s="23" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A149" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="B149" s="15"/>
-      <c r="C149" s="15"/>
+    <row r="149" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A149" s="13"/>
+      <c r="B149" s="20" t="s">
+        <v>419</v>
+      </c>
+      <c r="C149" s="20"/>
       <c r="D149" s="14" t="s">
-        <v>389</v>
+        <v>448</v>
       </c>
       <c r="E149" s="22"/>
       <c r="F149" s="22"/>
@@ -40984,15 +41002,13 @@
       <c r="IT149" s="22"/>
     </row>
     <row r="150" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A150" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B150" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="C150" s="15"/>
+      <c r="A150" s="13"/>
+      <c r="B150" s="20" t="s">
+        <v>428</v>
+      </c>
+      <c r="C150" s="20"/>
       <c r="D150" s="14" t="s">
-        <v>288</v>
+        <v>449</v>
       </c>
       <c r="E150" s="22"/>
       <c r="F150" s="22"/>
@@ -41245,18 +41261,14 @@
       <c r="IS150" s="22"/>
       <c r="IT150" s="22"/>
     </row>
-    <row r="151" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:254" s="23" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A151" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B151" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C151" s="13" t="s">
-        <v>138</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="B151" s="15"/>
+      <c r="C151" s="15"/>
       <c r="D151" s="14" t="s">
-        <v>289</v>
+        <v>389</v>
       </c>
       <c r="E151" s="22"/>
       <c r="F151" s="22"/>
@@ -41514,13 +41526,11 @@
         <v>5</v>
       </c>
       <c r="B152" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C152" s="20" t="s">
-        <v>139</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="C152" s="15"/>
       <c r="D152" s="14" t="s">
-        <v>355</v>
+        <v>288</v>
       </c>
       <c r="E152" s="22"/>
       <c r="F152" s="22"/>
@@ -41780,11 +41790,11 @@
       <c r="B153" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C153" s="20" t="s">
-        <v>430</v>
+      <c r="C153" s="13" t="s">
+        <v>138</v>
       </c>
       <c r="D153" s="14" t="s">
-        <v>432</v>
+        <v>289</v>
       </c>
       <c r="E153" s="22"/>
       <c r="F153" s="22"/>
@@ -42045,10 +42055,10 @@
         <v>5</v>
       </c>
       <c r="C154" s="20" t="s">
-        <v>431</v>
+        <v>139</v>
       </c>
       <c r="D154" s="14" t="s">
-        <v>290</v>
+        <v>355</v>
       </c>
       <c r="E154" s="22"/>
       <c r="F154" s="22"/>
@@ -42309,10 +42319,10 @@
         <v>5</v>
       </c>
       <c r="C155" s="20" t="s">
-        <v>140</v>
+        <v>429</v>
       </c>
       <c r="D155" s="14" t="s">
-        <v>291</v>
+        <v>431</v>
       </c>
       <c r="E155" s="22"/>
       <c r="F155" s="22"/>
@@ -42570,11 +42580,13 @@
         <v>5</v>
       </c>
       <c r="B156" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="C156" s="15"/>
+        <v>5</v>
+      </c>
+      <c r="C156" s="20" t="s">
+        <v>430</v>
+      </c>
       <c r="D156" s="14" t="s">
-        <v>342</v>
+        <v>290</v>
       </c>
       <c r="E156" s="22"/>
       <c r="F156" s="22"/>
@@ -42834,11 +42846,11 @@
       <c r="B157" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C157" s="13" t="s">
-        <v>142</v>
+      <c r="C157" s="20" t="s">
+        <v>140</v>
       </c>
       <c r="D157" s="14" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E157" s="22"/>
       <c r="F157" s="22"/>
@@ -43096,13 +43108,11 @@
         <v>5</v>
       </c>
       <c r="B158" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C158" s="13" t="s">
-        <v>143</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="C158" s="15"/>
       <c r="D158" s="14" t="s">
-        <v>294</v>
+        <v>342</v>
       </c>
       <c r="E158" s="22"/>
       <c r="F158" s="22"/>
@@ -43363,10 +43373,10 @@
         <v>5</v>
       </c>
       <c r="C159" s="13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D159" s="14" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E159" s="22"/>
       <c r="F159" s="22"/>
@@ -43627,10 +43637,10 @@
         <v>5</v>
       </c>
       <c r="C160" s="13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D160" s="14" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E160" s="22"/>
       <c r="F160" s="22"/>
@@ -43891,10 +43901,10 @@
         <v>5</v>
       </c>
       <c r="C161" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D161" s="14" t="s">
-        <v>343</v>
+        <v>295</v>
       </c>
       <c r="E161" s="22"/>
       <c r="F161" s="22"/>
@@ -44152,11 +44162,13 @@
         <v>5</v>
       </c>
       <c r="B162" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="C162" s="15"/>
+        <v>5</v>
+      </c>
+      <c r="C162" s="13" t="s">
+        <v>145</v>
+      </c>
       <c r="D162" s="14" t="s">
-        <v>344</v>
+        <v>293</v>
       </c>
       <c r="E162" s="22"/>
       <c r="F162" s="22"/>
@@ -44417,10 +44429,10 @@
         <v>5</v>
       </c>
       <c r="C163" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D163" s="14" t="s">
-        <v>297</v>
+        <v>343</v>
       </c>
       <c r="E163" s="22"/>
       <c r="F163" s="22"/>
@@ -44678,13 +44690,11 @@
         <v>5</v>
       </c>
       <c r="B164" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C164" s="13" t="s">
-        <v>149</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="C164" s="15"/>
       <c r="D164" s="14" t="s">
-        <v>296</v>
+        <v>344</v>
       </c>
       <c r="E164" s="22"/>
       <c r="F164" s="22"/>
@@ -44945,10 +44955,10 @@
         <v>5</v>
       </c>
       <c r="C165" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D165" s="14" t="s">
-        <v>356</v>
+        <v>297</v>
       </c>
       <c r="E165" s="22"/>
       <c r="F165" s="22"/>
@@ -45201,7 +45211,7 @@
       <c r="IS165" s="22"/>
       <c r="IT165" s="22"/>
     </row>
-    <row r="166" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A166" s="13" t="s">
         <v>5</v>
       </c>
@@ -45209,10 +45219,10 @@
         <v>5</v>
       </c>
       <c r="C166" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D166" s="14" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E166" s="22"/>
       <c r="F166" s="22"/>
@@ -45473,10 +45483,10 @@
         <v>5</v>
       </c>
       <c r="C167" s="13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D167" s="14" t="s">
-        <v>299</v>
+        <v>356</v>
       </c>
       <c r="E167" s="22"/>
       <c r="F167" s="22"/>
@@ -45729,18 +45739,18 @@
       <c r="IS167" s="22"/>
       <c r="IT167" s="22"/>
     </row>
-    <row r="168" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A168" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B168" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C168" s="20" t="s">
-        <v>433</v>
+      <c r="C168" s="13" t="s">
+        <v>151</v>
       </c>
       <c r="D168" s="14" t="s">
-        <v>459</v>
+        <v>298</v>
       </c>
       <c r="E168" s="22"/>
       <c r="F168" s="22"/>
@@ -46001,10 +46011,10 @@
         <v>5</v>
       </c>
       <c r="C169" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D169" s="14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E169" s="22"/>
       <c r="F169" s="22"/>
@@ -46262,11 +46272,13 @@
         <v>5</v>
       </c>
       <c r="B170" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="C170" s="15"/>
+        <v>5</v>
+      </c>
+      <c r="C170" s="20" t="s">
+        <v>432</v>
+      </c>
       <c r="D170" s="14" t="s">
-        <v>369</v>
+        <v>458</v>
       </c>
       <c r="E170" s="22"/>
       <c r="F170" s="22"/>
@@ -46527,10 +46539,10 @@
         <v>5</v>
       </c>
       <c r="C171" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D171" s="14" t="s">
-        <v>370</v>
+        <v>300</v>
       </c>
       <c r="E171" s="22"/>
       <c r="F171" s="22"/>
@@ -46788,13 +46800,11 @@
         <v>5</v>
       </c>
       <c r="B172" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C172" s="13" t="s">
-        <v>156</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="C172" s="15"/>
       <c r="D172" s="14" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E172" s="22"/>
       <c r="F172" s="22"/>
@@ -47055,10 +47065,10 @@
         <v>5</v>
       </c>
       <c r="C173" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D173" s="14" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E173" s="22"/>
       <c r="F173" s="22"/>
@@ -47311,14 +47321,18 @@
       <c r="IS173" s="22"/>
       <c r="IT173" s="22"/>
     </row>
-    <row r="174" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A174" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="B174" s="15"/>
-      <c r="C174" s="15"/>
+        <v>5</v>
+      </c>
+      <c r="B174" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C174" s="13" t="s">
+        <v>156</v>
+      </c>
       <c r="D174" s="14" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E174" s="22"/>
       <c r="F174" s="22"/>
@@ -47576,11 +47590,13 @@
         <v>5</v>
       </c>
       <c r="B175" s="13" t="s">
-        <v>378</v>
-      </c>
-      <c r="C175" s="15"/>
+        <v>5</v>
+      </c>
+      <c r="C175" s="13" t="s">
+        <v>157</v>
+      </c>
       <c r="D175" s="14" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="E175" s="22"/>
       <c r="F175" s="22"/>
@@ -47833,18 +47849,14 @@
       <c r="IS175" s="22"/>
       <c r="IT175" s="22"/>
     </row>
-    <row r="176" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A176" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B176" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C176" s="13" t="s">
-        <v>159</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="B176" s="15"/>
+      <c r="C176" s="15"/>
       <c r="D176" s="14" t="s">
-        <v>301</v>
+        <v>373</v>
       </c>
       <c r="E176" s="22"/>
       <c r="F176" s="22"/>
@@ -48102,13 +48114,11 @@
         <v>5</v>
       </c>
       <c r="B177" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C177" s="13" t="s">
-        <v>160</v>
-      </c>
+        <v>378</v>
+      </c>
+      <c r="C177" s="15"/>
       <c r="D177" s="14" t="s">
-        <v>302</v>
+        <v>379</v>
       </c>
       <c r="E177" s="22"/>
       <c r="F177" s="22"/>
@@ -48369,10 +48379,10 @@
         <v>5</v>
       </c>
       <c r="C178" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D178" s="14" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E178" s="22"/>
       <c r="F178" s="22"/>
@@ -48633,10 +48643,10 @@
         <v>5</v>
       </c>
       <c r="C179" s="13" t="s">
-        <v>376</v>
+        <v>160</v>
       </c>
       <c r="D179" s="14" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E179" s="22"/>
       <c r="F179" s="22"/>
@@ -48897,10 +48907,10 @@
         <v>5</v>
       </c>
       <c r="C180" s="13" t="s">
-        <v>377</v>
+        <v>161</v>
       </c>
       <c r="D180" s="14" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E180" s="22"/>
       <c r="F180" s="22"/>
@@ -49158,11 +49168,13 @@
         <v>5</v>
       </c>
       <c r="B181" s="13" t="s">
-        <v>380</v>
-      </c>
-      <c r="C181" s="15"/>
+        <v>5</v>
+      </c>
+      <c r="C181" s="13" t="s">
+        <v>376</v>
+      </c>
       <c r="D181" s="14" t="s">
-        <v>383</v>
+        <v>304</v>
       </c>
       <c r="E181" s="22"/>
       <c r="F181" s="22"/>
@@ -49423,10 +49435,10 @@
         <v>5</v>
       </c>
       <c r="C182" s="13" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D182" s="14" t="s">
-        <v>382</v>
+        <v>305</v>
       </c>
       <c r="E182" s="22"/>
       <c r="F182" s="22"/>
@@ -49679,18 +49691,16 @@
       <c r="IS182" s="22"/>
       <c r="IT182" s="22"/>
     </row>
-    <row r="183" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A183" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B183" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C183" s="13" t="s">
-        <v>166</v>
-      </c>
+        <v>380</v>
+      </c>
+      <c r="C183" s="15"/>
       <c r="D183" s="14" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E183" s="22"/>
       <c r="F183" s="22"/>
@@ -49948,11 +49958,13 @@
         <v>5</v>
       </c>
       <c r="B184" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="C184" s="15"/>
+        <v>5</v>
+      </c>
+      <c r="C184" s="13" t="s">
+        <v>381</v>
+      </c>
       <c r="D184" s="14" t="s">
-        <v>306</v>
+        <v>382</v>
       </c>
       <c r="E184" s="22"/>
       <c r="F184" s="22"/>
@@ -50205,7 +50217,7 @@
       <c r="IS184" s="22"/>
       <c r="IT184" s="22"/>
     </row>
-    <row r="185" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A185" s="13" t="s">
         <v>5</v>
       </c>
@@ -50213,10 +50225,10 @@
         <v>5</v>
       </c>
       <c r="C185" s="13" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D185" s="14" t="s">
-        <v>307</v>
+        <v>384</v>
       </c>
       <c r="E185" s="22"/>
       <c r="F185" s="22"/>
@@ -50474,13 +50486,11 @@
         <v>5</v>
       </c>
       <c r="B186" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C186" s="13" t="s">
-        <v>164</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="C186" s="15"/>
       <c r="D186" s="14" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E186" s="22"/>
       <c r="F186" s="22"/>
@@ -50738,11 +50748,13 @@
         <v>5</v>
       </c>
       <c r="B187" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="C187" s="15"/>
+        <v>5</v>
+      </c>
+      <c r="C187" s="13" t="s">
+        <v>163</v>
+      </c>
       <c r="D187" s="14" t="s">
-        <v>345</v>
+        <v>307</v>
       </c>
       <c r="E187" s="22"/>
       <c r="F187" s="22"/>
@@ -51003,10 +51015,10 @@
         <v>5</v>
       </c>
       <c r="C188" s="13" t="s">
-        <v>386</v>
+        <v>164</v>
       </c>
       <c r="D188" s="14" t="s">
-        <v>387</v>
+        <v>308</v>
       </c>
       <c r="E188" s="22"/>
       <c r="F188" s="22"/>
@@ -51264,13 +51276,11 @@
         <v>5</v>
       </c>
       <c r="B189" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C189" s="13" t="s">
-        <v>385</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="C189" s="15"/>
       <c r="D189" s="14" t="s">
-        <v>388</v>
+        <v>345</v>
       </c>
       <c r="E189" s="22"/>
       <c r="F189" s="22"/>
@@ -51525,12 +51535,16 @@
     </row>
     <row r="190" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A190" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="B190" s="15"/>
-      <c r="C190" s="15"/>
+        <v>5</v>
+      </c>
+      <c r="B190" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C190" s="13" t="s">
+        <v>386</v>
+      </c>
       <c r="D190" s="14" t="s">
-        <v>331</v>
+        <v>387</v>
       </c>
       <c r="E190" s="22"/>
       <c r="F190" s="22"/>
@@ -51788,11 +51802,13 @@
         <v>5</v>
       </c>
       <c r="B191" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="C191" s="15"/>
+        <v>5</v>
+      </c>
+      <c r="C191" s="13" t="s">
+        <v>385</v>
+      </c>
       <c r="D191" s="14" t="s">
-        <v>309</v>
+        <v>388</v>
       </c>
       <c r="E191" s="22"/>
       <c r="F191" s="22"/>
@@ -52047,16 +52063,12 @@
     </row>
     <row r="192" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A192" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B192" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C192" s="13" t="s">
-        <v>169</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="B192" s="15"/>
+      <c r="C192" s="15"/>
       <c r="D192" s="14" t="s">
-        <v>310</v>
+        <v>331</v>
       </c>
       <c r="E192" s="22"/>
       <c r="F192" s="22"/>
@@ -52314,13 +52326,11 @@
         <v>5</v>
       </c>
       <c r="B193" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C193" s="13" t="s">
-        <v>170</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="C193" s="15"/>
       <c r="D193" s="14" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="E193" s="22"/>
       <c r="F193" s="22"/>
@@ -52578,11 +52588,13 @@
         <v>5</v>
       </c>
       <c r="B194" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="C194" s="15"/>
+        <v>5</v>
+      </c>
+      <c r="C194" s="13" t="s">
+        <v>169</v>
+      </c>
       <c r="D194" s="14" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E194" s="22"/>
       <c r="F194" s="22"/>
@@ -52843,10 +52855,10 @@
         <v>5</v>
       </c>
       <c r="C195" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D195" s="14" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E195" s="22"/>
       <c r="F195" s="22"/>
@@ -53101,12 +53113,14 @@
     </row>
     <row r="196" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A196" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="B196" s="15"/>
+        <v>5</v>
+      </c>
+      <c r="B196" s="13" t="s">
+        <v>171</v>
+      </c>
       <c r="C196" s="15"/>
       <c r="D196" s="14" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="E196" s="22"/>
       <c r="F196" s="22"/>
@@ -53360,13 +53374,17 @@
       <c r="IT196" s="22"/>
     </row>
     <row r="197" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A197" s="13"/>
-      <c r="B197" s="25" t="s">
-        <v>434</v>
-      </c>
-      <c r="C197" s="15"/>
+      <c r="A197" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B197" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C197" s="13" t="s">
+        <v>172</v>
+      </c>
       <c r="D197" s="14" t="s">
-        <v>460</v>
+        <v>313</v>
       </c>
       <c r="E197" s="22"/>
       <c r="F197" s="22"/>
@@ -53620,13 +53638,13 @@
       <c r="IT197" s="22"/>
     </row>
     <row r="198" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A198" s="13"/>
-      <c r="B198" s="25"/>
-      <c r="C198" s="25" t="s">
-        <v>461</v>
-      </c>
+      <c r="A198" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="B198" s="15"/>
+      <c r="C198" s="15"/>
       <c r="D198" s="14" t="s">
-        <v>462</v>
+        <v>314</v>
       </c>
       <c r="E198" s="22"/>
       <c r="F198" s="22"/>
@@ -53880,15 +53898,13 @@
       <c r="IT198" s="22"/>
     </row>
     <row r="199" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A199" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B199" s="13" t="s">
-        <v>174</v>
+      <c r="A199" s="13"/>
+      <c r="B199" s="25" t="s">
+        <v>433</v>
       </c>
       <c r="C199" s="15"/>
       <c r="D199" s="14" t="s">
-        <v>315</v>
+        <v>459</v>
       </c>
       <c r="E199" s="22"/>
       <c r="F199" s="22"/>
@@ -54141,18 +54157,14 @@
       <c r="IS199" s="22"/>
       <c r="IT199" s="22"/>
     </row>
-    <row r="200" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A200" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B200" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C200" s="20" t="s">
-        <v>316</v>
+    <row r="200" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A200" s="13"/>
+      <c r="B200" s="25"/>
+      <c r="C200" s="25" t="s">
+        <v>460</v>
       </c>
       <c r="D200" s="14" t="s">
-        <v>317</v>
+        <v>461</v>
       </c>
       <c r="E200" s="22"/>
       <c r="F200" s="22"/>
@@ -54410,11 +54422,11 @@
         <v>5</v>
       </c>
       <c r="B201" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C201" s="15"/>
       <c r="D201" s="14" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E201" s="22"/>
       <c r="F201" s="22"/>
@@ -54667,18 +54679,18 @@
       <c r="IS201" s="22"/>
       <c r="IT201" s="22"/>
     </row>
-    <row r="202" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A202" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B202" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C202" s="13" t="s">
-        <v>176</v>
+      <c r="C202" s="20" t="s">
+        <v>316</v>
       </c>
       <c r="D202" s="14" t="s">
-        <v>357</v>
+        <v>317</v>
       </c>
       <c r="E202" s="22"/>
       <c r="F202" s="22"/>
@@ -54936,11 +54948,11 @@
         <v>5</v>
       </c>
       <c r="B203" s="13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C203" s="15"/>
       <c r="D203" s="14" t="s">
-        <v>358</v>
+        <v>318</v>
       </c>
       <c r="E203" s="22"/>
       <c r="F203" s="22"/>
@@ -55201,10 +55213,10 @@
         <v>5</v>
       </c>
       <c r="C204" s="13" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D204" s="14" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E204" s="22"/>
       <c r="F204" s="22"/>
@@ -55462,11 +55474,11 @@
         <v>5</v>
       </c>
       <c r="B205" s="13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C205" s="15"/>
       <c r="D205" s="14" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E205" s="22"/>
       <c r="F205" s="22"/>
@@ -55727,10 +55739,10 @@
         <v>5</v>
       </c>
       <c r="C206" s="13" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D206" s="14" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E206" s="22"/>
       <c r="F206" s="22"/>
@@ -55988,13 +56000,11 @@
         <v>5</v>
       </c>
       <c r="B207" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C207" s="13" t="s">
-        <v>181</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="C207" s="15"/>
       <c r="D207" s="14" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E207" s="22"/>
       <c r="F207" s="22"/>
@@ -56249,12 +56259,16 @@
     </row>
     <row r="208" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A208" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="B208" s="15"/>
-      <c r="C208" s="15"/>
+        <v>5</v>
+      </c>
+      <c r="B208" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C208" s="13" t="s">
+        <v>180</v>
+      </c>
       <c r="D208" s="14" t="s">
-        <v>319</v>
+        <v>361</v>
       </c>
       <c r="E208" s="22"/>
       <c r="F208" s="22"/>
@@ -56512,11 +56526,13 @@
         <v>5</v>
       </c>
       <c r="B209" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="C209" s="15"/>
+        <v>5</v>
+      </c>
+      <c r="C209" s="13" t="s">
+        <v>181</v>
+      </c>
       <c r="D209" s="14" t="s">
-        <v>320</v>
+        <v>362</v>
       </c>
       <c r="E209" s="22"/>
       <c r="F209" s="22"/>
@@ -56771,16 +56787,12 @@
     </row>
     <row r="210" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A210" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B210" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C210" s="13" t="s">
-        <v>184</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="B210" s="15"/>
+      <c r="C210" s="15"/>
       <c r="D210" s="14" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E210" s="22"/>
       <c r="F210" s="22"/>
@@ -57038,13 +57050,11 @@
         <v>5</v>
       </c>
       <c r="B211" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C211" s="13" t="s">
-        <v>185</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="C211" s="15"/>
       <c r="D211" s="14" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E211" s="22"/>
       <c r="F211" s="22"/>
@@ -57302,11 +57312,13 @@
         <v>5</v>
       </c>
       <c r="B212" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="C212" s="15"/>
-      <c r="D212" s="16" t="s">
-        <v>187</v>
+        <v>5</v>
+      </c>
+      <c r="C212" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="D212" s="14" t="s">
+        <v>321</v>
       </c>
       <c r="E212" s="22"/>
       <c r="F212" s="22"/>
@@ -57567,10 +57579,10 @@
         <v>5</v>
       </c>
       <c r="C213" s="13" t="s">
-        <v>374</v>
+        <v>185</v>
       </c>
       <c r="D213" s="14" t="s">
-        <v>375</v>
+        <v>322</v>
       </c>
       <c r="E213" s="22"/>
       <c r="F213" s="22"/>
@@ -57828,13 +57840,11 @@
         <v>5</v>
       </c>
       <c r="B214" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C214" s="13" t="s">
-        <v>188</v>
-      </c>
-      <c r="D214" s="14" t="s">
-        <v>323</v>
+        <v>186</v>
+      </c>
+      <c r="C214" s="15"/>
+      <c r="D214" s="16" t="s">
+        <v>187</v>
       </c>
       <c r="E214" s="22"/>
       <c r="F214" s="22"/>
@@ -58092,11 +58102,13 @@
         <v>5</v>
       </c>
       <c r="B215" s="13" t="s">
-        <v>189</v>
-      </c>
-      <c r="C215" s="15"/>
+        <v>5</v>
+      </c>
+      <c r="C215" s="13" t="s">
+        <v>374</v>
+      </c>
       <c r="D215" s="14" t="s">
-        <v>324</v>
+        <v>375</v>
       </c>
       <c r="E215" s="22"/>
       <c r="F215" s="22"/>
@@ -58349,7 +58361,7 @@
       <c r="IS215" s="22"/>
       <c r="IT215" s="22"/>
     </row>
-    <row r="216" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A216" s="13" t="s">
         <v>5</v>
       </c>
@@ -58357,10 +58369,10 @@
         <v>5</v>
       </c>
       <c r="C216" s="13" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D216" s="14" t="s">
-        <v>365</v>
+        <v>323</v>
       </c>
       <c r="E216" s="22"/>
       <c r="F216" s="22"/>
@@ -58615,12 +58627,14 @@
     </row>
     <row r="217" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A217" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="B217" s="15"/>
+        <v>5</v>
+      </c>
+      <c r="B217" s="13" t="s">
+        <v>189</v>
+      </c>
       <c r="C217" s="15"/>
       <c r="D217" s="14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E217" s="22"/>
       <c r="F217" s="22"/>
@@ -58873,16 +58887,18 @@
       <c r="IS217" s="22"/>
       <c r="IT217" s="22"/>
     </row>
-    <row r="218" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A218" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B218" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C218" s="15"/>
+        <v>5</v>
+      </c>
+      <c r="C218" s="13" t="s">
+        <v>190</v>
+      </c>
       <c r="D218" s="14" t="s">
-        <v>326</v>
+        <v>365</v>
       </c>
       <c r="E218" s="22"/>
       <c r="F218" s="22"/>
@@ -59137,16 +59153,12 @@
     </row>
     <row r="219" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A219" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B219" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C219" s="13" t="s">
-        <v>193</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="B219" s="15"/>
+      <c r="C219" s="15"/>
       <c r="D219" s="14" t="s">
-        <v>194</v>
+        <v>325</v>
       </c>
       <c r="E219" s="22"/>
       <c r="F219" s="22"/>
@@ -59404,11 +59416,11 @@
         <v>5</v>
       </c>
       <c r="B220" s="13" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C220" s="15"/>
       <c r="D220" s="14" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E220" s="22"/>
       <c r="F220" s="22"/>
@@ -59661,14 +59673,18 @@
       <c r="IS220" s="22"/>
       <c r="IT220" s="22"/>
     </row>
-    <row r="221" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A221" s="17" t="s">
-        <v>400</v>
-      </c>
-      <c r="B221" s="17"/>
-      <c r="C221" s="17"/>
-      <c r="D221" s="19" t="s">
-        <v>401</v>
+    <row r="221" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A221" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B221" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C221" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="D221" s="14" t="s">
+        <v>194</v>
       </c>
       <c r="E221" s="22"/>
       <c r="F221" s="22"/>
@@ -59921,14 +59937,16 @@
       <c r="IS221" s="22"/>
       <c r="IT221" s="22"/>
     </row>
-    <row r="222" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A222" s="18"/>
-      <c r="B222" s="17" t="s">
-        <v>402</v>
-      </c>
-      <c r="C222" s="17"/>
-      <c r="D222" s="19" t="s">
-        <v>403</v>
+    <row r="222" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A222" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B222" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="C222" s="15"/>
+      <c r="D222" s="14" t="s">
+        <v>327</v>
       </c>
       <c r="E222" s="22"/>
       <c r="F222" s="22"/>
@@ -60182,13 +60200,13 @@
       <c r="IT222" s="22"/>
     </row>
     <row r="223" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A223" s="18"/>
+      <c r="A223" s="17" t="s">
+        <v>399</v>
+      </c>
       <c r="B223" s="17"/>
-      <c r="C223" s="17" t="s">
-        <v>404</v>
-      </c>
+      <c r="C223" s="17"/>
       <c r="D223" s="19" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="E223" s="22"/>
       <c r="F223" s="22"/>
@@ -60443,12 +60461,12 @@
     </row>
     <row r="224" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A224" s="18"/>
-      <c r="B224" s="17"/>
-      <c r="C224" s="17" t="s">
-        <v>406</v>
-      </c>
+      <c r="B224" s="17" t="s">
+        <v>401</v>
+      </c>
+      <c r="C224" s="17"/>
       <c r="D224" s="19" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="E224" s="22"/>
       <c r="F224" s="22"/>
@@ -60705,10 +60723,10 @@
       <c r="A225" s="18"/>
       <c r="B225" s="17"/>
       <c r="C225" s="17" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="D225" s="19" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="E225" s="22"/>
       <c r="F225" s="22"/>
@@ -60961,14 +60979,14 @@
       <c r="IS225" s="22"/>
       <c r="IT225" s="22"/>
     </row>
-    <row r="226" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A226" s="18"/>
       <c r="B226" s="17"/>
       <c r="C226" s="17" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="D226" s="19" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="E226" s="22"/>
       <c r="F226" s="22"/>
@@ -61221,14 +61239,14 @@
       <c r="IS226" s="22"/>
       <c r="IT226" s="22"/>
     </row>
-    <row r="227" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A227" s="18"/>
       <c r="B227" s="17"/>
       <c r="C227" s="17" t="s">
-        <v>463</v>
+        <v>407</v>
       </c>
       <c r="D227" s="19" t="s">
-        <v>464</v>
+        <v>408</v>
       </c>
       <c r="E227" s="22"/>
       <c r="F227" s="22"/>
@@ -61483,12 +61501,12 @@
     </row>
     <row r="228" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A228" s="18"/>
-      <c r="B228" s="17" t="s">
-        <v>412</v>
-      </c>
-      <c r="C228" s="17"/>
+      <c r="B228" s="17"/>
+      <c r="C228" s="17" t="s">
+        <v>409</v>
+      </c>
       <c r="D228" s="19" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="E228" s="22"/>
       <c r="F228" s="22"/>
@@ -61745,10 +61763,10 @@
       <c r="A229" s="18"/>
       <c r="B229" s="17"/>
       <c r="C229" s="17" t="s">
-        <v>414</v>
+        <v>462</v>
       </c>
       <c r="D229" s="19" t="s">
-        <v>415</v>
+        <v>463</v>
       </c>
       <c r="E229" s="22"/>
       <c r="F229" s="22"/>
@@ -62003,12 +62021,12 @@
     </row>
     <row r="230" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A230" s="18"/>
-      <c r="B230" s="17"/>
-      <c r="C230" s="17" t="s">
-        <v>465</v>
-      </c>
+      <c r="B230" s="17" t="s">
+        <v>411</v>
+      </c>
+      <c r="C230" s="17"/>
       <c r="D230" s="19" t="s">
-        <v>466</v>
+        <v>412</v>
       </c>
       <c r="E230" s="22"/>
       <c r="F230" s="22"/>
@@ -62265,10 +62283,10 @@
       <c r="A231" s="18"/>
       <c r="B231" s="17"/>
       <c r="C231" s="17" t="s">
-        <v>435</v>
+        <v>413</v>
       </c>
       <c r="D231" s="19" t="s">
-        <v>467</v>
+        <v>414</v>
       </c>
       <c r="E231" s="22"/>
       <c r="F231" s="22"/>
@@ -62525,10 +62543,10 @@
       <c r="A232" s="18"/>
       <c r="B232" s="17"/>
       <c r="C232" s="17" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="D232" s="19" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="E232" s="22"/>
       <c r="F232" s="22"/>
@@ -62781,257 +62799,777 @@
       <c r="IS232" s="22"/>
       <c r="IT232" s="22"/>
     </row>
-    <row r="239" spans="1:254" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="E239" s="2"/>
-      <c r="F239" s="2"/>
-      <c r="G239" s="2"/>
-      <c r="H239" s="2"/>
-      <c r="I239" s="2"/>
-      <c r="J239" s="2"/>
-      <c r="K239" s="2"/>
-      <c r="L239" s="2"/>
-      <c r="M239" s="2"/>
-      <c r="N239" s="2"/>
-      <c r="O239" s="2"/>
-      <c r="P239" s="2"/>
-      <c r="Q239" s="2"/>
-      <c r="R239" s="2"/>
-      <c r="S239" s="2"/>
-      <c r="T239" s="2"/>
-      <c r="U239" s="2"/>
-      <c r="V239" s="2"/>
-      <c r="W239" s="2"/>
-      <c r="X239" s="2"/>
-      <c r="Y239" s="2"/>
-      <c r="Z239" s="2"/>
-      <c r="AA239" s="2"/>
-      <c r="AB239" s="2"/>
-      <c r="AC239" s="2"/>
-      <c r="AD239" s="2"/>
-      <c r="AE239" s="2"/>
-      <c r="AF239" s="2"/>
-      <c r="AG239" s="2"/>
-      <c r="AH239" s="2"/>
-      <c r="AI239" s="2"/>
-      <c r="AJ239" s="2"/>
-      <c r="AK239" s="2"/>
-      <c r="AL239" s="2"/>
-      <c r="AM239" s="2"/>
-      <c r="AN239" s="2"/>
-      <c r="AO239" s="2"/>
-      <c r="AP239" s="2"/>
-      <c r="AQ239" s="2"/>
-      <c r="AR239" s="2"/>
-      <c r="AS239" s="2"/>
-      <c r="AT239" s="2"/>
-      <c r="AU239" s="2"/>
-      <c r="AV239" s="2"/>
-      <c r="AW239" s="2"/>
-      <c r="AX239" s="2"/>
-      <c r="AY239" s="2"/>
-      <c r="AZ239" s="2"/>
-      <c r="BA239" s="2"/>
-      <c r="BB239" s="2"/>
-      <c r="BC239" s="2"/>
-      <c r="BD239" s="2"/>
-      <c r="BE239" s="2"/>
-      <c r="BF239" s="2"/>
-      <c r="BG239" s="2"/>
-      <c r="BH239" s="2"/>
-      <c r="BI239" s="2"/>
-      <c r="BJ239" s="2"/>
-      <c r="BK239" s="2"/>
-      <c r="BL239" s="2"/>
-      <c r="BM239" s="2"/>
-      <c r="BN239" s="2"/>
-      <c r="BO239" s="2"/>
-      <c r="BP239" s="2"/>
-      <c r="BQ239" s="2"/>
-      <c r="BR239" s="2"/>
-      <c r="BS239" s="2"/>
-      <c r="BT239" s="2"/>
-      <c r="BU239" s="2"/>
-      <c r="BV239" s="2"/>
-      <c r="BW239" s="2"/>
-      <c r="BX239" s="2"/>
-      <c r="BY239" s="2"/>
-      <c r="BZ239" s="2"/>
-      <c r="CA239" s="2"/>
-      <c r="CB239" s="2"/>
-      <c r="CC239" s="2"/>
-      <c r="CD239" s="2"/>
-      <c r="CE239" s="2"/>
-      <c r="CF239" s="2"/>
-      <c r="CG239" s="2"/>
-      <c r="CH239" s="2"/>
-      <c r="CI239" s="2"/>
-      <c r="CJ239" s="2"/>
-      <c r="CK239" s="2"/>
-      <c r="CL239" s="2"/>
-      <c r="CM239" s="2"/>
-      <c r="CN239" s="2"/>
-      <c r="CO239" s="2"/>
-      <c r="CP239" s="2"/>
-      <c r="CQ239" s="2"/>
-      <c r="CR239" s="2"/>
-      <c r="CS239" s="2"/>
-      <c r="CT239" s="2"/>
-      <c r="CU239" s="2"/>
-      <c r="CV239" s="2"/>
-      <c r="CW239" s="2"/>
-      <c r="CX239" s="2"/>
-      <c r="CY239" s="2"/>
-      <c r="CZ239" s="2"/>
-      <c r="DA239" s="2"/>
-      <c r="DB239" s="2"/>
-      <c r="DC239" s="2"/>
-      <c r="DD239" s="2"/>
-      <c r="DE239" s="2"/>
-      <c r="DF239" s="2"/>
-      <c r="DG239" s="2"/>
-      <c r="DH239" s="2"/>
-      <c r="DI239" s="2"/>
-      <c r="DJ239" s="2"/>
-      <c r="DK239" s="2"/>
-      <c r="DL239" s="2"/>
-      <c r="DM239" s="2"/>
-      <c r="DN239" s="2"/>
-      <c r="DO239" s="2"/>
-      <c r="DP239" s="2"/>
-      <c r="DQ239" s="2"/>
-      <c r="DR239" s="2"/>
-      <c r="DS239" s="2"/>
-      <c r="DT239" s="2"/>
-      <c r="DU239" s="2"/>
-      <c r="DV239" s="2"/>
-      <c r="DW239" s="2"/>
-      <c r="DX239" s="2"/>
-      <c r="DY239" s="2"/>
-      <c r="DZ239" s="2"/>
-      <c r="EA239" s="2"/>
-      <c r="EB239" s="2"/>
-      <c r="EC239" s="2"/>
-      <c r="ED239" s="2"/>
-      <c r="EE239" s="2"/>
-      <c r="EF239" s="2"/>
-      <c r="EG239" s="2"/>
-      <c r="EH239" s="2"/>
-      <c r="EI239" s="2"/>
-      <c r="EJ239" s="2"/>
-      <c r="EK239" s="2"/>
-      <c r="EL239" s="2"/>
-      <c r="EM239" s="2"/>
-      <c r="EN239" s="2"/>
-      <c r="EO239" s="2"/>
-      <c r="EP239" s="2"/>
-      <c r="EQ239" s="2"/>
-      <c r="ER239" s="2"/>
-      <c r="ES239" s="2"/>
-      <c r="ET239" s="2"/>
-      <c r="EU239" s="2"/>
-      <c r="EV239" s="2"/>
-      <c r="EW239" s="2"/>
-      <c r="EX239" s="2"/>
-      <c r="EY239" s="2"/>
-      <c r="EZ239" s="2"/>
-      <c r="FA239" s="2"/>
-      <c r="FB239" s="2"/>
-      <c r="FC239" s="2"/>
-      <c r="FD239" s="2"/>
-      <c r="FE239" s="2"/>
-      <c r="FF239" s="2"/>
-      <c r="FG239" s="2"/>
-      <c r="FH239" s="2"/>
-      <c r="FI239" s="2"/>
-      <c r="FJ239" s="2"/>
-      <c r="FK239" s="2"/>
-      <c r="FL239" s="2"/>
-      <c r="FM239" s="2"/>
-      <c r="FN239" s="2"/>
-      <c r="FO239" s="2"/>
-      <c r="FP239" s="2"/>
-      <c r="FQ239" s="2"/>
-      <c r="FR239" s="2"/>
-      <c r="FS239" s="2"/>
-      <c r="FT239" s="2"/>
-      <c r="FU239" s="2"/>
-      <c r="FV239" s="2"/>
-      <c r="FW239" s="2"/>
-      <c r="FX239" s="2"/>
-      <c r="FY239" s="2"/>
-      <c r="FZ239" s="2"/>
-      <c r="GA239" s="2"/>
-      <c r="GB239" s="2"/>
-      <c r="GC239" s="2"/>
-      <c r="GD239" s="2"/>
-      <c r="GE239" s="2"/>
-      <c r="GF239" s="2"/>
-      <c r="GG239" s="2"/>
-      <c r="GH239" s="2"/>
-      <c r="GI239" s="2"/>
-      <c r="GJ239" s="2"/>
-      <c r="GK239" s="2"/>
-      <c r="GL239" s="2"/>
-      <c r="GM239" s="2"/>
-      <c r="GN239" s="2"/>
-      <c r="GO239" s="2"/>
-      <c r="GP239" s="2"/>
-      <c r="GQ239" s="2"/>
-      <c r="GR239" s="2"/>
-      <c r="GS239" s="2"/>
-      <c r="GT239" s="2"/>
-      <c r="GU239" s="2"/>
-      <c r="GV239" s="2"/>
-      <c r="GW239" s="2"/>
-      <c r="GX239" s="2"/>
-      <c r="GY239" s="2"/>
-      <c r="GZ239" s="2"/>
-      <c r="HA239" s="2"/>
-      <c r="HB239" s="2"/>
-      <c r="HC239" s="2"/>
-      <c r="HD239" s="2"/>
-      <c r="HE239" s="2"/>
-      <c r="HF239" s="2"/>
-      <c r="HG239" s="2"/>
-      <c r="HH239" s="2"/>
-      <c r="HI239" s="2"/>
-      <c r="HJ239" s="2"/>
-      <c r="HK239" s="2"/>
-      <c r="HL239" s="2"/>
-      <c r="HM239" s="2"/>
-      <c r="HN239" s="2"/>
-      <c r="HO239" s="2"/>
-      <c r="HP239" s="2"/>
-      <c r="HQ239" s="2"/>
-      <c r="HR239" s="2"/>
-      <c r="HS239" s="2"/>
-      <c r="HT239" s="2"/>
-      <c r="HU239" s="2"/>
-      <c r="HV239" s="2"/>
-      <c r="HW239" s="2"/>
-      <c r="HX239" s="2"/>
-      <c r="HY239" s="2"/>
-      <c r="HZ239" s="2"/>
-      <c r="IA239" s="2"/>
-      <c r="IB239" s="2"/>
-      <c r="IC239" s="2"/>
-      <c r="ID239" s="2"/>
-      <c r="IE239" s="2"/>
-      <c r="IF239" s="2"/>
-      <c r="IG239" s="2"/>
-      <c r="IH239" s="2"/>
-      <c r="II239" s="2"/>
-      <c r="IJ239" s="2"/>
-      <c r="IK239" s="2"/>
-      <c r="IL239" s="2"/>
-      <c r="IM239" s="2"/>
-      <c r="IN239" s="2"/>
-      <c r="IO239" s="2"/>
-      <c r="IP239" s="2"/>
-      <c r="IQ239" s="2"/>
-      <c r="IR239" s="2"/>
-      <c r="IS239" s="2"/>
-      <c r="IT239" s="2"/>
+    <row r="233" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A233" s="18"/>
+      <c r="B233" s="17"/>
+      <c r="C233" s="17" t="s">
+        <v>434</v>
+      </c>
+      <c r="D233" s="19" t="s">
+        <v>466</v>
+      </c>
+      <c r="E233" s="22"/>
+      <c r="F233" s="22"/>
+      <c r="G233" s="22"/>
+      <c r="H233" s="22"/>
+      <c r="I233" s="22"/>
+      <c r="J233" s="22"/>
+      <c r="K233" s="22"/>
+      <c r="L233" s="22"/>
+      <c r="M233" s="22"/>
+      <c r="N233" s="22"/>
+      <c r="O233" s="22"/>
+      <c r="P233" s="22"/>
+      <c r="Q233" s="22"/>
+      <c r="R233" s="22"/>
+      <c r="S233" s="22"/>
+      <c r="T233" s="22"/>
+      <c r="U233" s="22"/>
+      <c r="V233" s="22"/>
+      <c r="W233" s="22"/>
+      <c r="X233" s="22"/>
+      <c r="Y233" s="22"/>
+      <c r="Z233" s="22"/>
+      <c r="AA233" s="22"/>
+      <c r="AB233" s="22"/>
+      <c r="AC233" s="22"/>
+      <c r="AD233" s="22"/>
+      <c r="AE233" s="22"/>
+      <c r="AF233" s="22"/>
+      <c r="AG233" s="22"/>
+      <c r="AH233" s="22"/>
+      <c r="AI233" s="22"/>
+      <c r="AJ233" s="22"/>
+      <c r="AK233" s="22"/>
+      <c r="AL233" s="22"/>
+      <c r="AM233" s="22"/>
+      <c r="AN233" s="22"/>
+      <c r="AO233" s="22"/>
+      <c r="AP233" s="22"/>
+      <c r="AQ233" s="22"/>
+      <c r="AR233" s="22"/>
+      <c r="AS233" s="22"/>
+      <c r="AT233" s="22"/>
+      <c r="AU233" s="22"/>
+      <c r="AV233" s="22"/>
+      <c r="AW233" s="22"/>
+      <c r="AX233" s="22"/>
+      <c r="AY233" s="22"/>
+      <c r="AZ233" s="22"/>
+      <c r="BA233" s="22"/>
+      <c r="BB233" s="22"/>
+      <c r="BC233" s="22"/>
+      <c r="BD233" s="22"/>
+      <c r="BE233" s="22"/>
+      <c r="BF233" s="22"/>
+      <c r="BG233" s="22"/>
+      <c r="BH233" s="22"/>
+      <c r="BI233" s="22"/>
+      <c r="BJ233" s="22"/>
+      <c r="BK233" s="22"/>
+      <c r="BL233" s="22"/>
+      <c r="BM233" s="22"/>
+      <c r="BN233" s="22"/>
+      <c r="BO233" s="22"/>
+      <c r="BP233" s="22"/>
+      <c r="BQ233" s="22"/>
+      <c r="BR233" s="22"/>
+      <c r="BS233" s="22"/>
+      <c r="BT233" s="22"/>
+      <c r="BU233" s="22"/>
+      <c r="BV233" s="22"/>
+      <c r="BW233" s="22"/>
+      <c r="BX233" s="22"/>
+      <c r="BY233" s="22"/>
+      <c r="BZ233" s="22"/>
+      <c r="CA233" s="22"/>
+      <c r="CB233" s="22"/>
+      <c r="CC233" s="22"/>
+      <c r="CD233" s="22"/>
+      <c r="CE233" s="22"/>
+      <c r="CF233" s="22"/>
+      <c r="CG233" s="22"/>
+      <c r="CH233" s="22"/>
+      <c r="CI233" s="22"/>
+      <c r="CJ233" s="22"/>
+      <c r="CK233" s="22"/>
+      <c r="CL233" s="22"/>
+      <c r="CM233" s="22"/>
+      <c r="CN233" s="22"/>
+      <c r="CO233" s="22"/>
+      <c r="CP233" s="22"/>
+      <c r="CQ233" s="22"/>
+      <c r="CR233" s="22"/>
+      <c r="CS233" s="22"/>
+      <c r="CT233" s="22"/>
+      <c r="CU233" s="22"/>
+      <c r="CV233" s="22"/>
+      <c r="CW233" s="22"/>
+      <c r="CX233" s="22"/>
+      <c r="CY233" s="22"/>
+      <c r="CZ233" s="22"/>
+      <c r="DA233" s="22"/>
+      <c r="DB233" s="22"/>
+      <c r="DC233" s="22"/>
+      <c r="DD233" s="22"/>
+      <c r="DE233" s="22"/>
+      <c r="DF233" s="22"/>
+      <c r="DG233" s="22"/>
+      <c r="DH233" s="22"/>
+      <c r="DI233" s="22"/>
+      <c r="DJ233" s="22"/>
+      <c r="DK233" s="22"/>
+      <c r="DL233" s="22"/>
+      <c r="DM233" s="22"/>
+      <c r="DN233" s="22"/>
+      <c r="DO233" s="22"/>
+      <c r="DP233" s="22"/>
+      <c r="DQ233" s="22"/>
+      <c r="DR233" s="22"/>
+      <c r="DS233" s="22"/>
+      <c r="DT233" s="22"/>
+      <c r="DU233" s="22"/>
+      <c r="DV233" s="22"/>
+      <c r="DW233" s="22"/>
+      <c r="DX233" s="22"/>
+      <c r="DY233" s="22"/>
+      <c r="DZ233" s="22"/>
+      <c r="EA233" s="22"/>
+      <c r="EB233" s="22"/>
+      <c r="EC233" s="22"/>
+      <c r="ED233" s="22"/>
+      <c r="EE233" s="22"/>
+      <c r="EF233" s="22"/>
+      <c r="EG233" s="22"/>
+      <c r="EH233" s="22"/>
+      <c r="EI233" s="22"/>
+      <c r="EJ233" s="22"/>
+      <c r="EK233" s="22"/>
+      <c r="EL233" s="22"/>
+      <c r="EM233" s="22"/>
+      <c r="EN233" s="22"/>
+      <c r="EO233" s="22"/>
+      <c r="EP233" s="22"/>
+      <c r="EQ233" s="22"/>
+      <c r="ER233" s="22"/>
+      <c r="ES233" s="22"/>
+      <c r="ET233" s="22"/>
+      <c r="EU233" s="22"/>
+      <c r="EV233" s="22"/>
+      <c r="EW233" s="22"/>
+      <c r="EX233" s="22"/>
+      <c r="EY233" s="22"/>
+      <c r="EZ233" s="22"/>
+      <c r="FA233" s="22"/>
+      <c r="FB233" s="22"/>
+      <c r="FC233" s="22"/>
+      <c r="FD233" s="22"/>
+      <c r="FE233" s="22"/>
+      <c r="FF233" s="22"/>
+      <c r="FG233" s="22"/>
+      <c r="FH233" s="22"/>
+      <c r="FI233" s="22"/>
+      <c r="FJ233" s="22"/>
+      <c r="FK233" s="22"/>
+      <c r="FL233" s="22"/>
+      <c r="FM233" s="22"/>
+      <c r="FN233" s="22"/>
+      <c r="FO233" s="22"/>
+      <c r="FP233" s="22"/>
+      <c r="FQ233" s="22"/>
+      <c r="FR233" s="22"/>
+      <c r="FS233" s="22"/>
+      <c r="FT233" s="22"/>
+      <c r="FU233" s="22"/>
+      <c r="FV233" s="22"/>
+      <c r="FW233" s="22"/>
+      <c r="FX233" s="22"/>
+      <c r="FY233" s="22"/>
+      <c r="FZ233" s="22"/>
+      <c r="GA233" s="22"/>
+      <c r="GB233" s="22"/>
+      <c r="GC233" s="22"/>
+      <c r="GD233" s="22"/>
+      <c r="GE233" s="22"/>
+      <c r="GF233" s="22"/>
+      <c r="GG233" s="22"/>
+      <c r="GH233" s="22"/>
+      <c r="GI233" s="22"/>
+      <c r="GJ233" s="22"/>
+      <c r="GK233" s="22"/>
+      <c r="GL233" s="22"/>
+      <c r="GM233" s="22"/>
+      <c r="GN233" s="22"/>
+      <c r="GO233" s="22"/>
+      <c r="GP233" s="22"/>
+      <c r="GQ233" s="22"/>
+      <c r="GR233" s="22"/>
+      <c r="GS233" s="22"/>
+      <c r="GT233" s="22"/>
+      <c r="GU233" s="22"/>
+      <c r="GV233" s="22"/>
+      <c r="GW233" s="22"/>
+      <c r="GX233" s="22"/>
+      <c r="GY233" s="22"/>
+      <c r="GZ233" s="22"/>
+      <c r="HA233" s="22"/>
+      <c r="HB233" s="22"/>
+      <c r="HC233" s="22"/>
+      <c r="HD233" s="22"/>
+      <c r="HE233" s="22"/>
+      <c r="HF233" s="22"/>
+      <c r="HG233" s="22"/>
+      <c r="HH233" s="22"/>
+      <c r="HI233" s="22"/>
+      <c r="HJ233" s="22"/>
+      <c r="HK233" s="22"/>
+      <c r="HL233" s="22"/>
+      <c r="HM233" s="22"/>
+      <c r="HN233" s="22"/>
+      <c r="HO233" s="22"/>
+      <c r="HP233" s="22"/>
+      <c r="HQ233" s="22"/>
+      <c r="HR233" s="22"/>
+      <c r="HS233" s="22"/>
+      <c r="HT233" s="22"/>
+      <c r="HU233" s="22"/>
+      <c r="HV233" s="22"/>
+      <c r="HW233" s="22"/>
+      <c r="HX233" s="22"/>
+      <c r="HY233" s="22"/>
+      <c r="HZ233" s="22"/>
+      <c r="IA233" s="22"/>
+      <c r="IB233" s="22"/>
+      <c r="IC233" s="22"/>
+      <c r="ID233" s="22"/>
+      <c r="IE233" s="22"/>
+      <c r="IF233" s="22"/>
+      <c r="IG233" s="22"/>
+      <c r="IH233" s="22"/>
+      <c r="II233" s="22"/>
+      <c r="IJ233" s="22"/>
+      <c r="IK233" s="22"/>
+      <c r="IL233" s="22"/>
+      <c r="IM233" s="22"/>
+      <c r="IN233" s="22"/>
+      <c r="IO233" s="22"/>
+      <c r="IP233" s="22"/>
+      <c r="IQ233" s="22"/>
+      <c r="IR233" s="22"/>
+      <c r="IS233" s="22"/>
+      <c r="IT233" s="22"/>
+    </row>
+    <row r="234" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A234" s="18"/>
+      <c r="B234" s="17"/>
+      <c r="C234" s="17" t="s">
+        <v>469</v>
+      </c>
+      <c r="D234" s="19" t="s">
+        <v>470</v>
+      </c>
+      <c r="E234" s="22"/>
+      <c r="F234" s="22"/>
+      <c r="G234" s="22"/>
+      <c r="H234" s="22"/>
+      <c r="I234" s="22"/>
+      <c r="J234" s="22"/>
+      <c r="K234" s="22"/>
+      <c r="L234" s="22"/>
+      <c r="M234" s="22"/>
+      <c r="N234" s="22"/>
+      <c r="O234" s="22"/>
+      <c r="P234" s="22"/>
+      <c r="Q234" s="22"/>
+      <c r="R234" s="22"/>
+      <c r="S234" s="22"/>
+      <c r="T234" s="22"/>
+      <c r="U234" s="22"/>
+      <c r="V234" s="22"/>
+      <c r="W234" s="22"/>
+      <c r="X234" s="22"/>
+      <c r="Y234" s="22"/>
+      <c r="Z234" s="22"/>
+      <c r="AA234" s="22"/>
+      <c r="AB234" s="22"/>
+      <c r="AC234" s="22"/>
+      <c r="AD234" s="22"/>
+      <c r="AE234" s="22"/>
+      <c r="AF234" s="22"/>
+      <c r="AG234" s="22"/>
+      <c r="AH234" s="22"/>
+      <c r="AI234" s="22"/>
+      <c r="AJ234" s="22"/>
+      <c r="AK234" s="22"/>
+      <c r="AL234" s="22"/>
+      <c r="AM234" s="22"/>
+      <c r="AN234" s="22"/>
+      <c r="AO234" s="22"/>
+      <c r="AP234" s="22"/>
+      <c r="AQ234" s="22"/>
+      <c r="AR234" s="22"/>
+      <c r="AS234" s="22"/>
+      <c r="AT234" s="22"/>
+      <c r="AU234" s="22"/>
+      <c r="AV234" s="22"/>
+      <c r="AW234" s="22"/>
+      <c r="AX234" s="22"/>
+      <c r="AY234" s="22"/>
+      <c r="AZ234" s="22"/>
+      <c r="BA234" s="22"/>
+      <c r="BB234" s="22"/>
+      <c r="BC234" s="22"/>
+      <c r="BD234" s="22"/>
+      <c r="BE234" s="22"/>
+      <c r="BF234" s="22"/>
+      <c r="BG234" s="22"/>
+      <c r="BH234" s="22"/>
+      <c r="BI234" s="22"/>
+      <c r="BJ234" s="22"/>
+      <c r="BK234" s="22"/>
+      <c r="BL234" s="22"/>
+      <c r="BM234" s="22"/>
+      <c r="BN234" s="22"/>
+      <c r="BO234" s="22"/>
+      <c r="BP234" s="22"/>
+      <c r="BQ234" s="22"/>
+      <c r="BR234" s="22"/>
+      <c r="BS234" s="22"/>
+      <c r="BT234" s="22"/>
+      <c r="BU234" s="22"/>
+      <c r="BV234" s="22"/>
+      <c r="BW234" s="22"/>
+      <c r="BX234" s="22"/>
+      <c r="BY234" s="22"/>
+      <c r="BZ234" s="22"/>
+      <c r="CA234" s="22"/>
+      <c r="CB234" s="22"/>
+      <c r="CC234" s="22"/>
+      <c r="CD234" s="22"/>
+      <c r="CE234" s="22"/>
+      <c r="CF234" s="22"/>
+      <c r="CG234" s="22"/>
+      <c r="CH234" s="22"/>
+      <c r="CI234" s="22"/>
+      <c r="CJ234" s="22"/>
+      <c r="CK234" s="22"/>
+      <c r="CL234" s="22"/>
+      <c r="CM234" s="22"/>
+      <c r="CN234" s="22"/>
+      <c r="CO234" s="22"/>
+      <c r="CP234" s="22"/>
+      <c r="CQ234" s="22"/>
+      <c r="CR234" s="22"/>
+      <c r="CS234" s="22"/>
+      <c r="CT234" s="22"/>
+      <c r="CU234" s="22"/>
+      <c r="CV234" s="22"/>
+      <c r="CW234" s="22"/>
+      <c r="CX234" s="22"/>
+      <c r="CY234" s="22"/>
+      <c r="CZ234" s="22"/>
+      <c r="DA234" s="22"/>
+      <c r="DB234" s="22"/>
+      <c r="DC234" s="22"/>
+      <c r="DD234" s="22"/>
+      <c r="DE234" s="22"/>
+      <c r="DF234" s="22"/>
+      <c r="DG234" s="22"/>
+      <c r="DH234" s="22"/>
+      <c r="DI234" s="22"/>
+      <c r="DJ234" s="22"/>
+      <c r="DK234" s="22"/>
+      <c r="DL234" s="22"/>
+      <c r="DM234" s="22"/>
+      <c r="DN234" s="22"/>
+      <c r="DO234" s="22"/>
+      <c r="DP234" s="22"/>
+      <c r="DQ234" s="22"/>
+      <c r="DR234" s="22"/>
+      <c r="DS234" s="22"/>
+      <c r="DT234" s="22"/>
+      <c r="DU234" s="22"/>
+      <c r="DV234" s="22"/>
+      <c r="DW234" s="22"/>
+      <c r="DX234" s="22"/>
+      <c r="DY234" s="22"/>
+      <c r="DZ234" s="22"/>
+      <c r="EA234" s="22"/>
+      <c r="EB234" s="22"/>
+      <c r="EC234" s="22"/>
+      <c r="ED234" s="22"/>
+      <c r="EE234" s="22"/>
+      <c r="EF234" s="22"/>
+      <c r="EG234" s="22"/>
+      <c r="EH234" s="22"/>
+      <c r="EI234" s="22"/>
+      <c r="EJ234" s="22"/>
+      <c r="EK234" s="22"/>
+      <c r="EL234" s="22"/>
+      <c r="EM234" s="22"/>
+      <c r="EN234" s="22"/>
+      <c r="EO234" s="22"/>
+      <c r="EP234" s="22"/>
+      <c r="EQ234" s="22"/>
+      <c r="ER234" s="22"/>
+      <c r="ES234" s="22"/>
+      <c r="ET234" s="22"/>
+      <c r="EU234" s="22"/>
+      <c r="EV234" s="22"/>
+      <c r="EW234" s="22"/>
+      <c r="EX234" s="22"/>
+      <c r="EY234" s="22"/>
+      <c r="EZ234" s="22"/>
+      <c r="FA234" s="22"/>
+      <c r="FB234" s="22"/>
+      <c r="FC234" s="22"/>
+      <c r="FD234" s="22"/>
+      <c r="FE234" s="22"/>
+      <c r="FF234" s="22"/>
+      <c r="FG234" s="22"/>
+      <c r="FH234" s="22"/>
+      <c r="FI234" s="22"/>
+      <c r="FJ234" s="22"/>
+      <c r="FK234" s="22"/>
+      <c r="FL234" s="22"/>
+      <c r="FM234" s="22"/>
+      <c r="FN234" s="22"/>
+      <c r="FO234" s="22"/>
+      <c r="FP234" s="22"/>
+      <c r="FQ234" s="22"/>
+      <c r="FR234" s="22"/>
+      <c r="FS234" s="22"/>
+      <c r="FT234" s="22"/>
+      <c r="FU234" s="22"/>
+      <c r="FV234" s="22"/>
+      <c r="FW234" s="22"/>
+      <c r="FX234" s="22"/>
+      <c r="FY234" s="22"/>
+      <c r="FZ234" s="22"/>
+      <c r="GA234" s="22"/>
+      <c r="GB234" s="22"/>
+      <c r="GC234" s="22"/>
+      <c r="GD234" s="22"/>
+      <c r="GE234" s="22"/>
+      <c r="GF234" s="22"/>
+      <c r="GG234" s="22"/>
+      <c r="GH234" s="22"/>
+      <c r="GI234" s="22"/>
+      <c r="GJ234" s="22"/>
+      <c r="GK234" s="22"/>
+      <c r="GL234" s="22"/>
+      <c r="GM234" s="22"/>
+      <c r="GN234" s="22"/>
+      <c r="GO234" s="22"/>
+      <c r="GP234" s="22"/>
+      <c r="GQ234" s="22"/>
+      <c r="GR234" s="22"/>
+      <c r="GS234" s="22"/>
+      <c r="GT234" s="22"/>
+      <c r="GU234" s="22"/>
+      <c r="GV234" s="22"/>
+      <c r="GW234" s="22"/>
+      <c r="GX234" s="22"/>
+      <c r="GY234" s="22"/>
+      <c r="GZ234" s="22"/>
+      <c r="HA234" s="22"/>
+      <c r="HB234" s="22"/>
+      <c r="HC234" s="22"/>
+      <c r="HD234" s="22"/>
+      <c r="HE234" s="22"/>
+      <c r="HF234" s="22"/>
+      <c r="HG234" s="22"/>
+      <c r="HH234" s="22"/>
+      <c r="HI234" s="22"/>
+      <c r="HJ234" s="22"/>
+      <c r="HK234" s="22"/>
+      <c r="HL234" s="22"/>
+      <c r="HM234" s="22"/>
+      <c r="HN234" s="22"/>
+      <c r="HO234" s="22"/>
+      <c r="HP234" s="22"/>
+      <c r="HQ234" s="22"/>
+      <c r="HR234" s="22"/>
+      <c r="HS234" s="22"/>
+      <c r="HT234" s="22"/>
+      <c r="HU234" s="22"/>
+      <c r="HV234" s="22"/>
+      <c r="HW234" s="22"/>
+      <c r="HX234" s="22"/>
+      <c r="HY234" s="22"/>
+      <c r="HZ234" s="22"/>
+      <c r="IA234" s="22"/>
+      <c r="IB234" s="22"/>
+      <c r="IC234" s="22"/>
+      <c r="ID234" s="22"/>
+      <c r="IE234" s="22"/>
+      <c r="IF234" s="22"/>
+      <c r="IG234" s="22"/>
+      <c r="IH234" s="22"/>
+      <c r="II234" s="22"/>
+      <c r="IJ234" s="22"/>
+      <c r="IK234" s="22"/>
+      <c r="IL234" s="22"/>
+      <c r="IM234" s="22"/>
+      <c r="IN234" s="22"/>
+      <c r="IO234" s="22"/>
+      <c r="IP234" s="22"/>
+      <c r="IQ234" s="22"/>
+      <c r="IR234" s="22"/>
+      <c r="IS234" s="22"/>
+      <c r="IT234" s="22"/>
+    </row>
+    <row r="241" spans="5:254" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E241" s="2"/>
+      <c r="F241" s="2"/>
+      <c r="G241" s="2"/>
+      <c r="H241" s="2"/>
+      <c r="I241" s="2"/>
+      <c r="J241" s="2"/>
+      <c r="K241" s="2"/>
+      <c r="L241" s="2"/>
+      <c r="M241" s="2"/>
+      <c r="N241" s="2"/>
+      <c r="O241" s="2"/>
+      <c r="P241" s="2"/>
+      <c r="Q241" s="2"/>
+      <c r="R241" s="2"/>
+      <c r="S241" s="2"/>
+      <c r="T241" s="2"/>
+      <c r="U241" s="2"/>
+      <c r="V241" s="2"/>
+      <c r="W241" s="2"/>
+      <c r="X241" s="2"/>
+      <c r="Y241" s="2"/>
+      <c r="Z241" s="2"/>
+      <c r="AA241" s="2"/>
+      <c r="AB241" s="2"/>
+      <c r="AC241" s="2"/>
+      <c r="AD241" s="2"/>
+      <c r="AE241" s="2"/>
+      <c r="AF241" s="2"/>
+      <c r="AG241" s="2"/>
+      <c r="AH241" s="2"/>
+      <c r="AI241" s="2"/>
+      <c r="AJ241" s="2"/>
+      <c r="AK241" s="2"/>
+      <c r="AL241" s="2"/>
+      <c r="AM241" s="2"/>
+      <c r="AN241" s="2"/>
+      <c r="AO241" s="2"/>
+      <c r="AP241" s="2"/>
+      <c r="AQ241" s="2"/>
+      <c r="AR241" s="2"/>
+      <c r="AS241" s="2"/>
+      <c r="AT241" s="2"/>
+      <c r="AU241" s="2"/>
+      <c r="AV241" s="2"/>
+      <c r="AW241" s="2"/>
+      <c r="AX241" s="2"/>
+      <c r="AY241" s="2"/>
+      <c r="AZ241" s="2"/>
+      <c r="BA241" s="2"/>
+      <c r="BB241" s="2"/>
+      <c r="BC241" s="2"/>
+      <c r="BD241" s="2"/>
+      <c r="BE241" s="2"/>
+      <c r="BF241" s="2"/>
+      <c r="BG241" s="2"/>
+      <c r="BH241" s="2"/>
+      <c r="BI241" s="2"/>
+      <c r="BJ241" s="2"/>
+      <c r="BK241" s="2"/>
+      <c r="BL241" s="2"/>
+      <c r="BM241" s="2"/>
+      <c r="BN241" s="2"/>
+      <c r="BO241" s="2"/>
+      <c r="BP241" s="2"/>
+      <c r="BQ241" s="2"/>
+      <c r="BR241" s="2"/>
+      <c r="BS241" s="2"/>
+      <c r="BT241" s="2"/>
+      <c r="BU241" s="2"/>
+      <c r="BV241" s="2"/>
+      <c r="BW241" s="2"/>
+      <c r="BX241" s="2"/>
+      <c r="BY241" s="2"/>
+      <c r="BZ241" s="2"/>
+      <c r="CA241" s="2"/>
+      <c r="CB241" s="2"/>
+      <c r="CC241" s="2"/>
+      <c r="CD241" s="2"/>
+      <c r="CE241" s="2"/>
+      <c r="CF241" s="2"/>
+      <c r="CG241" s="2"/>
+      <c r="CH241" s="2"/>
+      <c r="CI241" s="2"/>
+      <c r="CJ241" s="2"/>
+      <c r="CK241" s="2"/>
+      <c r="CL241" s="2"/>
+      <c r="CM241" s="2"/>
+      <c r="CN241" s="2"/>
+      <c r="CO241" s="2"/>
+      <c r="CP241" s="2"/>
+      <c r="CQ241" s="2"/>
+      <c r="CR241" s="2"/>
+      <c r="CS241" s="2"/>
+      <c r="CT241" s="2"/>
+      <c r="CU241" s="2"/>
+      <c r="CV241" s="2"/>
+      <c r="CW241" s="2"/>
+      <c r="CX241" s="2"/>
+      <c r="CY241" s="2"/>
+      <c r="CZ241" s="2"/>
+      <c r="DA241" s="2"/>
+      <c r="DB241" s="2"/>
+      <c r="DC241" s="2"/>
+      <c r="DD241" s="2"/>
+      <c r="DE241" s="2"/>
+      <c r="DF241" s="2"/>
+      <c r="DG241" s="2"/>
+      <c r="DH241" s="2"/>
+      <c r="DI241" s="2"/>
+      <c r="DJ241" s="2"/>
+      <c r="DK241" s="2"/>
+      <c r="DL241" s="2"/>
+      <c r="DM241" s="2"/>
+      <c r="DN241" s="2"/>
+      <c r="DO241" s="2"/>
+      <c r="DP241" s="2"/>
+      <c r="DQ241" s="2"/>
+      <c r="DR241" s="2"/>
+      <c r="DS241" s="2"/>
+      <c r="DT241" s="2"/>
+      <c r="DU241" s="2"/>
+      <c r="DV241" s="2"/>
+      <c r="DW241" s="2"/>
+      <c r="DX241" s="2"/>
+      <c r="DY241" s="2"/>
+      <c r="DZ241" s="2"/>
+      <c r="EA241" s="2"/>
+      <c r="EB241" s="2"/>
+      <c r="EC241" s="2"/>
+      <c r="ED241" s="2"/>
+      <c r="EE241" s="2"/>
+      <c r="EF241" s="2"/>
+      <c r="EG241" s="2"/>
+      <c r="EH241" s="2"/>
+      <c r="EI241" s="2"/>
+      <c r="EJ241" s="2"/>
+      <c r="EK241" s="2"/>
+      <c r="EL241" s="2"/>
+      <c r="EM241" s="2"/>
+      <c r="EN241" s="2"/>
+      <c r="EO241" s="2"/>
+      <c r="EP241" s="2"/>
+      <c r="EQ241" s="2"/>
+      <c r="ER241" s="2"/>
+      <c r="ES241" s="2"/>
+      <c r="ET241" s="2"/>
+      <c r="EU241" s="2"/>
+      <c r="EV241" s="2"/>
+      <c r="EW241" s="2"/>
+      <c r="EX241" s="2"/>
+      <c r="EY241" s="2"/>
+      <c r="EZ241" s="2"/>
+      <c r="FA241" s="2"/>
+      <c r="FB241" s="2"/>
+      <c r="FC241" s="2"/>
+      <c r="FD241" s="2"/>
+      <c r="FE241" s="2"/>
+      <c r="FF241" s="2"/>
+      <c r="FG241" s="2"/>
+      <c r="FH241" s="2"/>
+      <c r="FI241" s="2"/>
+      <c r="FJ241" s="2"/>
+      <c r="FK241" s="2"/>
+      <c r="FL241" s="2"/>
+      <c r="FM241" s="2"/>
+      <c r="FN241" s="2"/>
+      <c r="FO241" s="2"/>
+      <c r="FP241" s="2"/>
+      <c r="FQ241" s="2"/>
+      <c r="FR241" s="2"/>
+      <c r="FS241" s="2"/>
+      <c r="FT241" s="2"/>
+      <c r="FU241" s="2"/>
+      <c r="FV241" s="2"/>
+      <c r="FW241" s="2"/>
+      <c r="FX241" s="2"/>
+      <c r="FY241" s="2"/>
+      <c r="FZ241" s="2"/>
+      <c r="GA241" s="2"/>
+      <c r="GB241" s="2"/>
+      <c r="GC241" s="2"/>
+      <c r="GD241" s="2"/>
+      <c r="GE241" s="2"/>
+      <c r="GF241" s="2"/>
+      <c r="GG241" s="2"/>
+      <c r="GH241" s="2"/>
+      <c r="GI241" s="2"/>
+      <c r="GJ241" s="2"/>
+      <c r="GK241" s="2"/>
+      <c r="GL241" s="2"/>
+      <c r="GM241" s="2"/>
+      <c r="GN241" s="2"/>
+      <c r="GO241" s="2"/>
+      <c r="GP241" s="2"/>
+      <c r="GQ241" s="2"/>
+      <c r="GR241" s="2"/>
+      <c r="GS241" s="2"/>
+      <c r="GT241" s="2"/>
+      <c r="GU241" s="2"/>
+      <c r="GV241" s="2"/>
+      <c r="GW241" s="2"/>
+      <c r="GX241" s="2"/>
+      <c r="GY241" s="2"/>
+      <c r="GZ241" s="2"/>
+      <c r="HA241" s="2"/>
+      <c r="HB241" s="2"/>
+      <c r="HC241" s="2"/>
+      <c r="HD241" s="2"/>
+      <c r="HE241" s="2"/>
+      <c r="HF241" s="2"/>
+      <c r="HG241" s="2"/>
+      <c r="HH241" s="2"/>
+      <c r="HI241" s="2"/>
+      <c r="HJ241" s="2"/>
+      <c r="HK241" s="2"/>
+      <c r="HL241" s="2"/>
+      <c r="HM241" s="2"/>
+      <c r="HN241" s="2"/>
+      <c r="HO241" s="2"/>
+      <c r="HP241" s="2"/>
+      <c r="HQ241" s="2"/>
+      <c r="HR241" s="2"/>
+      <c r="HS241" s="2"/>
+      <c r="HT241" s="2"/>
+      <c r="HU241" s="2"/>
+      <c r="HV241" s="2"/>
+      <c r="HW241" s="2"/>
+      <c r="HX241" s="2"/>
+      <c r="HY241" s="2"/>
+      <c r="HZ241" s="2"/>
+      <c r="IA241" s="2"/>
+      <c r="IB241" s="2"/>
+      <c r="IC241" s="2"/>
+      <c r="ID241" s="2"/>
+      <c r="IE241" s="2"/>
+      <c r="IF241" s="2"/>
+      <c r="IG241" s="2"/>
+      <c r="IH241" s="2"/>
+      <c r="II241" s="2"/>
+      <c r="IJ241" s="2"/>
+      <c r="IK241" s="2"/>
+      <c r="IL241" s="2"/>
+      <c r="IM241" s="2"/>
+      <c r="IN241" s="2"/>
+      <c r="IO241" s="2"/>
+      <c r="IP241" s="2"/>
+      <c r="IQ241" s="2"/>
+      <c r="IR241" s="2"/>
+      <c r="IS241" s="2"/>
+      <c r="IT241" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -63058,7 +63596,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -63067,7 +63605,7 @@
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="7" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="5"/>
@@ -63075,27 +63613,27 @@
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="7" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="8" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="7" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="8" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="7" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="8"/>
@@ -63103,7 +63641,7 @@
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="7" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="8"/>

</xml_diff>

<commit_message>
Renamed Premium Rate Fraud and Click Fraud to 'Perform..' under Fraud for consistency
</commit_message>
<xml_diff>
--- a/mind_maps/malware_capabilities_descriptions.xlsx
+++ b/mind_maps/malware_capabilities_descriptions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="156" windowWidth="15960" windowHeight="9516" tabRatio="543"/>
+    <workbookView xWindow="0" yWindow="216" windowWidth="15960" windowHeight="9456" tabRatio="543"/>
   </bookViews>
   <sheets>
     <sheet name="malware_capabilities" sheetId="1" r:id="rId1"/>
@@ -593,16 +593,10 @@
     <t>Fraud</t>
   </si>
   <si>
-    <t xml:space="preserve"> Premium Rate Fraud</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Access Premium Service</t>
   </si>
   <si>
     <t>The 'access premium service' value indicates that the malware instance is able to access a premium service.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Click Fraud</t>
   </si>
   <si>
     <t>The ‘security degradation’ Capability indicates that the malware instance is able to bypass or disable security features and/or controls.</t>
@@ -993,12 +987,6 @@
   </si>
   <si>
     <t>The 'fraud' Capability indicates that the malware instance is able to defraud a user or a system.</t>
-  </si>
-  <si>
-    <t>The 'premium rate fraud' value indicates that the malware instance is able to send text messages or dial phone numbers that are charged at premium rates.</t>
-  </si>
-  <si>
-    <t>The 'click fraud' value indicates that the malware instance is able to simulate clicks on website advertisements for the purpose of revenue generation.</t>
   </si>
   <si>
     <t>The 'defeat linear disassembler' value indicates that the malware instance is able to prevent its disassembly in a linear disassembler.</t>
@@ -1525,6 +1513,18 @@
   </si>
   <si>
     <t>The 'prevent duplicate infection' value indicates that the malware instance is able to prevent itself from infecting a machine multiple times.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Perform Premium Rate Fraud</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Perform Click Fraud</t>
+  </si>
+  <si>
+    <t>The 'perform premium rate fraud' value indicates that the malware instance is able to send text messages or dial phone numbers that are charged at premium rates.</t>
+  </si>
+  <si>
+    <t>The 'perform click fraud' value indicates that the malware instance is able to simulate clicks on website advertisements for the purpose of revenue generation.</t>
   </si>
 </sst>
 </file>
@@ -2094,8 +2094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IT242"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A214" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C223" sqref="C223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.61328125" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -2128,7 +2128,7 @@
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
       <c r="D2" s="14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
@@ -2386,11 +2386,11 @@
         <v>5</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="16" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="E3" s="22"/>
       <c r="F3" s="22"/>
@@ -2652,7 +2652,7 @@
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="16" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E4" s="22"/>
       <c r="F4" s="22"/>
@@ -2916,7 +2916,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E5" s="22"/>
       <c r="F5" s="22"/>
@@ -3173,10 +3173,10 @@
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="24" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="22"/>
@@ -3440,7 +3440,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="E7" s="22"/>
       <c r="F7" s="22"/>
@@ -3704,7 +3704,7 @@
         <v>9</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="E8" s="22"/>
       <c r="F8" s="22"/>
@@ -3966,7 +3966,7 @@
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="16" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E9" s="22"/>
       <c r="F9" s="22"/>
@@ -4230,7 +4230,7 @@
         <v>11</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
@@ -4494,7 +4494,7 @@
         <v>12</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
@@ -4751,10 +4751,10 @@
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="20" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
@@ -5014,7 +5014,7 @@
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="D13" s="16" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E13" s="22"/>
       <c r="F13" s="22"/>
@@ -5276,7 +5276,7 @@
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="16" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E14" s="22"/>
       <c r="F14" s="22"/>
@@ -5540,7 +5540,7 @@
         <v>15</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E15" s="22"/>
       <c r="F15" s="22"/>
@@ -5804,7 +5804,7 @@
         <v>16</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E16" s="22"/>
       <c r="F16" s="22"/>
@@ -6066,7 +6066,7 @@
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="16" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E17" s="22"/>
       <c r="F17" s="22"/>
@@ -6330,7 +6330,7 @@
         <v>18</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
@@ -6590,7 +6590,7 @@
         <v>19</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
@@ -6854,7 +6854,7 @@
         <v>20</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
@@ -7114,7 +7114,7 @@
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="16" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
@@ -7376,7 +7376,7 @@
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="16" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
@@ -7640,7 +7640,7 @@
         <v>23</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E23" s="22"/>
       <c r="F23" s="22"/>
@@ -7904,7 +7904,7 @@
         <v>24</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E24" s="22"/>
       <c r="F24" s="22"/>
@@ -8166,7 +8166,7 @@
       </c>
       <c r="C25" s="15"/>
       <c r="D25" s="16" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E25" s="22"/>
       <c r="F25" s="22"/>
@@ -8430,7 +8430,7 @@
         <v>26</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
@@ -8694,7 +8694,7 @@
         <v>27</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E27" s="22"/>
       <c r="F27" s="22"/>
@@ -8958,7 +8958,7 @@
         <v>28</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E28" s="22"/>
       <c r="F28" s="22"/>
@@ -9222,7 +9222,7 @@
         <v>29</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
@@ -9486,7 +9486,7 @@
         <v>30</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="E30" s="22"/>
       <c r="F30" s="22"/>
@@ -9748,7 +9748,7 @@
       </c>
       <c r="C31" s="15"/>
       <c r="D31" s="16" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E31" s="22"/>
       <c r="F31" s="22"/>
@@ -10012,7 +10012,7 @@
         <v>32</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E32" s="22"/>
       <c r="F32" s="22"/>
@@ -10540,7 +10540,7 @@
         <v>35</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E34" s="22"/>
       <c r="F34" s="22"/>
@@ -10800,7 +10800,7 @@
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
       <c r="D35" s="16" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E35" s="22"/>
       <c r="F35" s="22"/>
@@ -11062,7 +11062,7 @@
       </c>
       <c r="C36" s="15"/>
       <c r="D36" s="16" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E36" s="22"/>
       <c r="F36" s="22"/>
@@ -11326,7 +11326,7 @@
         <v>38</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E37" s="22"/>
       <c r="F37" s="22"/>
@@ -11590,7 +11590,7 @@
         <v>39</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E38" s="22"/>
       <c r="F38" s="22"/>
@@ -11854,7 +11854,7 @@
         <v>40</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E39" s="22"/>
       <c r="F39" s="22"/>
@@ -12116,7 +12116,7 @@
       </c>
       <c r="C40" s="15"/>
       <c r="D40" s="16" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E40" s="22"/>
       <c r="F40" s="22"/>
@@ -12380,7 +12380,7 @@
         <v>42</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E41" s="22"/>
       <c r="F41" s="22"/>
@@ -12644,7 +12644,7 @@
         <v>43</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E42" s="22"/>
       <c r="F42" s="22"/>
@@ -12904,7 +12904,7 @@
         <v>44</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E43" s="22"/>
       <c r="F43" s="22"/>
@@ -13164,7 +13164,7 @@
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
       <c r="D44" s="16" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E44" s="22"/>
       <c r="F44" s="22"/>
@@ -13426,7 +13426,7 @@
       </c>
       <c r="C45" s="15"/>
       <c r="D45" s="16" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E45" s="22"/>
       <c r="F45" s="22"/>
@@ -13690,7 +13690,7 @@
         <v>47</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E46" s="22"/>
       <c r="F46" s="22"/>
@@ -13954,7 +13954,7 @@
         <v>48</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E47" s="22"/>
       <c r="F47" s="22"/>
@@ -14218,7 +14218,7 @@
         <v>49</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E48" s="22"/>
       <c r="F48" s="22"/>
@@ -14482,7 +14482,7 @@
         <v>50</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E49" s="22"/>
       <c r="F49" s="22"/>
@@ -14746,7 +14746,7 @@
         <v>51</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="E50" s="22"/>
       <c r="F50" s="22"/>
@@ -15008,7 +15008,7 @@
       </c>
       <c r="C51" s="15"/>
       <c r="D51" s="16" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E51" s="22"/>
       <c r="F51" s="22"/>
@@ -15272,7 +15272,7 @@
         <v>53</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E52" s="22"/>
       <c r="F52" s="22"/>
@@ -15536,7 +15536,7 @@
         <v>54</v>
       </c>
       <c r="D53" s="16" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E53" s="22"/>
       <c r="F53" s="22"/>
@@ -15800,7 +15800,7 @@
         <v>55</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E54" s="22"/>
       <c r="F54" s="22"/>
@@ -16064,7 +16064,7 @@
         <v>56</v>
       </c>
       <c r="D55" s="16" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E55" s="22"/>
       <c r="F55" s="22"/>
@@ -16328,7 +16328,7 @@
         <v>57</v>
       </c>
       <c r="D56" s="16" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E56" s="22"/>
       <c r="F56" s="22"/>
@@ -16592,7 +16592,7 @@
         <v>58</v>
       </c>
       <c r="D57" s="16" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="E57" s="22"/>
       <c r="F57" s="22"/>
@@ -16856,7 +16856,7 @@
         <v>59</v>
       </c>
       <c r="D58" s="16" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="E58" s="22"/>
       <c r="F58" s="22"/>
@@ -17120,7 +17120,7 @@
         <v>60</v>
       </c>
       <c r="D59" s="16" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E59" s="22"/>
       <c r="F59" s="22"/>
@@ -17382,7 +17382,7 @@
       </c>
       <c r="C60" s="15"/>
       <c r="D60" s="16" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E60" s="22"/>
       <c r="F60" s="22"/>
@@ -17646,7 +17646,7 @@
         <v>62</v>
       </c>
       <c r="D61" s="16" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E61" s="22"/>
       <c r="F61" s="22"/>
@@ -17910,7 +17910,7 @@
         <v>63</v>
       </c>
       <c r="D62" s="16" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E62" s="22"/>
       <c r="F62" s="22"/>
@@ -18174,7 +18174,7 @@
         <v>64</v>
       </c>
       <c r="D63" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E63" s="22"/>
       <c r="F63" s="22"/>
@@ -18436,7 +18436,7 @@
       </c>
       <c r="C64" s="15"/>
       <c r="D64" s="16" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E64" s="22"/>
       <c r="F64" s="22"/>
@@ -18700,7 +18700,7 @@
         <v>66</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="E65" s="22"/>
       <c r="F65" s="22"/>
@@ -18962,7 +18962,7 @@
       </c>
       <c r="C66" s="15"/>
       <c r="D66" s="16" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="E66" s="22"/>
       <c r="F66" s="22"/>
@@ -19226,7 +19226,7 @@
         <v>68</v>
       </c>
       <c r="D67" s="16" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E67" s="22"/>
       <c r="F67" s="22"/>
@@ -19752,7 +19752,7 @@
       </c>
       <c r="C69" s="15"/>
       <c r="D69" s="16" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E69" s="22"/>
       <c r="F69" s="22"/>
@@ -20016,7 +20016,7 @@
         <v>72</v>
       </c>
       <c r="D70" s="16" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E70" s="22"/>
       <c r="F70" s="22"/>
@@ -20276,7 +20276,7 @@
       <c r="B71" s="15"/>
       <c r="C71" s="15"/>
       <c r="D71" s="16" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E71" s="22"/>
       <c r="F71" s="22"/>
@@ -20538,7 +20538,7 @@
       </c>
       <c r="C72" s="15"/>
       <c r="D72" s="16" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="E72" s="22"/>
       <c r="F72" s="22"/>
@@ -20802,7 +20802,7 @@
         <v>75</v>
       </c>
       <c r="D73" s="16" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E73" s="22"/>
       <c r="F73" s="22"/>
@@ -21066,7 +21066,7 @@
         <v>76</v>
       </c>
       <c r="D74" s="16" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E74" s="22"/>
       <c r="F74" s="22"/>
@@ -21330,7 +21330,7 @@
         <v>77</v>
       </c>
       <c r="D75" s="16" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E75" s="22"/>
       <c r="F75" s="22"/>
@@ -21856,7 +21856,7 @@
         <v>80</v>
       </c>
       <c r="D77" s="16" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E77" s="22"/>
       <c r="F77" s="22"/>
@@ -22118,7 +22118,7 @@
       </c>
       <c r="C78" s="15"/>
       <c r="D78" s="16" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E78" s="22"/>
       <c r="F78" s="22"/>
@@ -22640,11 +22640,11 @@
         <v>5</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="C80" s="15"/>
       <c r="D80" s="16" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="E80" s="22"/>
       <c r="F80" s="22"/>
@@ -22905,10 +22905,10 @@
         <v>5</v>
       </c>
       <c r="C81" s="13" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="D81" s="16" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="E81" s="22"/>
       <c r="F81" s="22"/>
@@ -23168,7 +23168,7 @@
       <c r="B82" s="15"/>
       <c r="C82" s="15"/>
       <c r="D82" s="16" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E82" s="22"/>
       <c r="F82" s="22"/>
@@ -23430,7 +23430,7 @@
       </c>
       <c r="C83" s="15"/>
       <c r="D83" s="16" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="E83" s="22"/>
       <c r="F83" s="22"/>
@@ -23694,7 +23694,7 @@
         <v>86</v>
       </c>
       <c r="D84" s="16" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E84" s="22"/>
       <c r="F84" s="22"/>
@@ -23956,7 +23956,7 @@
       </c>
       <c r="C85" s="15"/>
       <c r="D85" s="16" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="E85" s="22"/>
       <c r="F85" s="22"/>
@@ -24748,7 +24748,7 @@
         <v>92</v>
       </c>
       <c r="D88" s="16" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E88" s="22"/>
       <c r="F88" s="22"/>
@@ -25009,10 +25009,10 @@
         <v>5</v>
       </c>
       <c r="C89" s="13" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="D89" s="16" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="E89" s="22"/>
       <c r="F89" s="22"/>
@@ -25270,7 +25270,7 @@
         <v>5</v>
       </c>
       <c r="B90" s="13" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C90" s="15"/>
       <c r="D90" s="16" t="s">
@@ -25538,7 +25538,7 @@
         <v>94</v>
       </c>
       <c r="D91" s="16" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="E91" s="22"/>
       <c r="F91" s="22"/>
@@ -26066,7 +26066,7 @@
         <v>97</v>
       </c>
       <c r="D93" s="21" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E93" s="22"/>
       <c r="F93" s="22"/>
@@ -26328,7 +26328,7 @@
       </c>
       <c r="C94" s="15"/>
       <c r="D94" s="21" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E94" s="22"/>
       <c r="F94" s="22"/>
@@ -26592,7 +26592,7 @@
         <v>99</v>
       </c>
       <c r="D95" s="21" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E95" s="22"/>
       <c r="F95" s="22"/>
@@ -26856,7 +26856,7 @@
         <v>100</v>
       </c>
       <c r="D96" s="21" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E96" s="22"/>
       <c r="F96" s="22"/>
@@ -27118,7 +27118,7 @@
       </c>
       <c r="C97" s="15"/>
       <c r="D97" s="21" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E97" s="22"/>
       <c r="F97" s="22"/>
@@ -27382,7 +27382,7 @@
         <v>102</v>
       </c>
       <c r="D98" s="21" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E98" s="22"/>
       <c r="F98" s="22"/>
@@ -27646,7 +27646,7 @@
         <v>103</v>
       </c>
       <c r="D99" s="21" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E99" s="22"/>
       <c r="F99" s="22"/>
@@ -27910,7 +27910,7 @@
         <v>104</v>
       </c>
       <c r="D100" s="21" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="E100" s="22"/>
       <c r="F100" s="22"/>
@@ -28174,7 +28174,7 @@
         <v>105</v>
       </c>
       <c r="D101" s="21" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E101" s="22"/>
       <c r="F101" s="22"/>
@@ -28438,7 +28438,7 @@
         <v>106</v>
       </c>
       <c r="D102" s="21" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E102" s="22"/>
       <c r="F102" s="22"/>
@@ -28698,7 +28698,7 @@
       <c r="B103" s="15"/>
       <c r="C103" s="15"/>
       <c r="D103" s="14" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="E103" s="22"/>
       <c r="F103" s="22"/>
@@ -28958,7 +28958,7 @@
       </c>
       <c r="C104" s="13"/>
       <c r="D104" s="14" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E104" s="22"/>
       <c r="F104" s="22"/>
@@ -29215,10 +29215,10 @@
       <c r="A105" s="13"/>
       <c r="B105" s="13"/>
       <c r="C105" s="14" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="D105" s="14" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E105" s="22"/>
       <c r="F105" s="22"/>
@@ -29476,11 +29476,11 @@
         <v>5</v>
       </c>
       <c r="B106" s="20" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="C106" s="15"/>
       <c r="D106" s="14" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="E106" s="22"/>
       <c r="F106" s="22"/>
@@ -29741,10 +29741,10 @@
         <v>5</v>
       </c>
       <c r="C107" s="20" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="D107" s="14" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="E107" s="22"/>
       <c r="F107" s="22"/>
@@ -30005,10 +30005,10 @@
         <v>5</v>
       </c>
       <c r="C108" s="20" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D108" s="14" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="E108" s="22"/>
       <c r="F108" s="22"/>
@@ -30265,10 +30265,10 @@
       <c r="A109" s="15"/>
       <c r="B109" s="20"/>
       <c r="C109" s="25" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="D109" s="14" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="E109" s="22"/>
       <c r="F109" s="22"/>
@@ -30524,11 +30524,11 @@
     <row r="110" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A110" s="15"/>
       <c r="B110" s="20" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="C110" s="15"/>
       <c r="D110" s="14" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="E110" s="22"/>
       <c r="F110" s="22"/>
@@ -30785,10 +30785,10 @@
       <c r="A111" s="15"/>
       <c r="B111" s="15"/>
       <c r="C111" s="13" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="D111" s="14" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="E111" s="22"/>
       <c r="F111" s="22"/>
@@ -31045,10 +31045,10 @@
       <c r="A112" s="15"/>
       <c r="B112" s="15"/>
       <c r="C112" s="13" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="D112" s="14" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="E112" s="22"/>
       <c r="F112" s="22"/>
@@ -31305,10 +31305,10 @@
       <c r="A113" s="15"/>
       <c r="B113" s="15"/>
       <c r="C113" s="20" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D113" s="14" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="E113" s="22"/>
       <c r="F113" s="22"/>
@@ -31563,12 +31563,12 @@
     </row>
     <row r="114" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A114" s="20" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="B114" s="15"/>
       <c r="C114" s="15"/>
       <c r="D114" s="14" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="E114" s="22"/>
       <c r="F114" s="22"/>
@@ -31824,11 +31824,11 @@
     <row r="115" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A115" s="13"/>
       <c r="B115" s="20" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="C115" s="13"/>
       <c r="D115" s="14" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="E115" s="22"/>
       <c r="F115" s="22"/>
@@ -32086,11 +32086,11 @@
         <v>5</v>
       </c>
       <c r="B116" s="20" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C116" s="15"/>
       <c r="D116" s="14" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="E116" s="22"/>
       <c r="F116" s="22"/>
@@ -32351,10 +32351,10 @@
         <v>5</v>
       </c>
       <c r="C117" s="13" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="D117" s="14" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="E117" s="22"/>
       <c r="F117" s="22"/>
@@ -32614,7 +32614,7 @@
       <c r="B118" s="15"/>
       <c r="C118" s="15"/>
       <c r="D118" s="14" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="E118" s="22"/>
       <c r="F118" s="22"/>
@@ -32876,7 +32876,7 @@
       </c>
       <c r="C119" s="15"/>
       <c r="D119" s="14" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="E119" s="22"/>
       <c r="F119" s="22"/>
@@ -33138,7 +33138,7 @@
       </c>
       <c r="C120" s="15"/>
       <c r="D120" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E120" s="22"/>
       <c r="F120" s="22"/>
@@ -33402,7 +33402,7 @@
         <v>112</v>
       </c>
       <c r="D121" s="14" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E121" s="22"/>
       <c r="F121" s="22"/>
@@ -33662,7 +33662,7 @@
       <c r="B122" s="15"/>
       <c r="C122" s="15"/>
       <c r="D122" s="14" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E122" s="22"/>
       <c r="F122" s="22"/>
@@ -33924,7 +33924,7 @@
       </c>
       <c r="C123" s="15"/>
       <c r="D123" s="14" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E123" s="22"/>
       <c r="F123" s="22"/>
@@ -34188,7 +34188,7 @@
         <v>115</v>
       </c>
       <c r="D124" s="14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E124" s="22"/>
       <c r="F124" s="22"/>
@@ -34450,7 +34450,7 @@
       </c>
       <c r="C125" s="15"/>
       <c r="D125" s="14" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E125" s="22"/>
       <c r="F125" s="22"/>
@@ -34710,7 +34710,7 @@
       <c r="B126" s="15"/>
       <c r="C126" s="15"/>
       <c r="D126" s="14" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E126" s="22"/>
       <c r="F126" s="22"/>
@@ -34972,7 +34972,7 @@
       </c>
       <c r="C127" s="15"/>
       <c r="D127" s="14" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E127" s="22"/>
       <c r="F127" s="22"/>
@@ -35236,7 +35236,7 @@
         <v>119</v>
       </c>
       <c r="D128" s="14" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E128" s="22"/>
       <c r="F128" s="22"/>
@@ -35500,7 +35500,7 @@
         <v>120</v>
       </c>
       <c r="D129" s="14" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E129" s="22"/>
       <c r="F129" s="22"/>
@@ -35762,7 +35762,7 @@
       </c>
       <c r="C130" s="15"/>
       <c r="D130" s="14" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E130" s="22"/>
       <c r="F130" s="22"/>
@@ -36026,7 +36026,7 @@
         <v>122</v>
       </c>
       <c r="D131" s="14" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E131" s="22"/>
       <c r="F131" s="22"/>
@@ -36290,7 +36290,7 @@
         <v>123</v>
       </c>
       <c r="D132" s="14" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E132" s="22"/>
       <c r="F132" s="22"/>
@@ -36548,11 +36548,11 @@
         <v>5</v>
       </c>
       <c r="B133" s="20" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C133" s="15"/>
       <c r="D133" s="14" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E133" s="22"/>
       <c r="F133" s="22"/>
@@ -36816,7 +36816,7 @@
         <v>124</v>
       </c>
       <c r="D134" s="14" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E134" s="22"/>
       <c r="F134" s="22"/>
@@ -37080,7 +37080,7 @@
         <v>125</v>
       </c>
       <c r="D135" s="14" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="E135" s="22"/>
       <c r="F135" s="22"/>
@@ -37344,7 +37344,7 @@
         <v>126</v>
       </c>
       <c r="D136" s="14" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E136" s="22"/>
       <c r="F136" s="22"/>
@@ -37608,7 +37608,7 @@
         <v>127</v>
       </c>
       <c r="D137" s="14" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E137" s="22"/>
       <c r="F137" s="22"/>
@@ -37872,7 +37872,7 @@
         <v>128</v>
       </c>
       <c r="D138" s="14" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E138" s="22"/>
       <c r="F138" s="22"/>
@@ -38136,7 +38136,7 @@
         <v>129</v>
       </c>
       <c r="D139" s="14" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E139" s="22"/>
       <c r="F139" s="22"/>
@@ -38391,12 +38391,12 @@
     </row>
     <row r="140" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A140" s="26" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="B140" s="15"/>
       <c r="C140" s="15"/>
       <c r="D140" s="14" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="E140" s="22"/>
       <c r="F140" s="22"/>
@@ -38658,7 +38658,7 @@
       </c>
       <c r="C141" s="15"/>
       <c r="D141" s="14" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E141" s="22"/>
       <c r="F141" s="22"/>
@@ -38922,7 +38922,7 @@
         <v>131</v>
       </c>
       <c r="D142" s="14" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E142" s="22"/>
       <c r="F142" s="22"/>
@@ -39186,7 +39186,7 @@
         <v>132</v>
       </c>
       <c r="D143" s="14" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E143" s="22"/>
       <c r="F143" s="22"/>
@@ -39443,10 +39443,10 @@
       <c r="A144" s="13"/>
       <c r="B144" s="13"/>
       <c r="C144" s="26" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="D144" s="14" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="E144" s="22"/>
       <c r="F144" s="22"/>
@@ -39708,7 +39708,7 @@
       </c>
       <c r="C145" s="15"/>
       <c r="D145" s="14" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E145" s="22"/>
       <c r="F145" s="22"/>
@@ -39972,7 +39972,7 @@
         <v>134</v>
       </c>
       <c r="D146" s="14" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E146" s="22"/>
       <c r="F146" s="22"/>
@@ -40236,7 +40236,7 @@
         <v>135</v>
       </c>
       <c r="D147" s="14" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E147" s="22"/>
       <c r="F147" s="22"/>
@@ -40492,11 +40492,11 @@
     <row r="148" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A148" s="13"/>
       <c r="B148" s="20" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="C148" s="13"/>
       <c r="D148" s="14" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="E148" s="22"/>
       <c r="F148" s="22"/>
@@ -40752,11 +40752,11 @@
     <row r="149" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A149" s="13"/>
       <c r="B149" s="20" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="C149" s="13"/>
       <c r="D149" s="14" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="E149" s="22"/>
       <c r="F149" s="22"/>
@@ -41012,11 +41012,11 @@
     <row r="150" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A150" s="13"/>
       <c r="B150" s="20" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="C150" s="20"/>
       <c r="D150" s="14" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="E150" s="22"/>
       <c r="F150" s="22"/>
@@ -41272,11 +41272,11 @@
     <row r="151" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A151" s="13"/>
       <c r="B151" s="20" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="C151" s="20"/>
       <c r="D151" s="14" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="E151" s="22"/>
       <c r="F151" s="22"/>
@@ -41536,7 +41536,7 @@
       <c r="B152" s="15"/>
       <c r="C152" s="15"/>
       <c r="D152" s="14" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="E152" s="22"/>
       <c r="F152" s="22"/>
@@ -41798,7 +41798,7 @@
       </c>
       <c r="C153" s="15"/>
       <c r="D153" s="14" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E153" s="22"/>
       <c r="F153" s="22"/>
@@ -42062,7 +42062,7 @@
         <v>138</v>
       </c>
       <c r="D154" s="14" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E154" s="22"/>
       <c r="F154" s="22"/>
@@ -42326,7 +42326,7 @@
         <v>139</v>
       </c>
       <c r="D155" s="14" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="E155" s="22"/>
       <c r="F155" s="22"/>
@@ -42587,10 +42587,10 @@
         <v>5</v>
       </c>
       <c r="C156" s="20" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="D156" s="14" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="E156" s="22"/>
       <c r="F156" s="22"/>
@@ -42851,10 +42851,10 @@
         <v>5</v>
       </c>
       <c r="C157" s="20" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="D157" s="14" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E157" s="22"/>
       <c r="F157" s="22"/>
@@ -43118,7 +43118,7 @@
         <v>140</v>
       </c>
       <c r="D158" s="14" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E158" s="22"/>
       <c r="F158" s="22"/>
@@ -43380,7 +43380,7 @@
       </c>
       <c r="C159" s="15"/>
       <c r="D159" s="14" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="E159" s="22"/>
       <c r="F159" s="22"/>
@@ -43644,7 +43644,7 @@
         <v>142</v>
       </c>
       <c r="D160" s="14" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E160" s="22"/>
       <c r="F160" s="22"/>
@@ -43908,7 +43908,7 @@
         <v>143</v>
       </c>
       <c r="D161" s="14" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E161" s="22"/>
       <c r="F161" s="22"/>
@@ -44172,7 +44172,7 @@
         <v>144</v>
       </c>
       <c r="D162" s="14" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E162" s="22"/>
       <c r="F162" s="22"/>
@@ -44436,7 +44436,7 @@
         <v>145</v>
       </c>
       <c r="D163" s="14" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E163" s="22"/>
       <c r="F163" s="22"/>
@@ -44700,7 +44700,7 @@
         <v>146</v>
       </c>
       <c r="D164" s="14" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="E164" s="22"/>
       <c r="F164" s="22"/>
@@ -44962,7 +44962,7 @@
       </c>
       <c r="C165" s="15"/>
       <c r="D165" s="14" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="E165" s="22"/>
       <c r="F165" s="22"/>
@@ -45226,7 +45226,7 @@
         <v>148</v>
       </c>
       <c r="D166" s="14" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E166" s="22"/>
       <c r="F166" s="22"/>
@@ -45490,7 +45490,7 @@
         <v>149</v>
       </c>
       <c r="D167" s="14" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E167" s="22"/>
       <c r="F167" s="22"/>
@@ -45754,7 +45754,7 @@
         <v>150</v>
       </c>
       <c r="D168" s="14" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="E168" s="22"/>
       <c r="F168" s="22"/>
@@ -46018,7 +46018,7 @@
         <v>151</v>
       </c>
       <c r="D169" s="14" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E169" s="22"/>
       <c r="F169" s="22"/>
@@ -46282,7 +46282,7 @@
         <v>152</v>
       </c>
       <c r="D170" s="14" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E170" s="22"/>
       <c r="F170" s="22"/>
@@ -46543,10 +46543,10 @@
         <v>5</v>
       </c>
       <c r="C171" s="20" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="D171" s="14" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="E171" s="22"/>
       <c r="F171" s="22"/>
@@ -46810,7 +46810,7 @@
         <v>153</v>
       </c>
       <c r="D172" s="14" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E172" s="22"/>
       <c r="F172" s="22"/>
@@ -47072,7 +47072,7 @@
       </c>
       <c r="C173" s="15"/>
       <c r="D173" s="14" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="E173" s="22"/>
       <c r="F173" s="22"/>
@@ -47336,7 +47336,7 @@
         <v>155</v>
       </c>
       <c r="D174" s="14" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="E174" s="22"/>
       <c r="F174" s="22"/>
@@ -47600,7 +47600,7 @@
         <v>156</v>
       </c>
       <c r="D175" s="14" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="E175" s="22"/>
       <c r="F175" s="22"/>
@@ -47864,7 +47864,7 @@
         <v>157</v>
       </c>
       <c r="D176" s="14" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="E176" s="22"/>
       <c r="F176" s="22"/>
@@ -48124,7 +48124,7 @@
       <c r="B177" s="15"/>
       <c r="C177" s="15"/>
       <c r="D177" s="14" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E177" s="22"/>
       <c r="F177" s="22"/>
@@ -48382,11 +48382,11 @@
         <v>5</v>
       </c>
       <c r="B178" s="13" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="C178" s="15"/>
       <c r="D178" s="14" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="E178" s="22"/>
       <c r="F178" s="22"/>
@@ -48650,7 +48650,7 @@
         <v>159</v>
       </c>
       <c r="D179" s="14" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E179" s="22"/>
       <c r="F179" s="22"/>
@@ -48914,7 +48914,7 @@
         <v>160</v>
       </c>
       <c r="D180" s="14" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E180" s="22"/>
       <c r="F180" s="22"/>
@@ -49178,7 +49178,7 @@
         <v>161</v>
       </c>
       <c r="D181" s="14" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E181" s="22"/>
       <c r="F181" s="22"/>
@@ -49439,10 +49439,10 @@
         <v>5</v>
       </c>
       <c r="C182" s="13" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="D182" s="14" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E182" s="22"/>
       <c r="F182" s="22"/>
@@ -49703,10 +49703,10 @@
         <v>5</v>
       </c>
       <c r="C183" s="13" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D183" s="14" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E183" s="22"/>
       <c r="F183" s="22"/>
@@ -49964,11 +49964,11 @@
         <v>5</v>
       </c>
       <c r="B184" s="13" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C184" s="15"/>
       <c r="D184" s="14" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="E184" s="22"/>
       <c r="F184" s="22"/>
@@ -50229,10 +50229,10 @@
         <v>5</v>
       </c>
       <c r="C185" s="13" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D185" s="14" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="E185" s="22"/>
       <c r="F185" s="22"/>
@@ -50496,7 +50496,7 @@
         <v>166</v>
       </c>
       <c r="D186" s="14" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="E186" s="22"/>
       <c r="F186" s="22"/>
@@ -50758,7 +50758,7 @@
       </c>
       <c r="C187" s="15"/>
       <c r="D187" s="14" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E187" s="22"/>
       <c r="F187" s="22"/>
@@ -51022,7 +51022,7 @@
         <v>163</v>
       </c>
       <c r="D188" s="14" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E188" s="22"/>
       <c r="F188" s="22"/>
@@ -51286,7 +51286,7 @@
         <v>164</v>
       </c>
       <c r="D189" s="14" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E189" s="22"/>
       <c r="F189" s="22"/>
@@ -51548,7 +51548,7 @@
       </c>
       <c r="C190" s="15"/>
       <c r="D190" s="14" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="E190" s="22"/>
       <c r="F190" s="22"/>
@@ -51809,10 +51809,10 @@
         <v>5</v>
       </c>
       <c r="C191" s="13" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="D191" s="14" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="E191" s="22"/>
       <c r="F191" s="22"/>
@@ -52073,10 +52073,10 @@
         <v>5</v>
       </c>
       <c r="C192" s="13" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D192" s="14" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="E192" s="22"/>
       <c r="F192" s="22"/>
@@ -52336,7 +52336,7 @@
       <c r="B193" s="15"/>
       <c r="C193" s="15"/>
       <c r="D193" s="14" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="E193" s="22"/>
       <c r="F193" s="22"/>
@@ -52598,7 +52598,7 @@
       </c>
       <c r="C194" s="15"/>
       <c r="D194" s="14" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E194" s="22"/>
       <c r="F194" s="22"/>
@@ -52862,7 +52862,7 @@
         <v>169</v>
       </c>
       <c r="D195" s="14" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E195" s="22"/>
       <c r="F195" s="22"/>
@@ -53126,7 +53126,7 @@
         <v>170</v>
       </c>
       <c r="D196" s="14" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E196" s="22"/>
       <c r="F196" s="22"/>
@@ -53388,7 +53388,7 @@
       </c>
       <c r="C197" s="15"/>
       <c r="D197" s="14" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E197" s="22"/>
       <c r="F197" s="22"/>
@@ -53652,7 +53652,7 @@
         <v>172</v>
       </c>
       <c r="D198" s="14" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E198" s="22"/>
       <c r="F198" s="22"/>
@@ -53912,7 +53912,7 @@
       <c r="B199" s="15"/>
       <c r="C199" s="15"/>
       <c r="D199" s="14" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E199" s="22"/>
       <c r="F199" s="22"/>
@@ -54168,11 +54168,11 @@
     <row r="200" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A200" s="13"/>
       <c r="B200" s="25" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="C200" s="15"/>
       <c r="D200" s="14" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="E200" s="22"/>
       <c r="F200" s="22"/>
@@ -54429,10 +54429,10 @@
       <c r="A201" s="13"/>
       <c r="B201" s="25"/>
       <c r="C201" s="25" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="D201" s="14" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="E201" s="22"/>
       <c r="F201" s="22"/>
@@ -54694,7 +54694,7 @@
       </c>
       <c r="C202" s="15"/>
       <c r="D202" s="14" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E202" s="22"/>
       <c r="F202" s="22"/>
@@ -54955,10 +54955,10 @@
         <v>5</v>
       </c>
       <c r="C203" s="20" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D203" s="14" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E203" s="22"/>
       <c r="F203" s="22"/>
@@ -55220,7 +55220,7 @@
       </c>
       <c r="C204" s="15"/>
       <c r="D204" s="14" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E204" s="22"/>
       <c r="F204" s="22"/>
@@ -55484,7 +55484,7 @@
         <v>176</v>
       </c>
       <c r="D205" s="14" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="E205" s="22"/>
       <c r="F205" s="22"/>
@@ -55746,7 +55746,7 @@
       </c>
       <c r="C206" s="15"/>
       <c r="D206" s="14" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="E206" s="22"/>
       <c r="F206" s="22"/>
@@ -56010,7 +56010,7 @@
         <v>178</v>
       </c>
       <c r="D207" s="14" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="E207" s="22"/>
       <c r="F207" s="22"/>
@@ -56272,7 +56272,7 @@
       </c>
       <c r="C208" s="15"/>
       <c r="D208" s="14" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="E208" s="22"/>
       <c r="F208" s="22"/>
@@ -56536,7 +56536,7 @@
         <v>180</v>
       </c>
       <c r="D209" s="14" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="E209" s="22"/>
       <c r="F209" s="22"/>
@@ -56800,7 +56800,7 @@
         <v>181</v>
       </c>
       <c r="D210" s="14" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="E210" s="22"/>
       <c r="F210" s="22"/>
@@ -57060,7 +57060,7 @@
       <c r="B211" s="15"/>
       <c r="C211" s="15"/>
       <c r="D211" s="14" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E211" s="22"/>
       <c r="F211" s="22"/>
@@ -57322,7 +57322,7 @@
       </c>
       <c r="C212" s="15"/>
       <c r="D212" s="14" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E212" s="22"/>
       <c r="F212" s="22"/>
@@ -57586,7 +57586,7 @@
         <v>184</v>
       </c>
       <c r="D213" s="14" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E213" s="22"/>
       <c r="F213" s="22"/>
@@ -57850,7 +57850,7 @@
         <v>185</v>
       </c>
       <c r="D214" s="14" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E214" s="22"/>
       <c r="F214" s="22"/>
@@ -58373,10 +58373,10 @@
         <v>5</v>
       </c>
       <c r="C216" s="13" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="D216" s="14" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="E216" s="22"/>
       <c r="F216" s="22"/>
@@ -58640,7 +58640,7 @@
         <v>188</v>
       </c>
       <c r="D217" s="14" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E217" s="22"/>
       <c r="F217" s="22"/>
@@ -58902,7 +58902,7 @@
       </c>
       <c r="C218" s="15"/>
       <c r="D218" s="14" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E218" s="22"/>
       <c r="F218" s="22"/>
@@ -59166,7 +59166,7 @@
         <v>190</v>
       </c>
       <c r="D219" s="14" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="E219" s="22"/>
       <c r="F219" s="22"/>
@@ -59426,7 +59426,7 @@
       <c r="B220" s="15"/>
       <c r="C220" s="15"/>
       <c r="D220" s="14" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E220" s="22"/>
       <c r="F220" s="22"/>
@@ -59679,16 +59679,16 @@
       <c r="IS220" s="22"/>
       <c r="IT220" s="22"/>
     </row>
-    <row r="221" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A221" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B221" s="13" t="s">
-        <v>192</v>
+        <v>477</v>
       </c>
       <c r="C221" s="15"/>
       <c r="D221" s="14" t="s">
-        <v>326</v>
+        <v>479</v>
       </c>
       <c r="E221" s="22"/>
       <c r="F221" s="22"/>
@@ -59949,10 +59949,10 @@
         <v>5</v>
       </c>
       <c r="C222" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="D222" s="14" t="s">
         <v>193</v>
-      </c>
-      <c r="D222" s="14" t="s">
-        <v>194</v>
       </c>
       <c r="E222" s="22"/>
       <c r="F222" s="22"/>
@@ -60205,16 +60205,16 @@
       <c r="IS222" s="22"/>
       <c r="IT222" s="22"/>
     </row>
-    <row r="223" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A223" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B223" s="13" t="s">
-        <v>195</v>
+        <v>478</v>
       </c>
       <c r="C223" s="15"/>
       <c r="D223" s="14" t="s">
-        <v>327</v>
+        <v>480</v>
       </c>
       <c r="E223" s="22"/>
       <c r="F223" s="22"/>
@@ -60469,12 +60469,12 @@
     </row>
     <row r="224" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A224" s="17" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B224" s="17"/>
       <c r="C224" s="17"/>
       <c r="D224" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="E224" s="22"/>
       <c r="F224" s="22"/>
@@ -60730,11 +60730,11 @@
     <row r="225" spans="1:254" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A225" s="18"/>
       <c r="B225" s="17" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="C225" s="17"/>
       <c r="D225" s="19" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="E225" s="22"/>
       <c r="F225" s="22"/>
@@ -60991,10 +60991,10 @@
       <c r="A226" s="18"/>
       <c r="B226" s="17"/>
       <c r="C226" s="17" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="D226" s="19" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="E226" s="22"/>
       <c r="F226" s="22"/>
@@ -61251,10 +61251,10 @@
       <c r="A227" s="18"/>
       <c r="B227" s="17"/>
       <c r="C227" s="17" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="D227" s="19" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="E227" s="22"/>
       <c r="F227" s="22"/>
@@ -61511,10 +61511,10 @@
       <c r="A228" s="18"/>
       <c r="B228" s="17"/>
       <c r="C228" s="17" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D228" s="19" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E228" s="22"/>
       <c r="F228" s="22"/>
@@ -61771,10 +61771,10 @@
       <c r="A229" s="18"/>
       <c r="B229" s="17"/>
       <c r="C229" s="17" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="D229" s="19" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="E229" s="22"/>
       <c r="F229" s="22"/>
@@ -62031,10 +62031,10 @@
       <c r="A230" s="18"/>
       <c r="B230" s="17"/>
       <c r="C230" s="17" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="D230" s="19" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="E230" s="22"/>
       <c r="F230" s="22"/>
@@ -62290,11 +62290,11 @@
     <row r="231" spans="1:254" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A231" s="18"/>
       <c r="B231" s="17" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="C231" s="17"/>
       <c r="D231" s="19" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="E231" s="22"/>
       <c r="F231" s="22"/>
@@ -62551,10 +62551,10 @@
       <c r="A232" s="18"/>
       <c r="B232" s="17"/>
       <c r="C232" s="17" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D232" s="19" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="E232" s="22"/>
       <c r="F232" s="22"/>
@@ -62811,10 +62811,10 @@
       <c r="A233" s="18"/>
       <c r="B233" s="17"/>
       <c r="C233" s="17" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="D233" s="19" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="E233" s="22"/>
       <c r="F233" s="22"/>
@@ -63071,10 +63071,10 @@
       <c r="A234" s="18"/>
       <c r="B234" s="17"/>
       <c r="C234" s="17" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="D234" s="19" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="E234" s="22"/>
       <c r="F234" s="22"/>
@@ -63331,10 +63331,10 @@
       <c r="A235" s="18"/>
       <c r="B235" s="17"/>
       <c r="C235" s="17" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="D235" s="19" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="E235" s="22"/>
       <c r="F235" s="22"/>
@@ -63864,7 +63864,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -63873,7 +63873,7 @@
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="7" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="5"/>
@@ -63881,27 +63881,27 @@
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="7" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="8" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="7" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="8" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="7" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="8"/>
@@ -63909,7 +63909,7 @@
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="7" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="8"/>

</xml_diff>